<commit_message>
almost done with metadata
</commit_message>
<xml_diff>
--- a/metadata/binddata.xlsx
+++ b/metadata/binddata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ual895/Git/newdictionary/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{869ADB6B-179C-324F-86C9-251C422DB875}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B9FA61-74A9-1C47-8773-B33522A51A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="471">
   <si>
     <t>primitive</t>
   </si>
@@ -391,96 +391,39 @@
     <t>n-of</t>
   </si>
   <si>
-    <t>subset, random</t>
-  </si>
-  <si>
     <t>one-of, count, any?, all?</t>
   </si>
   <si>
-    <t>Virus, Segregation Simple</t>
-  </si>
-  <si>
     <t>of</t>
   </si>
   <si>
-    <t>variable</t>
-  </si>
-  <si>
     <t>with, to-report, turtles-own, patches-own</t>
   </si>
   <si>
     <t>or</t>
   </si>
   <si>
-    <t>either, boolean</t>
-  </si>
-  <si>
-    <t>if, if-else, and, xor</t>
-  </si>
-  <si>
-    <t>Voronoi</t>
-  </si>
-  <si>
     <t>random</t>
   </si>
   <si>
-    <t>generate a random whole number within a specified range</t>
-  </si>
-  <si>
-    <t>probability, chance</t>
-  </si>
-  <si>
     <t>random-float, random-normal, globals, turtles-own</t>
   </si>
   <si>
-    <t>Fireworks, Virus</t>
-  </si>
-  <si>
     <t>random-float</t>
   </si>
   <si>
-    <t>generate a random real (non-whole) number within a specified range</t>
-  </si>
-  <si>
-    <t>decimal, floating, probability, chance</t>
-  </si>
-  <si>
     <t>random, random-normal, globals, turtles-own</t>
   </si>
   <si>
-    <t>Virus, Wolf Sheep Predation</t>
-  </si>
-  <si>
     <t>scale-color</t>
   </si>
   <si>
-    <t>generate a shade of a base hue (color) based on a given value</t>
-  </si>
-  <si>
-    <t>shade, legend, tint</t>
-  </si>
-  <si>
     <t>color, pcolor, set, turtles-own</t>
   </si>
   <si>
-    <t>Ants, Wolf Sheep Simple 3</t>
-  </si>
-  <si>
     <t>setxy</t>
   </si>
   <si>
-    <t>set the position of a turtle (in terms of X and Y coordinates)</t>
-  </si>
-  <si>
-    <t>position, coordinate</t>
-  </si>
-  <si>
-    <t>move-to, min-pxcor, max-pxcor, neighbors</t>
-  </si>
-  <si>
-    <t>Wolf Sheep Simple 2, Segregation Simple</t>
-  </si>
-  <si>
     <t>sort-by</t>
   </si>
   <si>
@@ -562,117 +505,42 @@
     <t>move-to</t>
   </si>
   <si>
-    <t>move, go, around, jump</t>
-  </si>
-  <si>
-    <t>setxy, face, distance, distancexy</t>
-  </si>
-  <si>
-    <t>Fairy Circles</t>
-  </si>
-  <si>
     <t>neighbors</t>
   </si>
   <si>
-    <t>neighbors, surrounding patches, surrounding, nearby, around, north, south, east, west, northeast, northwest, southeast, southwest, directions</t>
-  </si>
-  <si>
-    <t>neighbors4, patch-ahead, pxcor, pycor</t>
-  </si>
-  <si>
-    <t>Recycling, Rumor Mill</t>
-  </si>
-  <si>
     <t>neighbors4</t>
   </si>
   <si>
-    <t xml:space="preserve">neighbors4, neighbors, surrounding patches, surrounding, nearby, around, north, south, west, east, directions </t>
-  </si>
-  <si>
-    <t>neighbors, patch-ahead, pxcor, pycor</t>
-  </si>
-  <si>
-    <t>Rumor Mill</t>
-  </si>
-  <si>
     <t>other</t>
   </si>
   <si>
-    <t>other, omit</t>
-  </si>
-  <si>
-    <t>all?, any?, nobody, ask</t>
-  </si>
-  <si>
-    <t>Traffic Basic</t>
-  </si>
-  <si>
     <t>patch-ahead</t>
   </si>
   <si>
-    <t>patch ahead, ahead, distance, units, move ahead</t>
-  </si>
-  <si>
-    <t>neighbors, neighbors4, pxcor, pycor</t>
-  </si>
-  <si>
     <t>pcolor</t>
   </si>
   <si>
-    <t>built-in patch variable that holds the color of the patch</t>
-  </si>
-  <si>
-    <t>pcolor, patch color, color, patch, patches, change color</t>
-  </si>
-  <si>
     <t>color, set, patches, neighbors</t>
   </si>
   <si>
     <t>repeat</t>
   </si>
   <si>
-    <t>allows you to execute any set of commands n amount of times</t>
-  </si>
-  <si>
-    <t>repeat, repetition, again, multiple, move, go</t>
-  </si>
-  <si>
-    <t>pen-down, pen-up, ask, right</t>
-  </si>
-  <si>
     <t>round</t>
   </si>
   <si>
-    <t>reports the integer to the nearest whole number.</t>
-  </si>
-  <si>
-    <t>round, go up, go down, numbers</t>
-  </si>
-  <si>
     <t>count, floor, ceiling, mean</t>
   </si>
   <si>
     <t>semicolon</t>
   </si>
   <si>
-    <t>used for making helpful comments or notes on a line of code</t>
-  </si>
-  <si>
-    <t>semicolon, comments, comment, notes, help</t>
-  </si>
-  <si>
     <t>to, to-report, end, ask</t>
   </si>
   <si>
     <t>shape</t>
   </si>
   <si>
-    <t>represents the shape of each agent</t>
-  </si>
-  <si>
-    <t>shape, different shape, change shape, turtle</t>
-  </si>
-  <si>
     <t>color, turtles, set, of</t>
   </si>
   <si>
@@ -763,9 +631,6 @@
     <t>min-pxcor, min-pycor, move-to, setxy</t>
   </si>
   <si>
-    <t>Erosion, Traffic Grid</t>
-  </si>
-  <si>
     <t>max-pycor</t>
   </si>
   <si>
@@ -799,166 +664,70 @@
     <t>mod</t>
   </si>
   <si>
-    <t>modulo, remainder, divide</t>
-  </si>
-  <si>
     <t>mean, count, if, any?</t>
   </si>
   <si>
-    <t>Flocking, Wealth Distribution, Voting</t>
-  </si>
-  <si>
     <t>myself</t>
   </si>
   <si>
-    <t>interaction, me, caller</t>
-  </si>
-  <si>
     <t>nobody, ask, of, let</t>
   </si>
   <si>
-    <t>Virus on a Network, Scatter</t>
-  </si>
-  <si>
     <t>nobody</t>
   </si>
   <si>
-    <t>none, empty, dead</t>
-  </si>
-  <si>
-    <t>all?, any?, member?, with</t>
-  </si>
-  <si>
-    <t>Wolf Sheep Predation, Shepherds, Ants</t>
-  </si>
-  <si>
     <t>one-of</t>
   </si>
   <si>
-    <t>one, pick, select, single</t>
-  </si>
-  <si>
-    <t>n-of, random, max-n-of, any?</t>
-  </si>
-  <si>
-    <t>Flocking, Disease</t>
-  </si>
-  <si>
     <t>patch</t>
   </si>
   <si>
-    <t>patches, background</t>
-  </si>
-  <si>
     <t>patches, clear-patches, patches-own, neighbors</t>
   </si>
   <si>
-    <t>Paths, Rumor Mill</t>
-  </si>
-  <si>
     <t>patches-own</t>
   </si>
   <si>
-    <t>Declare a variable that belongs to patches.</t>
-  </si>
-  <si>
     <t>patches, variable, declare</t>
   </si>
   <si>
     <t>turtles-own, set, of, with</t>
   </si>
   <si>
-    <t>Rebellion, Traffic Grid, Paths</t>
-  </si>
-  <si>
-    <t>Address all patches of a model.</t>
-  </si>
-  <si>
-    <t>patch, background</t>
-  </si>
-  <si>
     <t xml:space="preserve"> clear-patches, patches-own, neighbors, move-to</t>
   </si>
   <si>
     <t>pen-down</t>
   </si>
   <si>
-    <t>Starts tracing the movement of the turtle.</t>
-  </si>
-  <si>
-    <t>trace, pen, draw, mark</t>
-  </si>
-  <si>
-    <t>pen-up, pen-erase, forward, right</t>
-  </si>
-  <si>
-    <t>Single Collision, Tumor, Free Gas</t>
-  </si>
-  <si>
     <t>pen-up</t>
   </si>
   <si>
     <t>Stops tracing a turtle's movement.</t>
   </si>
   <si>
-    <t>pen-down, pen-erase, forward, right</t>
-  </si>
-  <si>
     <t>random-normal</t>
   </si>
   <si>
-    <t>Randomly produces a number according to a normal distribution.</t>
-  </si>
-  <si>
-    <t>random, normal, distribution, bell, chance, probability</t>
-  </si>
-  <si>
-    <t>random, mean, set, mean</t>
-  </si>
-  <si>
-    <t>Sunflower, Echo, Autumn</t>
-  </si>
-  <si>
     <t>reset-ticks</t>
   </si>
   <si>
     <t>Sets the tick counter to 0.</t>
   </si>
   <si>
-    <t>ticks, counter</t>
-  </si>
-  <si>
     <t>tick, to, ask, clear-all</t>
   </si>
   <si>
     <t>right</t>
   </si>
   <si>
-    <t>Turn a certain amount of degrees to the right.</t>
-  </si>
-  <si>
-    <t>turn, spin</t>
-  </si>
-  <si>
     <t>left, heading, towards, face</t>
   </si>
   <si>
-    <t>Paths, Segregation</t>
-  </si>
-  <si>
     <t>set</t>
   </si>
   <si>
-    <t>Set the value of a variable.</t>
-  </si>
-  <si>
-    <t>variable, value</t>
-  </si>
-  <si>
     <t>let, globals, turtles-own, patches-own</t>
-  </si>
-  <si>
-    <t>Minority Game, Voting</t>
   </si>
   <si>
     <t>sprout</t>
@@ -1360,18 +1129,12 @@
     <t>Reports the smallest y-coordinate of the patches in a midel.</t>
   </si>
   <si>
-    <t>Performs the modulo operation and reports the remainder from the division of the first number by the second number.</t>
-  </si>
-  <si>
     <t>Moves a turtle to set its x and y coordinates to be the same as another turtle or patch.</t>
   </si>
   <si>
     <t>Reports the original turtle that asked another turtle to follow some rules.</t>
   </si>
   <si>
-    <t>Reports "n" randomly picked agents from an agentset.</t>
-  </si>
-  <si>
     <t>Reports an agentset containing the eight neighboring patches.</t>
   </si>
   <si>
@@ -1384,9 +1147,6 @@
     <t>Reports the value of an agent-owned variable.</t>
   </si>
   <si>
-    <t>Reports one randomly picked one agent from a provided agentset.</t>
-  </si>
-  <si>
     <t>Checks if either of two provided conditions is true.</t>
   </si>
   <si>
@@ -1564,9 +1324,6 @@
     <t>round, up, integer, decimal, floating, math, calculate</t>
   </si>
   <si>
-    <t>move, motion, straight, go, around, position, location, step</t>
-  </si>
-  <si>
     <t>Bidding Market, Vector Fields, CRISPR Ecosystem, Wolf Sheep Predation</t>
   </si>
   <si>
@@ -1645,9 +1402,6 @@
     <t>Planarity, Giant Component, Small Worlds</t>
   </si>
   <si>
-    <t>turn, angle, direction, orientation, twist</t>
-  </si>
-  <si>
     <t>right, set, face, forward</t>
   </si>
   <si>
@@ -1727,6 +1481,267 @@
   </si>
   <si>
     <t>Fire, Tumor, Blood Sugar Regulation, Ant Lines</t>
+  </si>
+  <si>
+    <t>Autumn, Fireworks, Galton Box, Rugby</t>
+  </si>
+  <si>
+    <t>Performs the modulo operation; reports the remainder from the division of the first number by the second number.</t>
+  </si>
+  <si>
+    <t>remainder, divide, math, calculate, arithmetic</t>
+  </si>
+  <si>
+    <t>Sunflower, Flocking Vee Formations, Voronoi, Fruit Wars</t>
+  </si>
+  <si>
+    <t>jump, travel, relocate, shift, transport, hop</t>
+  </si>
+  <si>
+    <t>move, motion, straight, go, around, position, location, step, walk, jog</t>
+  </si>
+  <si>
+    <t>setxy, set, pxcor, patches</t>
+  </si>
+  <si>
+    <t>Heatbugs, Shepherds, Membrane Formation, Grand Canyon</t>
+  </si>
+  <si>
+    <t>interaction, caller, original, nested, refer, talk</t>
+  </si>
+  <si>
+    <t>Sunflower Biomorphs, Mammoths, Autumn, Fairy Circles</t>
+  </si>
+  <si>
+    <t>Reports "n" randomly picked agents from an agentset or items from a list.</t>
+  </si>
+  <si>
+    <t>subset, random, batch, portion, fragment</t>
+  </si>
+  <si>
+    <t>Virus, Heatbugs, Voronoi, Virus on a Network</t>
+  </si>
+  <si>
+    <t>surrounding, nearby, around, directions, next, border, adjoin, touch</t>
+  </si>
+  <si>
+    <t>neighbors4, patch-ahead, turtles-here, patches</t>
+  </si>
+  <si>
+    <t>Fur, DLA, Segregation, Daisyworld</t>
+  </si>
+  <si>
+    <t>neighbors, patch-ahead, turtles-here, patches</t>
+  </si>
+  <si>
+    <t>Fire, Life, Sandpile, Altruism</t>
+  </si>
+  <si>
+    <t>none, empty, dead, exist, nothing</t>
+  </si>
+  <si>
+    <t>any?, member?, n-of, let</t>
+  </si>
+  <si>
+    <t>Tumor, Heatbugs, Shepherds, HIV</t>
+  </si>
+  <si>
+    <t>variable, characteristic, property, feature</t>
+  </si>
+  <si>
+    <t>Urban Suite - Recycling, Paths, Slime, Language Change</t>
+  </si>
+  <si>
+    <t>Reports one randomly picked member from a provided agentset or list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pick, select, draw, lottery </t>
+  </si>
+  <si>
+    <t>n-of, random, max-n-of, let</t>
+  </si>
+  <si>
+    <t>Mammoths, Ants, Shepherds, Fairy Circles</t>
+  </si>
+  <si>
+    <t>either, boolean, true, false, condition, compare</t>
+  </si>
+  <si>
+    <t>if, if-else, and, of</t>
+  </si>
+  <si>
+    <t>Lennard-Jones, GasLab Atmosphere, Bidding Market, Wealth Distribution</t>
+  </si>
+  <si>
+    <t>omit, exclude</t>
+  </si>
+  <si>
+    <t>any?, turtles-here, in-radius, patches</t>
+  </si>
+  <si>
+    <t>Virus, Flocking, Scatter, Fruit Wars</t>
+  </si>
+  <si>
+    <t>square, background, world</t>
+  </si>
+  <si>
+    <t>Ant Lines, Autumn, SmoothLife, Rumor Mill</t>
+  </si>
+  <si>
+    <t>before, see, detect, lead, onward</t>
+  </si>
+  <si>
+    <t>neighbors, in-radius, in-cone, nobody</t>
+  </si>
+  <si>
+    <t>Mammoths, Slime, Climate Change, Traffic Intersection</t>
+  </si>
+  <si>
+    <t>Reports an agentset that contains all the patches in a model.</t>
+  </si>
+  <si>
+    <t>Reports an agentset that contains all the turtles in a model.</t>
+  </si>
+  <si>
+    <t>Peppered Moths, Blood Sugar Regulation, Honeycomb</t>
+  </si>
+  <si>
+    <t>Defines custom characteristics (variables) for patches. Each custom characteristic can have a different value for each patch.</t>
+  </si>
+  <si>
+    <t>Diffusion Graphics, Grand Canyon, Life, Hoteling's Law</t>
+  </si>
+  <si>
+    <t>Reports a patch's color and changes a patch's color when used with the set primitive.</t>
+  </si>
+  <si>
+    <t>patch, square, world, background, paint</t>
+  </si>
+  <si>
+    <t>Vision Evolution, Rock Paper Scissors, Wolf Sheep Predation</t>
+  </si>
+  <si>
+    <t>Starts tracing the movement of the turtle on patches.</t>
+  </si>
+  <si>
+    <t>trace, draw, mark, paint, engrave, sketch</t>
+  </si>
+  <si>
+    <t>pen-up, clear-all, forward, right</t>
+  </si>
+  <si>
+    <t>Turtles Circling, Bidding Market, GasLab Single Collision, Pendulum</t>
+  </si>
+  <si>
+    <t>pen-down, clear-all, forward, right</t>
+  </si>
+  <si>
+    <t>Reports a random whole number between 0 and a specified number.</t>
+  </si>
+  <si>
+    <t>probability, chance, lottery, luck, toss, pick</t>
+  </si>
+  <si>
+    <t>Reports a random number with decimal points between 0 and a specified number.</t>
+  </si>
+  <si>
+    <t>decimal, floating, probability, chance, lottery, luck, toss, pick</t>
+  </si>
+  <si>
+    <t>Fire, Climate Change, Galton Box, Daisyworld</t>
+  </si>
+  <si>
+    <t>Reports a random number with decimal points that is picked from over a normal distribution with a specified mean and standard deviation.</t>
+  </si>
+  <si>
+    <t>distribution, bell, curve, chance, probability, lottery, luck, toss, pick</t>
+  </si>
+  <si>
+    <t>random, random-float, mean, set</t>
+  </si>
+  <si>
+    <t>Anisogamy, Autumn, Epidem Basic, Echo</t>
+  </si>
+  <si>
+    <t>Performs a provided set of rules (commands) repeatedly for a specified number of times.</t>
+  </si>
+  <si>
+    <t>repetition, again, multiple, loop, for, execute</t>
+  </si>
+  <si>
+    <t>ask, to, end, while</t>
+  </si>
+  <si>
+    <t>Disease Solo, Flocking Vee Formations, Peppered Moths, Ant Lines</t>
+  </si>
+  <si>
+    <t>counter, time, restart, clock, watch</t>
+  </si>
+  <si>
+    <t>Wolf Sheep Predation, Fire, Autumn, Climate Change</t>
+  </si>
+  <si>
+    <t>Changes a turtle's heading a certain amount of degrees to the right.</t>
+  </si>
+  <si>
+    <t>turn, angle, direction, orientation, twist, rotate</t>
+  </si>
+  <si>
+    <t>turn, spin, rotate, angle, direction, orientation</t>
+  </si>
+  <si>
+    <t>Wolf Sheep Simple, Mammoths, Anisogamy, DLA Simple</t>
+  </si>
+  <si>
+    <t>Reports the integer that is nearest to a specified value.</t>
+  </si>
+  <si>
+    <t>decimal, floating, near, approximate, roughly</t>
+  </si>
+  <si>
+    <t>Sex Ratio Equilibrium, Bug Hunt Camouflage, GenDrift T Interact, Blood Sugar Regulation</t>
+  </si>
+  <si>
+    <t>Reports a shade of a base hue (color) based on where a speficied value falls is within a specified range (min-max).</t>
+  </si>
+  <si>
+    <t>shade, legend, tint, paint, tone, saturation, gradient</t>
+  </si>
+  <si>
+    <t>Moths, Ants, Honeycomb, Autumn</t>
+  </si>
+  <si>
+    <t>Starts a comments to take notes on a line of code. Anything that follows a semicolon (;) will not be considered code.</t>
+  </si>
+  <si>
+    <t>comment, note</t>
+  </si>
+  <si>
+    <t>Changes the value of a variable (global, local, or agent-owned).</t>
+  </si>
+  <si>
+    <t>variable, value, change, modify, alter</t>
+  </si>
+  <si>
+    <t>Moves a turtle to the exact location defined by the provided x and y coordinates.</t>
+  </si>
+  <si>
+    <t>position, coordinate, location, move, jump, transport</t>
+  </si>
+  <si>
+    <t>move-to, min-pxcor, max-pycor, neighbors</t>
+  </si>
+  <si>
+    <t>Vision Evolution, Tumor, Virus, Flocking</t>
+  </si>
+  <si>
+    <t>Reports a turtles or link's shape and changes a turtle's or link's shape when used with the set primitive.</t>
+  </si>
+  <si>
+    <t>look, design, style, outline, image, bitmap, vector, picture, icon, appearance, figure, photo</t>
+  </si>
+  <si>
+    <t>Urban Suite - Pollution, Traffic Intersection, Mimicry, Ant Lines</t>
   </si>
 </sst>
 </file>
@@ -2264,9 +2279,9 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J44" sqref="J44"/>
+    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2333,13 +2348,13 @@
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>128</v>
+        <v>84</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>308</v>
+        <v>231</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>356</v>
+        <v>276</v>
       </c>
       <c r="D2" s="24" t="b">
         <v>0</v>
@@ -2357,10 +2372,10 @@
         <v>1</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>357</v>
+        <v>277</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>358</v>
+        <v>278</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2368,10 +2383,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>309</v>
+        <v>232</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>361</v>
+        <v>281</v>
       </c>
       <c r="D3" s="24" t="b">
         <v>0</v>
@@ -2389,10 +2404,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>360</v>
+        <v>280</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>359</v>
+        <v>279</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2400,10 +2415,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>310</v>
+        <v>233</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>362</v>
+        <v>282</v>
       </c>
       <c r="D4" s="25" t="b">
         <v>0</v>
@@ -2421,21 +2436,21 @@
         <v>1</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>363</v>
+        <v>283</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>364</v>
+        <v>284</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>311</v>
+        <v>234</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>367</v>
+        <v>287</v>
       </c>
       <c r="D5" s="24" t="b">
         <v>1</v>
@@ -2453,10 +2468,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>366</v>
+        <v>286</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>365</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2464,10 +2479,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>312</v>
+        <v>235</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>368</v>
+        <v>288</v>
       </c>
       <c r="D6" s="24" t="b">
         <v>1</v>
@@ -2485,21 +2500,21 @@
         <v>0</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>369</v>
+        <v>289</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>370</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>313</v>
+        <v>236</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>410</v>
+        <v>330</v>
       </c>
       <c r="D7" s="24" t="b">
         <v>0</v>
@@ -2517,21 +2532,21 @@
         <v>1</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>371</v>
+        <v>291</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>372</v>
+        <v>292</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>326</v>
+        <v>249</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>314</v>
+        <v>237</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>375</v>
+        <v>295</v>
       </c>
       <c r="D8" s="24" t="b">
         <v>1</v>
@@ -2549,21 +2564,21 @@
         <v>0</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>374</v>
+        <v>294</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>373</v>
+        <v>293</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>314</v>
+        <v>237</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>375</v>
+        <v>295</v>
       </c>
       <c r="D9" s="24" t="b">
         <v>1</v>
@@ -2581,21 +2596,21 @@
         <v>0</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>374</v>
+        <v>294</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>373</v>
+        <v>293</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>71</v>
+        <v>52</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>315</v>
+        <v>238</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>375</v>
+        <v>295</v>
       </c>
       <c r="D10" s="24" t="b">
         <v>1</v>
@@ -2613,21 +2628,21 @@
         <v>0</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>376</v>
+        <v>296</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>378</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>316</v>
+        <v>239</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>375</v>
+        <v>295</v>
       </c>
       <c r="D11" s="24" t="b">
         <v>1</v>
@@ -2645,21 +2660,21 @@
         <v>0</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>377</v>
+        <v>297</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>379</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>73</v>
+        <v>54</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>393</v>
+        <v>313</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>382</v>
+        <v>302</v>
       </c>
       <c r="D12" s="24" t="b">
         <v>0</v>
@@ -2677,21 +2692,21 @@
         <v>0</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>380</v>
+        <v>300</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>381</v>
+        <v>301</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>130</v>
+        <v>86</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>317</v>
+        <v>240</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>383</v>
+        <v>303</v>
       </c>
       <c r="D13" s="24" t="b">
         <v>0</v>
@@ -2709,10 +2724,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>384</v>
+        <v>304</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>385</v>
+        <v>305</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2720,10 +2735,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>318</v>
+        <v>241</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>447</v>
+        <v>365</v>
       </c>
       <c r="D14" s="25" t="b">
         <v>0</v>
@@ -2744,18 +2759,18 @@
         <v>14</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>386</v>
+        <v>306</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>327</v>
+        <v>250</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>319</v>
+        <v>242</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>388</v>
+        <v>308</v>
       </c>
       <c r="D15" s="24" t="b">
         <v>1</v>
@@ -2773,21 +2788,21 @@
         <v>0</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>389</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>74</v>
+        <v>55</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>319</v>
+        <v>242</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>387</v>
+        <v>307</v>
       </c>
       <c r="D16" s="24" t="b">
         <v>1</v>
@@ -2805,21 +2820,21 @@
         <v>0</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>389</v>
+        <v>309</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>320</v>
+        <v>243</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>392</v>
+        <v>312</v>
       </c>
       <c r="D17" s="25" t="b">
         <v>0</v>
@@ -2837,10 +2852,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>391</v>
+        <v>311</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>390</v>
+        <v>310</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -2848,10 +2863,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>394</v>
+        <v>314</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>395</v>
+        <v>315</v>
       </c>
       <c r="D18" s="25" t="b">
         <v>0</v>
@@ -2869,21 +2884,21 @@
         <v>0</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>396</v>
+        <v>316</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>397</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>401</v>
+        <v>321</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>400</v>
+        <v>320</v>
       </c>
       <c r="D19" s="25" t="b">
         <v>0</v>
@@ -2901,21 +2916,21 @@
         <v>0</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>399</v>
+        <v>319</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>398</v>
+        <v>318</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>321</v>
+        <v>244</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>402</v>
+        <v>322</v>
       </c>
       <c r="D20" s="24" t="b">
         <v>1</v>
@@ -2933,21 +2948,21 @@
         <v>0</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>403</v>
+        <v>323</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>406</v>
+        <v>326</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>405</v>
+        <v>325</v>
       </c>
       <c r="D21" s="25" t="b">
         <v>0</v>
@@ -2965,21 +2980,21 @@
         <v>0</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>404</v>
+        <v>324</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>407</v>
+        <v>327</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>405</v>
+        <v>325</v>
       </c>
       <c r="D22" s="24" t="b">
         <v>0</v>
@@ -2997,21 +3012,21 @@
         <v>0</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>408</v>
+        <v>328</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>322</v>
+        <v>245</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>410</v>
+        <v>330</v>
       </c>
       <c r="D23" s="24" t="b">
         <v>0</v>
@@ -3029,21 +3044,21 @@
         <v>1</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>409</v>
+        <v>329</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>323</v>
+        <v>246</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D24" s="24" t="b">
         <v>0</v>
@@ -3061,21 +3076,21 @@
         <v>0</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>412</v>
+        <v>331</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
-        <v>325</v>
+        <v>248</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>323</v>
+        <v>246</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>411</v>
+        <v>389</v>
       </c>
       <c r="D25" s="24" t="b">
         <v>0</v>
@@ -3093,10 +3108,10 @@
         <v>0</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>412</v>
+        <v>331</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3104,10 +3119,10 @@
         <v>16</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>413</v>
+        <v>332</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>414</v>
+        <v>333</v>
       </c>
       <c r="D26" s="24" t="b">
         <v>1</v>
@@ -3125,21 +3140,21 @@
         <v>0</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>415</v>
+        <v>334</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>416</v>
+        <v>335</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>419</v>
+        <v>338</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>418</v>
+        <v>337</v>
       </c>
       <c r="D27" s="25" t="b">
         <v>0</v>
@@ -3157,21 +3172,21 @@
         <v>0</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>417</v>
+        <v>336</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>421</v>
+        <v>340</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>423</v>
+        <v>342</v>
       </c>
       <c r="D28" s="24" t="b">
         <v>0</v>
@@ -3189,10 +3204,10 @@
         <v>1</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>420</v>
+        <v>339</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3200,10 +3215,10 @@
         <v>17</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>422</v>
+        <v>341</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>424</v>
+        <v>343</v>
       </c>
       <c r="D29" s="25" t="b">
         <v>0</v>
@@ -3221,10 +3236,10 @@
         <v>1</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>425</v>
+        <v>344</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>426</v>
+        <v>345</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3232,10 +3247,10 @@
         <v>18</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>324</v>
+        <v>247</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>427</v>
+        <v>346</v>
       </c>
       <c r="D30" s="25" t="b">
         <v>0</v>
@@ -3253,10 +3268,10 @@
         <v>1</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>428</v>
+        <v>347</v>
       </c>
       <c r="J30" s="29" t="s">
-        <v>429</v>
+        <v>348</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3264,10 +3279,10 @@
         <v>19</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>330</v>
+        <v>253</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>432</v>
+        <v>351</v>
       </c>
       <c r="D31" s="25" t="b">
         <v>0</v>
@@ -3288,7 +3303,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>430</v>
+        <v>349</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3296,10 +3311,10 @@
         <v>21</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>329</v>
+        <v>252</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>431</v>
+        <v>350</v>
       </c>
       <c r="D32" s="25" t="b">
         <v>0</v>
@@ -3317,10 +3332,10 @@
         <v>0</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>433</v>
+        <v>352</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>434</v>
+        <v>353</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3328,10 +3343,10 @@
         <v>22</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>331</v>
+        <v>254</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>435</v>
+        <v>354</v>
       </c>
       <c r="D33" s="24" t="b">
         <v>1</v>
@@ -3349,21 +3364,21 @@
         <v>0</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>436</v>
+        <v>355</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>437</v>
+        <v>356</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>332</v>
+        <v>255</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>438</v>
+        <v>451</v>
       </c>
       <c r="D34" s="25" t="b">
         <v>0</v>
@@ -3381,21 +3396,21 @@
         <v>0</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>439</v>
+        <v>357</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>440</v>
+        <v>358</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>441</v>
+        <v>359</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>442</v>
+        <v>360</v>
       </c>
       <c r="D35" s="24" t="b">
         <v>0</v>
@@ -3413,10 +3428,10 @@
         <v>1</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>443</v>
+        <v>361</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3424,10 +3439,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>333</v>
+        <v>256</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>448</v>
+        <v>366</v>
       </c>
       <c r="D36" s="25" t="b">
         <v>0</v>
@@ -3445,10 +3460,10 @@
         <v>0</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>445</v>
+        <v>363</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>444</v>
+        <v>362</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3456,10 +3471,10 @@
         <v>6</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>334</v>
+        <v>257</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>448</v>
+        <v>366</v>
       </c>
       <c r="D37" s="25" t="b">
         <v>0</v>
@@ -3477,21 +3492,21 @@
         <v>0</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>446</v>
+        <v>364</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>449</v>
+        <v>367</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>335</v>
+        <v>258</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>462</v>
+        <v>380</v>
       </c>
       <c r="D38" s="24" t="b">
         <v>0</v>
@@ -3509,21 +3524,21 @@
         <v>1</v>
       </c>
       <c r="I38" s="23" t="s">
-        <v>450</v>
+        <v>368</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>451</v>
+        <v>369</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>151</v>
+        <v>106</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>336</v>
+        <v>259</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>462</v>
+        <v>380</v>
       </c>
       <c r="D39" s="24" t="b">
         <v>0</v>
@@ -3541,21 +3556,21 @@
         <v>1</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>452</v>
+        <v>370</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>453</v>
+        <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>337</v>
+        <v>260</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>454</v>
+        <v>372</v>
       </c>
       <c r="D40" s="24" t="b">
         <v>0</v>
@@ -3573,21 +3588,21 @@
         <v>1</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>456</v>
+        <v>374</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>338</v>
+        <v>261</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>455</v>
+        <v>373</v>
       </c>
       <c r="D41" s="24" t="b">
         <v>0</v>
@@ -3605,21 +3620,21 @@
         <v>1</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>457</v>
+        <v>375</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>153</v>
+        <v>108</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>339</v>
+        <v>262</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>458</v>
+        <v>376</v>
       </c>
       <c r="D42" s="24" t="b">
         <v>0</v>
@@ -3637,21 +3652,21 @@
         <v>1</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>154</v>
+        <v>109</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>459</v>
+        <v>377</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>155</v>
+        <v>110</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>340</v>
+        <v>263</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>156</v>
+        <v>111</v>
       </c>
       <c r="D43" s="24" t="b">
         <v>0</v>
@@ -3669,21 +3684,21 @@
         <v>1</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>460</v>
+        <v>378</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>461</v>
+        <v>379</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
-        <v>157</v>
+        <v>112</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>341</v>
+        <v>264</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>463</v>
+        <v>381</v>
       </c>
       <c r="D44" s="24" t="b">
         <v>0</v>
@@ -3701,21 +3716,21 @@
         <v>1</v>
       </c>
       <c r="I44" s="23" t="s">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>465</v>
+        <v>383</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>159</v>
+        <v>114</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>342</v>
+        <v>265</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>464</v>
+        <v>382</v>
       </c>
       <c r="D45" s="24" t="b">
         <v>0</v>
@@ -3733,21 +3748,21 @@
         <v>1</v>
       </c>
       <c r="I45" s="23" t="s">
-        <v>158</v>
+        <v>113</v>
       </c>
       <c r="J45" s="30" t="s">
-        <v>149</v>
+        <v>384</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
-        <v>160</v>
+        <v>115</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>343</v>
+        <v>385</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>161</v>
+        <v>386</v>
       </c>
       <c r="D46" s="24" t="b">
         <v>0</v>
@@ -3765,21 +3780,21 @@
         <v>1</v>
       </c>
       <c r="I46" s="23" t="s">
-        <v>162</v>
+        <v>116</v>
       </c>
       <c r="J46" s="23" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>344</v>
+        <v>266</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>82</v>
+        <v>388</v>
       </c>
       <c r="D47" s="24" t="b">
         <v>0</v>
@@ -3797,21 +3812,21 @@
         <v>0</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>83</v>
+        <v>390</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
-        <v>164</v>
+        <v>117</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>345</v>
+        <v>267</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>165</v>
+        <v>392</v>
       </c>
       <c r="D48" s="25" t="b">
         <v>0</v>
@@ -3829,10 +3844,10 @@
         <v>0</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>166</v>
+        <v>118</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>167</v>
+        <v>393</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3840,42 +3855,42 @@
         <v>24</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>346</v>
+        <v>394</v>
       </c>
       <c r="C49" s="23" t="s">
+        <v>395</v>
+      </c>
+      <c r="D49" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F49" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G49" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H49" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="D49" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F49" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G49" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H49" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="I49" s="23" t="s">
-        <v>26</v>
-      </c>
       <c r="J49" s="23" t="s">
-        <v>27</v>
+        <v>396</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>347</v>
+        <v>268</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>86</v>
+        <v>397</v>
       </c>
       <c r="D50" s="24" t="b">
         <v>0</v>
@@ -3893,21 +3908,21 @@
         <v>0</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>87</v>
+        <v>398</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>88</v>
+        <v>399</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>89</v>
+        <v>64</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>348</v>
+        <v>269</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>90</v>
+        <v>397</v>
       </c>
       <c r="D51" s="24" t="b">
         <v>0</v>
@@ -3925,21 +3940,21 @@
         <v>0</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>91</v>
+        <v>400</v>
       </c>
       <c r="J51" s="30" t="s">
-        <v>92</v>
+        <v>401</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>168</v>
+        <v>119</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>349</v>
+        <v>270</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>169</v>
+        <v>402</v>
       </c>
       <c r="D52" s="25" t="b">
         <v>0</v>
@@ -3957,21 +3972,21 @@
         <v>1</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>170</v>
+        <v>403</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>350</v>
+        <v>271</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>29</v>
+        <v>405</v>
       </c>
       <c r="D53" s="25" t="b">
         <v>0</v>
@@ -3989,19 +4004,21 @@
         <v>1</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="J53" s="23"/>
+        <v>27</v>
+      </c>
+      <c r="J53" s="23" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>351</v>
+        <v>407</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>173</v>
+        <v>408</v>
       </c>
       <c r="D54" s="25" t="b">
         <v>0</v>
@@ -4019,21 +4036,21 @@
         <v>1</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>174</v>
+        <v>409</v>
       </c>
       <c r="J54" s="23" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>352</v>
+        <v>272</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>32</v>
+        <v>411</v>
       </c>
       <c r="D55" s="25" t="b">
         <v>0</v>
@@ -4051,21 +4068,21 @@
         <v>1</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>33</v>
+        <v>412</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>34</v>
+        <v>413</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>353</v>
+        <v>273</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>94</v>
+        <v>414</v>
       </c>
       <c r="D56" s="25" t="b">
         <v>0</v>
@@ -4083,21 +4100,21 @@
         <v>0</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>95</v>
+        <v>415</v>
       </c>
       <c r="J56" s="23" t="s">
-        <v>96</v>
+        <v>416</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
-        <v>176</v>
+        <v>121</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>354</v>
+        <v>274</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>177</v>
+        <v>417</v>
       </c>
       <c r="D57" s="24" t="b">
         <v>1</v>
@@ -4115,21 +4132,21 @@
         <v>0</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>178</v>
+        <v>122</v>
       </c>
       <c r="J57" s="23" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>355</v>
+        <v>275</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>98</v>
+        <v>419</v>
       </c>
       <c r="D58" s="24" t="b">
         <v>0</v>
@@ -4147,21 +4164,21 @@
         <v>0</v>
       </c>
       <c r="I58" s="23" t="s">
-        <v>99</v>
+        <v>420</v>
       </c>
       <c r="J58" s="23" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A59" s="22" t="s">
         <v>5</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>185</v>
+        <v>422</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>186</v>
+        <v>417</v>
       </c>
       <c r="D59" s="24" t="b">
         <v>1</v>
@@ -4179,21 +4196,21 @@
         <v>0</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="J59" s="23" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
-        <v>180</v>
+        <v>123</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>181</v>
+        <v>425</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>182</v>
+        <v>124</v>
       </c>
       <c r="D60" s="24" t="b">
         <v>1</v>
@@ -4211,27 +4228,27 @@
         <v>0</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>183</v>
+        <v>125</v>
       </c>
       <c r="J60" s="23" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>101</v>
+        <v>427</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>102</v>
+        <v>428</v>
       </c>
       <c r="D61" s="25" t="b">
         <v>0</v>
       </c>
       <c r="E61" s="25" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F61" s="24" t="b">
         <v>1</v>
@@ -4243,19 +4260,21 @@
         <v>0</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="J61" s="23"/>
-    </row>
-    <row r="62" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="J61" s="23" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="s">
-        <v>188</v>
+        <v>127</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>189</v>
+        <v>430</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>190</v>
+        <v>431</v>
       </c>
       <c r="D62" s="25" t="b">
         <v>0</v>
@@ -4273,21 +4292,21 @@
         <v>0</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>191</v>
+        <v>432</v>
       </c>
       <c r="J62" s="23" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A63" s="22" t="s">
-        <v>193</v>
+        <v>128</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>194</v>
+        <v>129</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>190</v>
+        <v>431</v>
       </c>
       <c r="D63" s="25" t="b">
         <v>0</v>
@@ -4305,21 +4324,21 @@
         <v>0</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>195</v>
-      </c>
-      <c r="J63" s="30" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+      <c r="J63" s="23" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A64" s="22" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>36</v>
+        <v>435</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>37</v>
+        <v>436</v>
       </c>
       <c r="D64" s="25" t="b">
         <v>0</v>
@@ -4337,21 +4356,21 @@
         <v>1</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="J64" s="23" t="s">
-        <v>39</v>
+        <v>393</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="22" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>41</v>
+        <v>437</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>42</v>
+        <v>438</v>
       </c>
       <c r="D65" s="25" t="b">
         <v>0</v>
@@ -4369,21 +4388,21 @@
         <v>1</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="J65" s="23" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A66" s="22" t="s">
-        <v>196</v>
+        <v>130</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>197</v>
+        <v>440</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>198</v>
+        <v>441</v>
       </c>
       <c r="D66" s="24" t="b">
         <v>0</v>
@@ -4401,21 +4420,21 @@
         <v>1</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>199</v>
+        <v>442</v>
       </c>
       <c r="J66" s="23" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A67" s="22" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>105</v>
+        <v>444</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>106</v>
+        <v>445</v>
       </c>
       <c r="D67" s="24" t="b">
         <v>0</v>
@@ -4433,19 +4452,21 @@
         <v>1</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="J67" s="23"/>
-    </row>
-    <row r="68" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>446</v>
+      </c>
+      <c r="J67" s="23" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A68" s="22" t="s">
-        <v>201</v>
+        <v>131</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>202</v>
+        <v>132</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>203</v>
+        <v>448</v>
       </c>
       <c r="D68" s="24" t="b">
         <v>1</v>
@@ -4463,53 +4484,53 @@
         <v>0</v>
       </c>
       <c r="I68" s="23" t="s">
-        <v>204</v>
+        <v>133</v>
       </c>
       <c r="J68" s="23" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+      <c r="A69" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69" s="23" t="s">
+        <v>450</v>
+      </c>
+      <c r="C69" s="23" t="s">
+        <v>452</v>
+      </c>
+      <c r="D69" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E69" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F69" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G69" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H69" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I69" s="23" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="69" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A69" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="B69" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="C69" s="23" t="s">
-        <v>207</v>
-      </c>
-      <c r="D69" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E69" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F69" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G69" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H69" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I69" s="23" t="s">
-        <v>208</v>
-      </c>
       <c r="J69" s="23" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A70" s="22" t="s">
-        <v>108</v>
+        <v>70</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>109</v>
+        <v>454</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>110</v>
+        <v>455</v>
       </c>
       <c r="D70" s="24" t="b">
         <v>0</v>
@@ -4527,19 +4548,21 @@
         <v>1</v>
       </c>
       <c r="I70" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="J70" s="23"/>
+        <v>71</v>
+      </c>
+      <c r="J70" s="23" t="s">
+        <v>456</v>
+      </c>
     </row>
     <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="22" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>46</v>
+        <v>457</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>47</v>
+        <v>458</v>
       </c>
       <c r="D71" s="25" t="b">
         <v>0</v>
@@ -4557,21 +4580,21 @@
         <v>1</v>
       </c>
       <c r="I71" s="23" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="J71" s="23" t="s">
-        <v>49</v>
+        <v>459</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="22" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>113</v>
+        <v>460</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>114</v>
+        <v>461</v>
       </c>
       <c r="D72" s="25" t="b">
         <v>0</v>
@@ -4589,19 +4612,21 @@
         <v>1</v>
       </c>
       <c r="I72" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="J72" s="23"/>
-    </row>
-    <row r="73" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="J72" s="23" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A73" s="22" t="s">
-        <v>210</v>
+        <v>136</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>211</v>
+        <v>462</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>212</v>
+        <v>463</v>
       </c>
       <c r="D73" s="24" t="b">
         <v>0</v>
@@ -4619,21 +4644,21 @@
         <v>1</v>
       </c>
       <c r="I73" s="23" t="s">
-        <v>213</v>
+        <v>137</v>
       </c>
       <c r="J73" s="23" t="s">
-        <v>214</v>
+        <v>449</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="22" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>51</v>
+        <v>464</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>52</v>
+        <v>465</v>
       </c>
       <c r="D74" s="24" t="b">
         <v>0</v>
@@ -4651,21 +4676,21 @@
         <v>0</v>
       </c>
       <c r="I74" s="23" t="s">
-        <v>53</v>
+        <v>466</v>
       </c>
       <c r="J74" s="24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A75" s="22" t="s">
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>117</v>
+        <v>468</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>118</v>
+        <v>469</v>
       </c>
       <c r="D75" s="24" t="b">
         <v>0</v>
@@ -4683,19 +4708,21 @@
         <v>0</v>
       </c>
       <c r="I75" s="23" t="s">
-        <v>119</v>
-      </c>
-      <c r="J75" s="23"/>
+        <v>75</v>
+      </c>
+      <c r="J75" s="23" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="22" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>56</v>
+        <v>37</v>
       </c>
       <c r="C76" s="23" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D76" s="25" t="b">
         <v>0</v>
@@ -4713,21 +4740,21 @@
         <v>1</v>
       </c>
       <c r="I76" s="23" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="J76" s="23" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="22" t="s">
-        <v>60</v>
+        <v>41</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>57</v>
+        <v>38</v>
       </c>
       <c r="D77" s="25" t="b">
         <v>0</v>
@@ -4745,21 +4772,21 @@
         <v>1</v>
       </c>
       <c r="I77" s="23" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="J77" s="23" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="22" t="s">
-        <v>215</v>
+        <v>138</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>216</v>
+        <v>139</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>217</v>
+        <v>140</v>
       </c>
       <c r="D78" s="25" t="b">
         <v>0</v>
@@ -4777,21 +4804,21 @@
         <v>0</v>
       </c>
       <c r="I78" s="23" t="s">
-        <v>218</v>
+        <v>141</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>219</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
-        <v>220</v>
+        <v>143</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>221</v>
+        <v>144</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>222</v>
+        <v>145</v>
       </c>
       <c r="D79" s="24" t="b">
         <v>1</v>
@@ -4809,21 +4836,21 @@
         <v>0</v>
       </c>
       <c r="I79" s="23" t="s">
-        <v>223</v>
+        <v>146</v>
       </c>
       <c r="J79" s="23" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="D80" s="25" t="b">
         <v>0</v>
@@ -4841,21 +4868,21 @@
         <v>0</v>
       </c>
       <c r="I80" s="23" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="J80" s="23" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
-        <v>120</v>
+        <v>76</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>122</v>
+        <v>78</v>
       </c>
       <c r="D81" s="24" t="b">
         <v>1</v>
@@ -4873,21 +4900,21 @@
         <v>1</v>
       </c>
       <c r="I81" s="23" t="s">
-        <v>123</v>
+        <v>79</v>
       </c>
       <c r="J81" s="23" t="s">
-        <v>124</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
-        <v>224</v>
+        <v>147</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>225</v>
+        <v>148</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>226</v>
+        <v>149</v>
       </c>
       <c r="D82" s="24" t="b">
         <v>0</v>
@@ -4905,21 +4932,21 @@
         <v>1</v>
       </c>
       <c r="I82" s="23" t="s">
-        <v>227</v>
+        <v>150</v>
       </c>
       <c r="J82" s="23" t="s">
-        <v>228</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
-        <v>229</v>
+        <v>152</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>230</v>
+        <v>153</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>231</v>
+        <v>154</v>
       </c>
       <c r="D83" s="25" t="b">
         <v>0</v>
@@ -4937,21 +4964,21 @@
         <v>0</v>
       </c>
       <c r="I83" s="23" t="s">
-        <v>232</v>
+        <v>155</v>
       </c>
       <c r="J83" s="23" t="s">
-        <v>233</v>
+        <v>156</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
-        <v>328</v>
+        <v>251</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>125</v>
+        <v>81</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="D84" s="24" t="b">
         <v>1</v>
@@ -4969,10 +4996,10 @@
         <v>0</v>
       </c>
       <c r="I84" s="23" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="J84" s="23" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4980,10 +5007,10 @@
         <v>4</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>125</v>
+        <v>423</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="D85" s="24" t="b">
         <v>1</v>
@@ -5001,21 +5028,21 @@
         <v>0</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="J85" s="23" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="22" t="s">
-        <v>234</v>
+        <v>157</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>235</v>
+        <v>158</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>236</v>
+        <v>159</v>
       </c>
       <c r="D86" s="25" t="b">
         <v>0</v>
@@ -5033,21 +5060,21 @@
         <v>0</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>237</v>
+        <v>160</v>
       </c>
       <c r="J86" s="23" t="s">
-        <v>238</v>
+        <v>161</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="22" t="s">
-        <v>239</v>
+        <v>162</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>240</v>
+        <v>163</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>241</v>
+        <v>164</v>
       </c>
       <c r="D87" s="24" t="b">
         <v>1</v>
@@ -5065,21 +5092,21 @@
         <v>0</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>242</v>
+        <v>165</v>
       </c>
       <c r="J87" s="23" t="s">
-        <v>243</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="22" t="s">
-        <v>244</v>
+        <v>167</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>245</v>
+        <v>168</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>246</v>
+        <v>169</v>
       </c>
       <c r="D88" s="24" t="b">
         <v>1</v>
@@ -5097,21 +5124,21 @@
         <v>0</v>
       </c>
       <c r="I88" s="23" t="s">
-        <v>247</v>
+        <v>170</v>
       </c>
       <c r="J88" s="23" t="s">
-        <v>248</v>
+        <v>171</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="28" t="s">
-        <v>249</v>
+        <v>172</v>
       </c>
       <c r="B89" s="29" t="s">
-        <v>250</v>
+        <v>173</v>
       </c>
       <c r="C89" s="29" t="s">
-        <v>251</v>
+        <v>174</v>
       </c>
       <c r="D89" s="27"/>
       <c r="E89" s="27"/>
@@ -5119,7 +5146,7 @@
       <c r="G89" s="27"/>
       <c r="H89" s="27"/>
       <c r="I89" s="29" t="s">
-        <v>252</v>
+        <v>175</v>
       </c>
       <c r="J89" s="23"/>
     </row>
@@ -8057,34 +8084,34 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>253</v>
+        <v>176</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>254</v>
+        <v>177</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>255</v>
+        <v>178</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>256</v>
+        <v>179</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>257</v>
+        <v>180</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>258</v>
+        <v>181</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>259</v>
+        <v>182</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>260</v>
+        <v>183</v>
       </c>
       <c r="E2" s="4" t="b">
         <v>1</v>
@@ -8092,16 +8119,16 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>262</v>
+        <v>185</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>263</v>
+        <v>186</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>264</v>
+        <v>187</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>261</v>
+        <v>184</v>
       </c>
       <c r="E3" s="4" t="b">
         <v>1</v>
@@ -8109,16 +8136,16 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>265</v>
+        <v>188</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>266</v>
+        <v>189</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>267</v>
+        <v>190</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>268</v>
+        <v>191</v>
       </c>
       <c r="E4" s="4" t="b">
         <v>1</v>
@@ -8126,16 +8153,16 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>269</v>
+        <v>192</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>270</v>
+        <v>193</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>271</v>
+        <v>194</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>268</v>
+        <v>191</v>
       </c>
       <c r="E5" s="4" t="b">
         <v>1</v>
@@ -8143,16 +8170,16 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>272</v>
+        <v>195</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>273</v>
+        <v>196</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>274</v>
+        <v>197</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>260</v>
+        <v>183</v>
       </c>
       <c r="E6" s="4" t="b">
         <v>1</v>
@@ -8160,16 +8187,16 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>275</v>
+        <v>198</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>276</v>
+        <v>199</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>277</v>
+        <v>200</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>278</v>
+        <v>201</v>
       </c>
       <c r="E7" s="4" t="b">
         <v>0</v>
@@ -8177,16 +8204,16 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>279</v>
+        <v>202</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>280</v>
+        <v>203</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>281</v>
+        <v>204</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>278</v>
+        <v>201</v>
       </c>
       <c r="E8" s="4" t="b">
         <v>0</v>
@@ -8194,16 +8221,16 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>282</v>
+        <v>205</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>280</v>
+        <v>203</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>283</v>
+        <v>206</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>278</v>
+        <v>201</v>
       </c>
       <c r="E9" s="4" t="b">
         <v>0</v>
@@ -8211,16 +8238,16 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>284</v>
+        <v>207</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>285</v>
+        <v>208</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>286</v>
+        <v>209</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>261</v>
+        <v>184</v>
       </c>
       <c r="E10" s="4" t="b">
         <v>0</v>
@@ -8228,16 +8255,16 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>287</v>
+        <v>210</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>288</v>
+        <v>211</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>289</v>
+        <v>212</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>260</v>
+        <v>183</v>
       </c>
       <c r="E11" s="4" t="b">
         <v>0</v>
@@ -8245,16 +8272,16 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>290</v>
+        <v>213</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>291</v>
+        <v>214</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>292</v>
+        <v>215</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>268</v>
+        <v>191</v>
       </c>
       <c r="E12" s="4" t="b">
         <v>0</v>
@@ -8588,27 +8615,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>253</v>
+        <v>176</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>254</v>
+        <v>177</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>256</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>293</v>
+        <v>216</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>294</v>
+        <v>217</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>295</v>
+        <v>218</v>
       </c>
       <c r="D2" s="4" t="b">
         <v>1</v>
@@ -8616,13 +8643,13 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
-        <v>296</v>
+        <v>219</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>297</v>
+        <v>220</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>298</v>
+        <v>221</v>
       </c>
       <c r="D3" s="4" t="b">
         <v>1</v>
@@ -8630,13 +8657,13 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>299</v>
+        <v>222</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>300</v>
+        <v>223</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>301</v>
+        <v>224</v>
       </c>
       <c r="D4" s="4" t="b">
         <v>1</v>
@@ -8644,13 +8671,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>302</v>
+        <v>225</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>303</v>
+        <v>226</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>304</v>
+        <v>227</v>
       </c>
       <c r="D5" s="4" t="b">
         <v>1</v>
@@ -8658,13 +8685,13 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>305</v>
+        <v>228</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>306</v>
+        <v>229</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>307</v>
+        <v>230</v>
       </c>
       <c r="D6" s="4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
finished updating the metadata
</commit_message>
<xml_diff>
--- a/metadata/binddata.xlsx
+++ b/metadata/binddata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ual895/Git/newdictionary/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B9FA61-74A9-1C47-8773-B33522A51A42}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890781FE-CCBF-2B45-9EF9-E5315FF5928D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="500" windowWidth="27800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29440" yWindow="5440" windowWidth="27800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primitives" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="471">
   <si>
     <t>primitive</t>
   </si>
@@ -427,45 +427,15 @@
     <t>sort-by</t>
   </si>
   <si>
-    <t>sort a list based on a user-defined comparison reporter</t>
-  </si>
-  <si>
-    <t>list, array</t>
-  </si>
-  <si>
-    <t>sort-on, sort, count, mean</t>
-  </si>
-  <si>
-    <t>Ask Ordering Example</t>
-  </si>
-  <si>
     <t>sort-on</t>
   </si>
   <si>
-    <t>sort an agentset into a list ordered by the value of a given reporter</t>
-  </si>
-  <si>
-    <t>sort-by, sort, count, mean</t>
-  </si>
-  <si>
-    <t>Birthdays</t>
-  </si>
-  <si>
     <t>tie</t>
   </si>
   <si>
-    <t>make a link into a solid connection that can move turtles in the world</t>
-  </si>
-  <si>
-    <t>link, connection, attachment</t>
-  </si>
-  <si>
     <t>links, create-links-with, link-neighbors, layout-circle</t>
   </si>
   <si>
-    <t>Tie System Example</t>
-  </si>
-  <si>
     <t>ask</t>
   </si>
   <si>
@@ -499,9 +469,6 @@
     <t>right, heading, turtles, move-to</t>
   </si>
   <si>
-    <t>Ant Lines</t>
-  </si>
-  <si>
     <t>move-to</t>
   </si>
   <si>
@@ -553,18 +520,6 @@
     <t>to, begin, command</t>
   </si>
   <si>
-    <t>to-report, end, ask, repeat</t>
-  </si>
-  <si>
-    <t>Bird Breeder, Rabbits Grass Weeds</t>
-  </si>
-  <si>
-    <t>used to complete actions in NetLogo</t>
-  </si>
-  <si>
-    <t>turtle, shape, triangle</t>
-  </si>
-  <si>
     <t>ask, turtles-own, patches, links</t>
   </si>
   <si>
@@ -589,9 +544,6 @@
     <t>to, to-report, ask, semicolon</t>
   </si>
   <si>
-    <t>Wolf Sheep Predation, Forest Fire, Segregation</t>
-  </si>
-  <si>
     <t>face</t>
   </si>
   <si>
@@ -733,90 +685,39 @@
     <t>sprout</t>
   </si>
   <si>
-    <t>Create new turtles from a patch.</t>
-  </si>
-  <si>
-    <t>create, birth, new, turtles</t>
-  </si>
-  <si>
     <t>hatch, create-turtles, die, ask</t>
   </si>
   <si>
-    <t>Fire, Paths, Segregation</t>
-  </si>
-  <si>
     <t>tick</t>
   </si>
   <si>
-    <t>Advance the tick counter by 1.</t>
-  </si>
-  <si>
-    <t>time, counter</t>
-  </si>
-  <si>
-    <t>reset-ticks, to, repeat, clear-all</t>
-  </si>
-  <si>
     <t>to-report</t>
   </si>
   <si>
     <t>Begin a procedure to create a custom reporter.</t>
   </si>
   <si>
-    <t>reporter, procedure</t>
-  </si>
-  <si>
-    <t>to, end, ask, if-else</t>
-  </si>
-  <si>
-    <t>Boiling, Rebellion, Scatter</t>
-  </si>
-  <si>
     <t>towards</t>
   </si>
   <si>
     <t>Reports the angle of the caller towards an agent.</t>
   </si>
   <si>
-    <t>turn, angle, face</t>
-  </si>
-  <si>
     <t>face, right, left, heading</t>
   </si>
   <si>
-    <t>Moths, Flocking, Paths</t>
-  </si>
-  <si>
     <t>turtles-here</t>
   </si>
   <si>
     <t>Reports the agentset of all the turtles on a caller's patch.</t>
   </si>
   <si>
-    <t>turtles, here, location, with</t>
-  </si>
-  <si>
-    <t>count, neighbors, patches, other</t>
-  </si>
-  <si>
-    <t>Segregation, Rebellion, Virus</t>
-  </si>
-  <si>
     <t>turtles-own</t>
   </si>
   <si>
     <t>Declare a variable that belongs to turtles.</t>
   </si>
   <si>
-    <t>turtle, variable, declare, own</t>
-  </si>
-  <si>
-    <t>set, of, patches-own, globals</t>
-  </si>
-  <si>
-    <t>Segregation, Traffic Basic, Flocking</t>
-  </si>
-  <si>
     <t>while</t>
   </si>
   <si>
@@ -833,15 +734,6 @@
   </si>
   <si>
     <t>with</t>
-  </si>
-  <si>
-    <t>Narrows down an agentset.</t>
-  </si>
-  <si>
-    <t>specific, agentset</t>
-  </si>
-  <si>
-    <t>turtles, if, ask</t>
   </si>
   <si>
     <t>title</t>
@@ -1742,6 +1634,114 @@
   </si>
   <si>
     <t>Urban Suite - Pollution, Traffic Intersection, Mimicry, Ant Lines</t>
+  </si>
+  <si>
+    <t>Hoteling's Law, GasLab Circular Particles, CRISPR Bacterium, Ask Ordering Example</t>
+  </si>
+  <si>
+    <t>sort-on, count, mean, ask</t>
+  </si>
+  <si>
+    <t>sort-by, count, mean, ask</t>
+  </si>
+  <si>
+    <t>Reports a sorted version of a provided list based on a user-defined comparison.</t>
+  </si>
+  <si>
+    <t>Reports a sorted version of a provided agentset based on a user-defined comparison.</t>
+  </si>
+  <si>
+    <t>list, array, order, arrange, sift, cull, assort</t>
+  </si>
+  <si>
+    <t>Birthdays, Dice, DNA Protein Synthesis, Rnd Example</t>
+  </si>
+  <si>
+    <t>Daisyworld, Ant Lines, Heatbugs, Fairy Circles</t>
+  </si>
+  <si>
+    <t>create, birth, new, turtle, grow, germinate, spring, vegetate, root</t>
+  </si>
+  <si>
+    <t>Advances the tick counter by 1.</t>
+  </si>
+  <si>
+    <t>Creates new turtles at the center of a patch.</t>
+  </si>
+  <si>
+    <t>time, counter, clock, watch</t>
+  </si>
+  <si>
+    <t>reset-ticks, ask, to, clear-all</t>
+  </si>
+  <si>
+    <t>Flocking, BeeSmart Hive Finding, Slime, Shepherds</t>
+  </si>
+  <si>
+    <t>Turns a link between two turtles into a rigid connection so that the movement of one turtle impacts the movement of the other.</t>
+  </si>
+  <si>
+    <t>link, connection, attachment, lock, hook, anchor</t>
+  </si>
+  <si>
+    <t>Vision Evolution, DNA Replication Fork, Bug Hunt Environmental Changes, Connected Chemistry 8 Gas Particle Sandbox</t>
+  </si>
+  <si>
+    <t>Wolf Sheep Predation, Fire, Ants, Segregation</t>
+  </si>
+  <si>
+    <t>Mimicry, Moths, Rock Paper Scissors, HIV</t>
+  </si>
+  <si>
+    <t>to-report, end, ask, create-turtles</t>
+  </si>
+  <si>
+    <t>to, end, ask, if</t>
+  </si>
+  <si>
+    <t>procedure, function, return, calculate, transform, input, output</t>
+  </si>
+  <si>
+    <t>turn, angle, face, direction, twist, spin</t>
+  </si>
+  <si>
+    <t>Chaos in a Box, Bug Hunt Coevolution, GenEvo 1 Genetic Switch, Traffic 2 Lanes</t>
+  </si>
+  <si>
+    <t>shape, triangle, mobile, agent, tortoise, animal, person, people, object, thing</t>
+  </si>
+  <si>
+    <t>Reports a specific turtle that has the provided who number.</t>
+  </si>
+  <si>
+    <t>El Farol, Party, Segregation, Chemical Equilibrium</t>
+  </si>
+  <si>
+    <t>neighbors, patches, other, in-radius</t>
+  </si>
+  <si>
+    <t>touch, contact, near, communicate, rub, tangent, tap, collide, notice, recognize, sense</t>
+  </si>
+  <si>
+    <t>Disease Solo, Flocking Vee Formations, Tumor, Wolf Sheep Predation</t>
+  </si>
+  <si>
+    <t>set, globals, patches-own, with, of</t>
+  </si>
+  <si>
+    <t>variable, declare, characteristic, property, attribute, trait, quality, phenotype</t>
+  </si>
+  <si>
+    <t>Reports a subset of the original agentset that only contains the agents with specified characteristics.</t>
+  </si>
+  <si>
+    <t>specific, agentset, query, narrow, subset, reduce, fragment, select</t>
+  </si>
+  <si>
+    <t>if, of, turtles-own, patches-own</t>
+  </si>
+  <si>
+    <t>Fur, Mimicry, Ants, Heatbugs</t>
   </si>
 </sst>
 </file>
@@ -2279,9 +2279,9 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2348,13 +2348,13 @@
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>231</v>
+        <v>195</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>276</v>
+        <v>240</v>
       </c>
       <c r="D2" s="24" t="b">
         <v>0</v>
@@ -2372,10 +2372,10 @@
         <v>1</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>277</v>
+        <v>241</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>278</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2383,10 +2383,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>232</v>
+        <v>196</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>281</v>
+        <v>245</v>
       </c>
       <c r="D3" s="24" t="b">
         <v>0</v>
@@ -2404,10 +2404,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>280</v>
+        <v>244</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>279</v>
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2415,10 +2415,10 @@
         <v>11</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>233</v>
+        <v>197</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>282</v>
+        <v>246</v>
       </c>
       <c r="D4" s="25" t="b">
         <v>0</v>
@@ -2436,21 +2436,21 @@
         <v>1</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>283</v>
+        <v>247</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>284</v>
+        <v>248</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>287</v>
+        <v>251</v>
       </c>
       <c r="D5" s="24" t="b">
         <v>1</v>
@@ -2468,10 +2468,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>286</v>
+        <v>250</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>285</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2479,10 +2479,10 @@
         <v>12</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>235</v>
+        <v>199</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>288</v>
+        <v>252</v>
       </c>
       <c r="D6" s="24" t="b">
         <v>1</v>
@@ -2500,21 +2500,21 @@
         <v>0</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>289</v>
+        <v>253</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>290</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>236</v>
+        <v>200</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>330</v>
+        <v>294</v>
       </c>
       <c r="D7" s="24" t="b">
         <v>0</v>
@@ -2532,21 +2532,21 @@
         <v>1</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>291</v>
+        <v>255</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>292</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>249</v>
+        <v>213</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>237</v>
+        <v>201</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>295</v>
+        <v>259</v>
       </c>
       <c r="D8" s="24" t="b">
         <v>1</v>
@@ -2564,21 +2564,21 @@
         <v>0</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>294</v>
+        <v>258</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>237</v>
+        <v>201</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>295</v>
+        <v>259</v>
       </c>
       <c r="D9" s="24" t="b">
         <v>1</v>
@@ -2596,21 +2596,21 @@
         <v>0</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>294</v>
+        <v>258</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>293</v>
+        <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>238</v>
+        <v>202</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>295</v>
+        <v>259</v>
       </c>
       <c r="D10" s="24" t="b">
         <v>1</v>
@@ -2628,21 +2628,21 @@
         <v>0</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>296</v>
+        <v>260</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>298</v>
+        <v>262</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>239</v>
+        <v>203</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>295</v>
+        <v>259</v>
       </c>
       <c r="D11" s="24" t="b">
         <v>1</v>
@@ -2660,21 +2660,21 @@
         <v>0</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>297</v>
+        <v>261</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>299</v>
+        <v>263</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>313</v>
+        <v>277</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="D12" s="24" t="b">
         <v>0</v>
@@ -2692,21 +2692,21 @@
         <v>0</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>300</v>
+        <v>264</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>301</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>86</v>
+        <v>71</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>240</v>
+        <v>204</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="D13" s="24" t="b">
         <v>0</v>
@@ -2724,10 +2724,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>304</v>
+        <v>268</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>305</v>
+        <v>269</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2735,10 +2735,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="23" t="s">
-        <v>241</v>
+        <v>205</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>365</v>
+        <v>329</v>
       </c>
       <c r="D14" s="25" t="b">
         <v>0</v>
@@ -2759,18 +2759,18 @@
         <v>14</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>306</v>
+        <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>250</v>
+        <v>214</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>308</v>
+        <v>272</v>
       </c>
       <c r="D15" s="24" t="b">
         <v>1</v>
@@ -2788,21 +2788,21 @@
         <v>0</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>242</v>
+        <v>206</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>307</v>
+        <v>271</v>
       </c>
       <c r="D16" s="24" t="b">
         <v>1</v>
@@ -2820,21 +2820,21 @@
         <v>0</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>309</v>
+        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>87</v>
+        <v>72</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>243</v>
+        <v>207</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>312</v>
+        <v>276</v>
       </c>
       <c r="D17" s="25" t="b">
         <v>0</v>
@@ -2852,10 +2852,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>311</v>
+        <v>275</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>310</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -2863,10 +2863,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>314</v>
+        <v>278</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>315</v>
+        <v>279</v>
       </c>
       <c r="D18" s="25" t="b">
         <v>0</v>
@@ -2884,21 +2884,21 @@
         <v>0</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>316</v>
+        <v>280</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>317</v>
+        <v>281</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>321</v>
+        <v>285</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>320</v>
+        <v>284</v>
       </c>
       <c r="D19" s="25" t="b">
         <v>0</v>
@@ -2916,21 +2916,21 @@
         <v>0</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>319</v>
+        <v>283</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>318</v>
+        <v>282</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>244</v>
+        <v>208</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>322</v>
+        <v>286</v>
       </c>
       <c r="D20" s="24" t="b">
         <v>1</v>
@@ -2948,21 +2948,21 @@
         <v>0</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>323</v>
+        <v>287</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>326</v>
+        <v>290</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>325</v>
+        <v>289</v>
       </c>
       <c r="D21" s="25" t="b">
         <v>0</v>
@@ -2980,21 +2980,21 @@
         <v>0</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>324</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>327</v>
+        <v>291</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>325</v>
+        <v>289</v>
       </c>
       <c r="D22" s="24" t="b">
         <v>0</v>
@@ -3012,21 +3012,21 @@
         <v>0</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>328</v>
+        <v>292</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>245</v>
+        <v>209</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>330</v>
+        <v>294</v>
       </c>
       <c r="D23" s="24" t="b">
         <v>0</v>
@@ -3044,21 +3044,21 @@
         <v>1</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>329</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>389</v>
+        <v>353</v>
       </c>
       <c r="D24" s="24" t="b">
         <v>0</v>
@@ -3076,21 +3076,21 @@
         <v>0</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>331</v>
+        <v>295</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
-        <v>248</v>
+        <v>212</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>246</v>
+        <v>210</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>389</v>
+        <v>353</v>
       </c>
       <c r="D25" s="24" t="b">
         <v>0</v>
@@ -3108,10 +3108,10 @@
         <v>0</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>331</v>
+        <v>295</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3119,10 +3119,10 @@
         <v>16</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>332</v>
+        <v>296</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>333</v>
+        <v>297</v>
       </c>
       <c r="D26" s="24" t="b">
         <v>1</v>
@@ -3140,21 +3140,21 @@
         <v>0</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>334</v>
+        <v>298</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>335</v>
+        <v>299</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>338</v>
+        <v>302</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>337</v>
+        <v>301</v>
       </c>
       <c r="D27" s="25" t="b">
         <v>0</v>
@@ -3172,21 +3172,21 @@
         <v>0</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>340</v>
+        <v>304</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>342</v>
+        <v>306</v>
       </c>
       <c r="D28" s="24" t="b">
         <v>0</v>
@@ -3204,10 +3204,10 @@
         <v>1</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>339</v>
+        <v>303</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3215,10 +3215,10 @@
         <v>17</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>341</v>
+        <v>305</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>343</v>
+        <v>307</v>
       </c>
       <c r="D29" s="25" t="b">
         <v>0</v>
@@ -3236,10 +3236,10 @@
         <v>1</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>344</v>
+        <v>308</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>345</v>
+        <v>309</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3247,10 +3247,10 @@
         <v>18</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>247</v>
+        <v>211</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>346</v>
+        <v>310</v>
       </c>
       <c r="D30" s="25" t="b">
         <v>0</v>
@@ -3268,10 +3268,10 @@
         <v>1</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>347</v>
+        <v>311</v>
       </c>
       <c r="J30" s="29" t="s">
-        <v>348</v>
+        <v>312</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3279,10 +3279,10 @@
         <v>19</v>
       </c>
       <c r="B31" s="23" t="s">
-        <v>253</v>
+        <v>217</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>351</v>
+        <v>315</v>
       </c>
       <c r="D31" s="25" t="b">
         <v>0</v>
@@ -3303,7 +3303,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3311,10 +3311,10 @@
         <v>21</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>252</v>
+        <v>216</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>350</v>
+        <v>314</v>
       </c>
       <c r="D32" s="25" t="b">
         <v>0</v>
@@ -3332,10 +3332,10 @@
         <v>0</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>352</v>
+        <v>316</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>353</v>
+        <v>317</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3343,10 +3343,10 @@
         <v>22</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>354</v>
+        <v>318</v>
       </c>
       <c r="D33" s="24" t="b">
         <v>1</v>
@@ -3364,21 +3364,21 @@
         <v>0</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>355</v>
+        <v>319</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>356</v>
+        <v>320</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>451</v>
+        <v>415</v>
       </c>
       <c r="D34" s="25" t="b">
         <v>0</v>
@@ -3396,21 +3396,21 @@
         <v>0</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>357</v>
+        <v>321</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>358</v>
+        <v>322</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>359</v>
+        <v>323</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>360</v>
+        <v>324</v>
       </c>
       <c r="D35" s="24" t="b">
         <v>0</v>
@@ -3428,10 +3428,10 @@
         <v>1</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>361</v>
+        <v>325</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3439,10 +3439,10 @@
         <v>23</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>366</v>
+        <v>330</v>
       </c>
       <c r="D36" s="25" t="b">
         <v>0</v>
@@ -3460,10 +3460,10 @@
         <v>0</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>363</v>
+        <v>327</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>362</v>
+        <v>326</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3471,10 +3471,10 @@
         <v>6</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>366</v>
+        <v>330</v>
       </c>
       <c r="D37" s="25" t="b">
         <v>0</v>
@@ -3492,21 +3492,21 @@
         <v>0</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>364</v>
+        <v>328</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>367</v>
+        <v>331</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>107</v>
+        <v>91</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>380</v>
+        <v>344</v>
       </c>
       <c r="D38" s="24" t="b">
         <v>0</v>
@@ -3524,21 +3524,21 @@
         <v>1</v>
       </c>
       <c r="I38" s="23" t="s">
-        <v>368</v>
+        <v>332</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>369</v>
+        <v>333</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>259</v>
+        <v>223</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>380</v>
+        <v>344</v>
       </c>
       <c r="D39" s="24" t="b">
         <v>0</v>
@@ -3556,21 +3556,21 @@
         <v>1</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>370</v>
+        <v>334</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>371</v>
+        <v>335</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>103</v>
+        <v>87</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>372</v>
+        <v>336</v>
       </c>
       <c r="D40" s="24" t="b">
         <v>0</v>
@@ -3588,21 +3588,21 @@
         <v>1</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>374</v>
+        <v>338</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>105</v>
+        <v>89</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>373</v>
+        <v>337</v>
       </c>
       <c r="D41" s="24" t="b">
         <v>0</v>
@@ -3620,21 +3620,21 @@
         <v>1</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>104</v>
+        <v>88</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>375</v>
+        <v>339</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>108</v>
+        <v>92</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>376</v>
+        <v>340</v>
       </c>
       <c r="D42" s="24" t="b">
         <v>0</v>
@@ -3652,21 +3652,21 @@
         <v>1</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>109</v>
+        <v>93</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>377</v>
+        <v>341</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>110</v>
+        <v>94</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>111</v>
+        <v>95</v>
       </c>
       <c r="D43" s="24" t="b">
         <v>0</v>
@@ -3684,21 +3684,21 @@
         <v>1</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>378</v>
+        <v>342</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>379</v>
+        <v>343</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
-        <v>112</v>
+        <v>96</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>381</v>
+        <v>345</v>
       </c>
       <c r="D44" s="24" t="b">
         <v>0</v>
@@ -3716,21 +3716,21 @@
         <v>1</v>
       </c>
       <c r="I44" s="23" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>383</v>
+        <v>347</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>382</v>
+        <v>346</v>
       </c>
       <c r="D45" s="24" t="b">
         <v>0</v>
@@ -3748,21 +3748,21 @@
         <v>1</v>
       </c>
       <c r="I45" s="23" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="J45" s="30" t="s">
-        <v>384</v>
+        <v>348</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>385</v>
+        <v>349</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>386</v>
+        <v>350</v>
       </c>
       <c r="D46" s="24" t="b">
         <v>0</v>
@@ -3780,21 +3780,21 @@
         <v>1</v>
       </c>
       <c r="I46" s="23" t="s">
-        <v>116</v>
+        <v>100</v>
       </c>
       <c r="J46" s="23" t="s">
-        <v>387</v>
+        <v>351</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>388</v>
+        <v>352</v>
       </c>
       <c r="D47" s="24" t="b">
         <v>0</v>
@@ -3812,21 +3812,21 @@
         <v>0</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>390</v>
+        <v>354</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>391</v>
+        <v>355</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
-        <v>117</v>
+        <v>101</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>267</v>
+        <v>231</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>392</v>
+        <v>356</v>
       </c>
       <c r="D48" s="25" t="b">
         <v>0</v>
@@ -3844,10 +3844,10 @@
         <v>0</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>393</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3855,10 +3855,10 @@
         <v>24</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>394</v>
+        <v>358</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>395</v>
+        <v>359</v>
       </c>
       <c r="D49" s="25" t="b">
         <v>0</v>
@@ -3879,18 +3879,18 @@
         <v>25</v>
       </c>
       <c r="J49" s="23" t="s">
-        <v>396</v>
+        <v>360</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>268</v>
+        <v>232</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>397</v>
+        <v>361</v>
       </c>
       <c r="D50" s="24" t="b">
         <v>0</v>
@@ -3908,21 +3908,21 @@
         <v>0</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>398</v>
+        <v>362</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>399</v>
+        <v>363</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>269</v>
+        <v>233</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>397</v>
+        <v>361</v>
       </c>
       <c r="D51" s="24" t="b">
         <v>0</v>
@@ -3940,21 +3940,21 @@
         <v>0</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>400</v>
+        <v>364</v>
       </c>
       <c r="J51" s="30" t="s">
-        <v>401</v>
+        <v>365</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>119</v>
+        <v>103</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>270</v>
+        <v>234</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>402</v>
+        <v>366</v>
       </c>
       <c r="D52" s="25" t="b">
         <v>0</v>
@@ -3972,10 +3972,10 @@
         <v>1</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>403</v>
+        <v>367</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>404</v>
+        <v>368</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3983,10 +3983,10 @@
         <v>26</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>271</v>
+        <v>235</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>405</v>
+        <v>369</v>
       </c>
       <c r="D53" s="25" t="b">
         <v>0</v>
@@ -4007,18 +4007,18 @@
         <v>27</v>
       </c>
       <c r="J53" s="23" t="s">
-        <v>406</v>
+        <v>370</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
-        <v>120</v>
+        <v>104</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>407</v>
+        <v>371</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>408</v>
+        <v>372</v>
       </c>
       <c r="D54" s="25" t="b">
         <v>0</v>
@@ -4036,10 +4036,10 @@
         <v>1</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>409</v>
+        <v>373</v>
       </c>
       <c r="J54" s="23" t="s">
-        <v>410</v>
+        <v>374</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4047,10 +4047,10 @@
         <v>28</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>272</v>
+        <v>236</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>411</v>
+        <v>375</v>
       </c>
       <c r="D55" s="25" t="b">
         <v>0</v>
@@ -4068,21 +4068,21 @@
         <v>1</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>412</v>
+        <v>376</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>413</v>
+        <v>377</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>273</v>
+        <v>237</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>414</v>
+        <v>378</v>
       </c>
       <c r="D56" s="25" t="b">
         <v>0</v>
@@ -4100,21 +4100,21 @@
         <v>0</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>415</v>
+        <v>379</v>
       </c>
       <c r="J56" s="23" t="s">
-        <v>416</v>
+        <v>380</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>417</v>
+        <v>381</v>
       </c>
       <c r="D57" s="24" t="b">
         <v>1</v>
@@ -4132,21 +4132,21 @@
         <v>0</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="J57" s="23" t="s">
-        <v>418</v>
+        <v>382</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>419</v>
+        <v>383</v>
       </c>
       <c r="D58" s="24" t="b">
         <v>0</v>
@@ -4164,10 +4164,10 @@
         <v>0</v>
       </c>
       <c r="I58" s="23" t="s">
-        <v>420</v>
+        <v>384</v>
       </c>
       <c r="J58" s="23" t="s">
-        <v>421</v>
+        <v>385</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4175,10 +4175,10 @@
         <v>5</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>422</v>
+        <v>386</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>417</v>
+        <v>381</v>
       </c>
       <c r="D59" s="24" t="b">
         <v>1</v>
@@ -4196,21 +4196,21 @@
         <v>0</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>126</v>
+        <v>110</v>
       </c>
       <c r="J59" s="23" t="s">
-        <v>424</v>
+        <v>388</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>425</v>
+        <v>389</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
       <c r="D60" s="24" t="b">
         <v>1</v>
@@ -4228,21 +4228,21 @@
         <v>0</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>125</v>
+        <v>109</v>
       </c>
       <c r="J60" s="23" t="s">
-        <v>426</v>
+        <v>390</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>427</v>
+        <v>391</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>428</v>
+        <v>392</v>
       </c>
       <c r="D61" s="25" t="b">
         <v>0</v>
@@ -4260,21 +4260,21 @@
         <v>0</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>68</v>
+        <v>57</v>
       </c>
       <c r="J61" s="23" t="s">
-        <v>429</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>430</v>
+        <v>394</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>431</v>
+        <v>395</v>
       </c>
       <c r="D62" s="25" t="b">
         <v>0</v>
@@ -4292,21 +4292,21 @@
         <v>0</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>432</v>
+        <v>396</v>
       </c>
       <c r="J62" s="23" t="s">
-        <v>433</v>
+        <v>397</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A63" s="22" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>431</v>
+        <v>395</v>
       </c>
       <c r="D63" s="25" t="b">
         <v>0</v>
@@ -4324,10 +4324,10 @@
         <v>0</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>434</v>
+        <v>398</v>
       </c>
       <c r="J63" s="23" t="s">
-        <v>433</v>
+        <v>397</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4335,10 +4335,10 @@
         <v>29</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>435</v>
+        <v>399</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>436</v>
+        <v>400</v>
       </c>
       <c r="D64" s="25" t="b">
         <v>0</v>
@@ -4359,7 +4359,7 @@
         <v>30</v>
       </c>
       <c r="J64" s="23" t="s">
-        <v>393</v>
+        <v>357</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4367,10 +4367,10 @@
         <v>31</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>437</v>
+        <v>401</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>438</v>
+        <v>402</v>
       </c>
       <c r="D65" s="25" t="b">
         <v>0</v>
@@ -4391,18 +4391,18 @@
         <v>32</v>
       </c>
       <c r="J65" s="23" t="s">
-        <v>439</v>
+        <v>403</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A66" s="22" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>440</v>
+        <v>404</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>441</v>
+        <v>405</v>
       </c>
       <c r="D66" s="24" t="b">
         <v>0</v>
@@ -4420,21 +4420,21 @@
         <v>1</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>442</v>
+        <v>406</v>
       </c>
       <c r="J66" s="23" t="s">
-        <v>443</v>
+        <v>407</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A67" s="22" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>444</v>
+        <v>408</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>445</v>
+        <v>409</v>
       </c>
       <c r="D67" s="24" t="b">
         <v>0</v>
@@ -4452,21 +4452,21 @@
         <v>1</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>446</v>
+        <v>410</v>
       </c>
       <c r="J67" s="23" t="s">
-        <v>447</v>
+        <v>411</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A68" s="22" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>448</v>
+        <v>412</v>
       </c>
       <c r="D68" s="24" t="b">
         <v>1</v>
@@ -4484,21 +4484,21 @@
         <v>0</v>
       </c>
       <c r="I68" s="23" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="J68" s="23" t="s">
-        <v>449</v>
+        <v>413</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A69" s="22" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>450</v>
+        <v>414</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>452</v>
+        <v>416</v>
       </c>
       <c r="D69" s="25" t="b">
         <v>0</v>
@@ -4516,21 +4516,21 @@
         <v>0</v>
       </c>
       <c r="I69" s="23" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="J69" s="23" t="s">
-        <v>453</v>
+        <v>417</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A70" s="22" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>454</v>
+        <v>418</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>455</v>
+        <v>419</v>
       </c>
       <c r="D70" s="24" t="b">
         <v>0</v>
@@ -4548,10 +4548,10 @@
         <v>1</v>
       </c>
       <c r="I70" s="23" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="J70" s="23" t="s">
-        <v>456</v>
+        <v>420</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4559,10 +4559,10 @@
         <v>33</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>457</v>
+        <v>421</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>458</v>
+        <v>422</v>
       </c>
       <c r="D71" s="25" t="b">
         <v>0</v>
@@ -4583,18 +4583,18 @@
         <v>34</v>
       </c>
       <c r="J71" s="23" t="s">
-        <v>459</v>
+        <v>423</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="22" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>460</v>
+        <v>424</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>461</v>
+        <v>425</v>
       </c>
       <c r="D72" s="25" t="b">
         <v>0</v>
@@ -4612,21 +4612,21 @@
         <v>1</v>
       </c>
       <c r="I72" s="23" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="J72" s="23" t="s">
-        <v>459</v>
+        <v>423</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A73" s="22" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>462</v>
+        <v>426</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>463</v>
+        <v>427</v>
       </c>
       <c r="D73" s="24" t="b">
         <v>0</v>
@@ -4644,10 +4644,10 @@
         <v>1</v>
       </c>
       <c r="I73" s="23" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="J73" s="23" t="s">
-        <v>449</v>
+        <v>413</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4655,10 +4655,10 @@
         <v>35</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>464</v>
+        <v>428</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>465</v>
+        <v>429</v>
       </c>
       <c r="D74" s="24" t="b">
         <v>0</v>
@@ -4676,21 +4676,21 @@
         <v>0</v>
       </c>
       <c r="I74" s="23" t="s">
-        <v>466</v>
+        <v>430</v>
       </c>
       <c r="J74" s="24" t="s">
-        <v>467</v>
+        <v>431</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A75" s="22" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>468</v>
+        <v>432</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>469</v>
+        <v>433</v>
       </c>
       <c r="D75" s="24" t="b">
         <v>0</v>
@@ -4708,53 +4708,53 @@
         <v>0</v>
       </c>
       <c r="I75" s="23" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="J75" s="23" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A76" s="22" t="s">
         <v>36</v>
       </c>
       <c r="B76" s="23" t="s">
+        <v>438</v>
+      </c>
+      <c r="C76" s="23" t="s">
+        <v>440</v>
+      </c>
+      <c r="D76" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E76" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="F76" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G76" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H76" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I76" s="23" t="s">
+        <v>436</v>
+      </c>
+      <c r="J76" s="23" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+      <c r="A77" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="C76" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="D76" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E76" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="F76" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G76" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H76" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="I76" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="J76" s="23" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="15" x14ac:dyDescent="0.2">
-      <c r="A77" s="22" t="s">
-        <v>41</v>
-      </c>
       <c r="B77" s="23" t="s">
-        <v>42</v>
+        <v>439</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>38</v>
+        <v>440</v>
       </c>
       <c r="D77" s="25" t="b">
         <v>0</v>
@@ -4772,21 +4772,21 @@
         <v>1</v>
       </c>
       <c r="I77" s="23" t="s">
-        <v>43</v>
+        <v>437</v>
       </c>
       <c r="J77" s="23" t="s">
-        <v>44</v>
+        <v>441</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="22" t="s">
-        <v>138</v>
+        <v>122</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>139</v>
+        <v>445</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>140</v>
+        <v>443</v>
       </c>
       <c r="D78" s="25" t="b">
         <v>0</v>
@@ -4804,21 +4804,21 @@
         <v>0</v>
       </c>
       <c r="I78" s="23" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>144</v>
+        <v>444</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>145</v>
+        <v>446</v>
       </c>
       <c r="D79" s="24" t="b">
         <v>1</v>
@@ -4836,21 +4836,21 @@
         <v>0</v>
       </c>
       <c r="I79" s="23" t="s">
-        <v>146</v>
+        <v>447</v>
       </c>
       <c r="J79" s="23" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>46</v>
+        <v>449</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>47</v>
+        <v>450</v>
       </c>
       <c r="D80" s="25" t="b">
         <v>0</v>
@@ -4868,21 +4868,21 @@
         <v>0</v>
       </c>
       <c r="I80" s="23" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J80" s="23" t="s">
-        <v>49</v>
+        <v>451</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="D81" s="24" t="b">
         <v>1</v>
@@ -4900,21 +4900,21 @@
         <v>1</v>
       </c>
       <c r="I81" s="23" t="s">
-        <v>79</v>
+        <v>454</v>
       </c>
       <c r="J81" s="23" t="s">
-        <v>80</v>
+        <v>452</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
-        <v>147</v>
+        <v>125</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>149</v>
+        <v>456</v>
       </c>
       <c r="D82" s="24" t="b">
         <v>0</v>
@@ -4932,21 +4932,21 @@
         <v>1</v>
       </c>
       <c r="I82" s="23" t="s">
-        <v>150</v>
+        <v>455</v>
       </c>
       <c r="J82" s="23" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>153</v>
+        <v>128</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>154</v>
+        <v>457</v>
       </c>
       <c r="D83" s="25" t="b">
         <v>0</v>
@@ -4964,21 +4964,21 @@
         <v>0</v>
       </c>
       <c r="I83" s="23" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="J83" s="23" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" s="10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
-        <v>251</v>
+        <v>215</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>81</v>
+        <v>460</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>82</v>
+        <v>459</v>
       </c>
       <c r="D84" s="24" t="b">
         <v>1</v>
@@ -4996,21 +4996,21 @@
         <v>0</v>
       </c>
       <c r="I84" s="23" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="J84" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A85" s="22" t="s">
         <v>4</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>423</v>
+        <v>387</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>82</v>
+        <v>459</v>
       </c>
       <c r="D85" s="24" t="b">
         <v>1</v>
@@ -5028,21 +5028,21 @@
         <v>0</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="J85" s="23" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A86" s="22" t="s">
-        <v>157</v>
+        <v>130</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>158</v>
+        <v>131</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>159</v>
+        <v>463</v>
       </c>
       <c r="D86" s="25" t="b">
         <v>0</v>
@@ -5060,21 +5060,21 @@
         <v>0</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>160</v>
+        <v>462</v>
       </c>
       <c r="J86" s="23" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A87" s="22" t="s">
-        <v>162</v>
+        <v>132</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>164</v>
+        <v>466</v>
       </c>
       <c r="D87" s="24" t="b">
         <v>1</v>
@@ -5092,21 +5092,21 @@
         <v>0</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>165</v>
+        <v>465</v>
       </c>
       <c r="J87" s="23" t="s">
-        <v>166</v>
+        <v>464</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="22" t="s">
-        <v>167</v>
+        <v>134</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>168</v>
+        <v>135</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="D88" s="24" t="b">
         <v>1</v>
@@ -5124,31 +5124,43 @@
         <v>0</v>
       </c>
       <c r="I88" s="23" t="s">
-        <v>170</v>
+        <v>137</v>
       </c>
       <c r="J88" s="23" t="s">
-        <v>171</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="28" t="s">
-        <v>172</v>
+        <v>139</v>
       </c>
       <c r="B89" s="29" t="s">
-        <v>173</v>
+        <v>467</v>
       </c>
       <c r="C89" s="29" t="s">
-        <v>174</v>
-      </c>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
+        <v>468</v>
+      </c>
+      <c r="D89" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="E89" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="F89" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="G89" s="25" t="b">
+        <v>1</v>
+      </c>
+      <c r="H89" s="25" t="b">
+        <v>0</v>
+      </c>
       <c r="I89" s="29" t="s">
-        <v>175</v>
-      </c>
-      <c r="J89" s="23"/>
+        <v>469</v>
+      </c>
+      <c r="J89" s="23" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="90" spans="1:10" ht="14" x14ac:dyDescent="0.2">
       <c r="A90" s="6"/>
@@ -8084,34 +8096,34 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>178</v>
+        <v>142</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>180</v>
+        <v>144</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>181</v>
+        <v>145</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>182</v>
+        <v>146</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="E2" s="4" t="b">
         <v>1</v>
@@ -8119,16 +8131,16 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>185</v>
+        <v>149</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>187</v>
+        <v>151</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="E3" s="4" t="b">
         <v>1</v>
@@ -8136,16 +8148,16 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>189</v>
+        <v>153</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>190</v>
+        <v>154</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="E4" s="4" t="b">
         <v>1</v>
@@ -8153,16 +8165,16 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>192</v>
+        <v>156</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>193</v>
+        <v>157</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>194</v>
+        <v>158</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="E5" s="4" t="b">
         <v>1</v>
@@ -8170,16 +8182,16 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>195</v>
+        <v>159</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>196</v>
+        <v>160</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>197</v>
+        <v>161</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="E6" s="4" t="b">
         <v>1</v>
@@ -8187,16 +8199,16 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>198</v>
+        <v>162</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>199</v>
+        <v>163</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="E7" s="4" t="b">
         <v>0</v>
@@ -8204,16 +8216,16 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>204</v>
+        <v>168</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="E8" s="4" t="b">
         <v>0</v>
@@ -8221,16 +8233,16 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>205</v>
+        <v>169</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>206</v>
+        <v>170</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>201</v>
+        <v>165</v>
       </c>
       <c r="E9" s="4" t="b">
         <v>0</v>
@@ -8238,16 +8250,16 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>207</v>
+        <v>171</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="E10" s="4" t="b">
         <v>0</v>
@@ -8255,16 +8267,16 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="E11" s="4" t="b">
         <v>0</v>
@@ -8272,16 +8284,16 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>215</v>
+        <v>179</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>191</v>
+        <v>155</v>
       </c>
       <c r="E12" s="4" t="b">
         <v>0</v>
@@ -8615,27 +8627,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>176</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>141</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>179</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>217</v>
+        <v>181</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>218</v>
+        <v>182</v>
       </c>
       <c r="D2" s="4" t="b">
         <v>1</v>
@@ -8643,13 +8655,13 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
-        <v>219</v>
+        <v>183</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>220</v>
+        <v>184</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>221</v>
+        <v>185</v>
       </c>
       <c r="D3" s="4" t="b">
         <v>1</v>
@@ -8657,13 +8669,13 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>222</v>
+        <v>186</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>223</v>
+        <v>187</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>224</v>
+        <v>188</v>
       </c>
       <c r="D4" s="4" t="b">
         <v>1</v>
@@ -8671,13 +8683,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>226</v>
+        <v>190</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>227</v>
+        <v>191</v>
       </c>
       <c r="D5" s="4" t="b">
         <v>1</v>
@@ -8685,13 +8697,13 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>228</v>
+        <v>192</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>230</v>
+        <v>194</v>
       </c>
       <c r="D6" s="4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
minor spelling fixes to primitive descriptions
</commit_message>
<xml_diff>
--- a/metadata/binddata.xlsx
+++ b/metadata/binddata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ual895/Git/newdictionary/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890781FE-CCBF-2B45-9EF9-E5315FF5928D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411421A2-71ED-0A44-BDC0-9752E64698C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29440" yWindow="5440" windowWidth="27800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primitives" sheetId="1" r:id="rId1"/>
@@ -1003,24 +1003,12 @@
     <t>Reports a list of top values in a provided list.</t>
   </si>
   <si>
-    <t>Reports the largest x-coordinate of the patches in a midel.</t>
-  </si>
-  <si>
-    <t>Reports the largest y-coordinate of the patches in a midel.</t>
-  </si>
-  <si>
     <t>Reports the average of a provided list of numerical values.</t>
   </si>
   <si>
     <t>Reports true if a value is within a list or if an agent is in an agentset.</t>
   </si>
   <si>
-    <t>Reports the smallest x-coordinate of the patches in a midel.</t>
-  </si>
-  <si>
-    <t>Reports the smallest y-coordinate of the patches in a midel.</t>
-  </si>
-  <si>
     <t>Moves a turtle to set its x and y coordinates to be the same as another turtle or patch.</t>
   </si>
   <si>
@@ -1069,9 +1057,6 @@
     <t>both, boolean, true, false, combine</t>
   </si>
   <si>
-    <t>any, within, count, agentset,remaining</t>
-  </si>
-  <si>
     <t>all?, count, if, other, nobody</t>
   </si>
   <si>
@@ -1357,9 +1342,6 @@
     <t>Mimicry, Flocking, Scatter, CRISPR Ecosystem</t>
   </si>
   <si>
-    <t>count, if, if-else, n-of</t>
-  </si>
-  <si>
     <t>Fairy Circles, Small Worlds, Party, Traffic Grid Goal</t>
   </si>
   <si>
@@ -1742,6 +1724,24 @@
   </si>
   <si>
     <t>Fur, Mimicry, Ants, Heatbugs</t>
+  </si>
+  <si>
+    <t>count, if, n-of, with</t>
+  </si>
+  <si>
+    <t>Reports the largest x-coordinate of the patches in a model.</t>
+  </si>
+  <si>
+    <t>Reports the largest y-coordinate of the patches in a model.</t>
+  </si>
+  <si>
+    <t>Reports the smallest x-coordinate of the patches in a model.</t>
+  </si>
+  <si>
+    <t>Reports the smallest y-coordinate of the patches in a model.</t>
+  </si>
+  <si>
+    <t>any, within, count, agentset, remaining</t>
   </si>
 </sst>
 </file>
@@ -2279,9 +2279,9 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I84" sqref="I84"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2354,7 +2354,7 @@
         <v>195</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="D2" s="24" t="b">
         <v>0</v>
@@ -2372,10 +2372,10 @@
         <v>1</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2386,7 +2386,7 @@
         <v>196</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="D3" s="24" t="b">
         <v>0</v>
@@ -2404,10 +2404,10 @@
         <v>1</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2418,7 +2418,7 @@
         <v>197</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>246</v>
+        <v>470</v>
       </c>
       <c r="D4" s="25" t="b">
         <v>0</v>
@@ -2436,10 +2436,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2450,7 +2450,7 @@
         <v>198</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D5" s="24" t="b">
         <v>1</v>
@@ -2468,10 +2468,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2482,7 +2482,7 @@
         <v>199</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D6" s="24" t="b">
         <v>1</v>
@@ -2500,10 +2500,10 @@
         <v>0</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2514,7 +2514,7 @@
         <v>200</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D7" s="24" t="b">
         <v>0</v>
@@ -2532,10 +2532,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
@@ -2546,7 +2546,7 @@
         <v>201</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D8" s="24" t="b">
         <v>1</v>
@@ -2564,10 +2564,10 @@
         <v>0</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2578,7 +2578,7 @@
         <v>201</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D9" s="24" t="b">
         <v>1</v>
@@ -2596,10 +2596,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2610,7 +2610,7 @@
         <v>202</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D10" s="24" t="b">
         <v>1</v>
@@ -2628,10 +2628,10 @@
         <v>0</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2642,7 +2642,7 @@
         <v>203</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D11" s="24" t="b">
         <v>1</v>
@@ -2660,10 +2660,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2671,10 +2671,10 @@
         <v>44</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D12" s="24" t="b">
         <v>0</v>
@@ -2692,10 +2692,10 @@
         <v>0</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2706,7 +2706,7 @@
         <v>204</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D13" s="24" t="b">
         <v>0</v>
@@ -2724,10 +2724,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2738,7 +2738,7 @@
         <v>205</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="D14" s="25" t="b">
         <v>0</v>
@@ -2759,7 +2759,7 @@
         <v>14</v>
       </c>
       <c r="J14" s="23" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
@@ -2770,7 +2770,7 @@
         <v>206</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D15" s="24" t="b">
         <v>1</v>
@@ -2791,7 +2791,7 @@
         <v>46</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2802,7 +2802,7 @@
         <v>206</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D16" s="24" t="b">
         <v>1</v>
@@ -2823,7 +2823,7 @@
         <v>46</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -2834,7 +2834,7 @@
         <v>207</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D17" s="25" t="b">
         <v>0</v>
@@ -2852,10 +2852,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -2863,10 +2863,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D18" s="25" t="b">
         <v>0</v>
@@ -2884,10 +2884,10 @@
         <v>0</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -2895,10 +2895,10 @@
         <v>73</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D19" s="25" t="b">
         <v>0</v>
@@ -2916,10 +2916,10 @@
         <v>0</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -2930,7 +2930,7 @@
         <v>208</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D20" s="24" t="b">
         <v>1</v>
@@ -2951,7 +2951,7 @@
         <v>75</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -2959,10 +2959,10 @@
         <v>76</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D21" s="25" t="b">
         <v>0</v>
@@ -2983,7 +2983,7 @@
         <v>77</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -2991,10 +2991,10 @@
         <v>47</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="D22" s="24" t="b">
         <v>0</v>
@@ -3015,7 +3015,7 @@
         <v>48</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3026,7 +3026,7 @@
         <v>209</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D23" s="24" t="b">
         <v>0</v>
@@ -3047,7 +3047,7 @@
         <v>79</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
@@ -3058,7 +3058,7 @@
         <v>210</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D24" s="24" t="b">
         <v>0</v>
@@ -3079,7 +3079,7 @@
         <v>50</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3090,7 +3090,7 @@
         <v>210</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>353</v>
+        <v>347</v>
       </c>
       <c r="D25" s="24" t="b">
         <v>0</v>
@@ -3111,7 +3111,7 @@
         <v>50</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3119,10 +3119,10 @@
         <v>16</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D26" s="24" t="b">
         <v>1</v>
@@ -3140,10 +3140,10 @@
         <v>0</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3151,10 +3151,10 @@
         <v>80</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="D27" s="25" t="b">
         <v>0</v>
@@ -3175,7 +3175,7 @@
         <v>81</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3183,10 +3183,10 @@
         <v>82</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D28" s="24" t="b">
         <v>0</v>
@@ -3207,7 +3207,7 @@
         <v>83</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3215,10 +3215,10 @@
         <v>17</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D29" s="25" t="b">
         <v>0</v>
@@ -3236,10 +3236,10 @@
         <v>1</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3250,7 +3250,7 @@
         <v>211</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="D30" s="25" t="b">
         <v>0</v>
@@ -3268,10 +3268,10 @@
         <v>1</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="J30" s="29" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3282,7 +3282,7 @@
         <v>217</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="D31" s="25" t="b">
         <v>0</v>
@@ -3303,7 +3303,7 @@
         <v>20</v>
       </c>
       <c r="J31" s="23" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3314,7 +3314,7 @@
         <v>216</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="D32" s="25" t="b">
         <v>0</v>
@@ -3332,10 +3332,10 @@
         <v>0</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3346,7 +3346,7 @@
         <v>218</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="D33" s="24" t="b">
         <v>1</v>
@@ -3364,10 +3364,10 @@
         <v>0</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3378,7 +3378,7 @@
         <v>219</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="D34" s="25" t="b">
         <v>0</v>
@@ -3396,10 +3396,10 @@
         <v>0</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3407,10 +3407,10 @@
         <v>85</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="D35" s="24" t="b">
         <v>0</v>
@@ -3431,7 +3431,7 @@
         <v>86</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3442,7 +3442,7 @@
         <v>220</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D36" s="25" t="b">
         <v>0</v>
@@ -3460,10 +3460,10 @@
         <v>0</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3474,7 +3474,7 @@
         <v>221</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D37" s="25" t="b">
         <v>0</v>
@@ -3492,10 +3492,10 @@
         <v>0</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3506,7 +3506,7 @@
         <v>222</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D38" s="24" t="b">
         <v>0</v>
@@ -3524,10 +3524,10 @@
         <v>1</v>
       </c>
       <c r="I38" s="23" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3538,7 +3538,7 @@
         <v>223</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="D39" s="24" t="b">
         <v>0</v>
@@ -3556,10 +3556,10 @@
         <v>1</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3567,10 +3567,10 @@
         <v>87</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>224</v>
+        <v>466</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="D40" s="24" t="b">
         <v>0</v>
@@ -3591,7 +3591,7 @@
         <v>88</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3599,10 +3599,10 @@
         <v>89</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>225</v>
+        <v>467</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="D41" s="24" t="b">
         <v>0</v>
@@ -3623,7 +3623,7 @@
         <v>88</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3631,10 +3631,10 @@
         <v>92</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="D42" s="24" t="b">
         <v>0</v>
@@ -3655,7 +3655,7 @@
         <v>93</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3663,7 +3663,7 @@
         <v>94</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C43" s="23" t="s">
         <v>95</v>
@@ -3684,10 +3684,10 @@
         <v>1</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>342</v>
+        <v>465</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3695,10 +3695,10 @@
         <v>96</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>228</v>
+        <v>468</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="D44" s="24" t="b">
         <v>0</v>
@@ -3719,7 +3719,7 @@
         <v>97</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3727,10 +3727,10 @@
         <v>98</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>229</v>
+        <v>469</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="D45" s="24" t="b">
         <v>0</v>
@@ -3751,7 +3751,7 @@
         <v>97</v>
       </c>
       <c r="J45" s="30" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -3759,10 +3759,10 @@
         <v>99</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="D46" s="24" t="b">
         <v>0</v>
@@ -3783,7 +3783,7 @@
         <v>100</v>
       </c>
       <c r="J46" s="23" t="s">
-        <v>351</v>
+        <v>345</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3791,10 +3791,10 @@
         <v>51</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="D47" s="24" t="b">
         <v>0</v>
@@ -3812,10 +3812,10 @@
         <v>0</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>355</v>
+        <v>349</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3823,10 +3823,10 @@
         <v>101</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>356</v>
+        <v>350</v>
       </c>
       <c r="D48" s="25" t="b">
         <v>0</v>
@@ -3847,7 +3847,7 @@
         <v>102</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3855,10 +3855,10 @@
         <v>24</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>358</v>
+        <v>352</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>359</v>
+        <v>353</v>
       </c>
       <c r="D49" s="25" t="b">
         <v>0</v>
@@ -3879,7 +3879,7 @@
         <v>25</v>
       </c>
       <c r="J49" s="23" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3887,10 +3887,10 @@
         <v>52</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D50" s="24" t="b">
         <v>0</v>
@@ -3908,10 +3908,10 @@
         <v>0</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -3919,10 +3919,10 @@
         <v>53</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="D51" s="24" t="b">
         <v>0</v>
@@ -3940,10 +3940,10 @@
         <v>0</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="J51" s="30" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3951,10 +3951,10 @@
         <v>103</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="D52" s="25" t="b">
         <v>0</v>
@@ -3972,10 +3972,10 @@
         <v>1</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3983,10 +3983,10 @@
         <v>26</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="D53" s="25" t="b">
         <v>0</v>
@@ -4007,7 +4007,7 @@
         <v>27</v>
       </c>
       <c r="J53" s="23" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4015,10 +4015,10 @@
         <v>104</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="D54" s="25" t="b">
         <v>0</v>
@@ -4036,10 +4036,10 @@
         <v>1</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="J54" s="23" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4047,10 +4047,10 @@
         <v>28</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="D55" s="25" t="b">
         <v>0</v>
@@ -4068,10 +4068,10 @@
         <v>1</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4079,10 +4079,10 @@
         <v>54</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="D56" s="25" t="b">
         <v>0</v>
@@ -4100,10 +4100,10 @@
         <v>0</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="J56" s="23" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4111,10 +4111,10 @@
         <v>105</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D57" s="24" t="b">
         <v>1</v>
@@ -4135,7 +4135,7 @@
         <v>106</v>
       </c>
       <c r="J57" s="23" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4143,10 +4143,10 @@
         <v>55</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="D58" s="24" t="b">
         <v>0</v>
@@ -4164,10 +4164,10 @@
         <v>0</v>
       </c>
       <c r="I58" s="23" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="J58" s="23" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4175,10 +4175,10 @@
         <v>5</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D59" s="24" t="b">
         <v>1</v>
@@ -4199,7 +4199,7 @@
         <v>110</v>
       </c>
       <c r="J59" s="23" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4207,7 +4207,7 @@
         <v>107</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C60" s="23" t="s">
         <v>108</v>
@@ -4231,7 +4231,7 @@
         <v>109</v>
       </c>
       <c r="J60" s="23" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4239,10 +4239,10 @@
         <v>56</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D61" s="25" t="b">
         <v>0</v>
@@ -4263,7 +4263,7 @@
         <v>57</v>
       </c>
       <c r="J61" s="23" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4271,10 +4271,10 @@
         <v>111</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D62" s="25" t="b">
         <v>0</v>
@@ -4292,10 +4292,10 @@
         <v>0</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>396</v>
+        <v>390</v>
       </c>
       <c r="J62" s="23" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4306,7 +4306,7 @@
         <v>113</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="D63" s="25" t="b">
         <v>0</v>
@@ -4324,10 +4324,10 @@
         <v>0</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>398</v>
+        <v>392</v>
       </c>
       <c r="J63" s="23" t="s">
-        <v>397</v>
+        <v>391</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4335,10 +4335,10 @@
         <v>29</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>399</v>
+        <v>393</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>400</v>
+        <v>394</v>
       </c>
       <c r="D64" s="25" t="b">
         <v>0</v>
@@ -4359,7 +4359,7 @@
         <v>30</v>
       </c>
       <c r="J64" s="23" t="s">
-        <v>357</v>
+        <v>351</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4367,10 +4367,10 @@
         <v>31</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>401</v>
+        <v>395</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>402</v>
+        <v>396</v>
       </c>
       <c r="D65" s="25" t="b">
         <v>0</v>
@@ -4391,7 +4391,7 @@
         <v>32</v>
       </c>
       <c r="J65" s="23" t="s">
-        <v>403</v>
+        <v>397</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4399,10 +4399,10 @@
         <v>114</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>405</v>
+        <v>399</v>
       </c>
       <c r="D66" s="24" t="b">
         <v>0</v>
@@ -4420,10 +4420,10 @@
         <v>1</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>406</v>
+        <v>400</v>
       </c>
       <c r="J66" s="23" t="s">
-        <v>407</v>
+        <v>401</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4431,10 +4431,10 @@
         <v>58</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>408</v>
+        <v>402</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>409</v>
+        <v>403</v>
       </c>
       <c r="D67" s="24" t="b">
         <v>0</v>
@@ -4452,10 +4452,10 @@
         <v>1</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>410</v>
+        <v>404</v>
       </c>
       <c r="J67" s="23" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4466,7 +4466,7 @@
         <v>116</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>412</v>
+        <v>406</v>
       </c>
       <c r="D68" s="24" t="b">
         <v>1</v>
@@ -4487,7 +4487,7 @@
         <v>117</v>
       </c>
       <c r="J68" s="23" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4495,10 +4495,10 @@
         <v>118</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>414</v>
+        <v>408</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>416</v>
+        <v>410</v>
       </c>
       <c r="D69" s="25" t="b">
         <v>0</v>
@@ -4519,7 +4519,7 @@
         <v>119</v>
       </c>
       <c r="J69" s="23" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4527,10 +4527,10 @@
         <v>59</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>418</v>
+        <v>412</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>419</v>
+        <v>413</v>
       </c>
       <c r="D70" s="24" t="b">
         <v>0</v>
@@ -4551,7 +4551,7 @@
         <v>60</v>
       </c>
       <c r="J70" s="23" t="s">
-        <v>420</v>
+        <v>414</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4559,10 +4559,10 @@
         <v>33</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>421</v>
+        <v>415</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>422</v>
+        <v>416</v>
       </c>
       <c r="D71" s="25" t="b">
         <v>0</v>
@@ -4583,7 +4583,7 @@
         <v>34</v>
       </c>
       <c r="J71" s="23" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4591,10 +4591,10 @@
         <v>61</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>424</v>
+        <v>418</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>425</v>
+        <v>419</v>
       </c>
       <c r="D72" s="25" t="b">
         <v>0</v>
@@ -4615,7 +4615,7 @@
         <v>62</v>
       </c>
       <c r="J72" s="23" t="s">
-        <v>423</v>
+        <v>417</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4623,10 +4623,10 @@
         <v>120</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>426</v>
+        <v>420</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="D73" s="24" t="b">
         <v>0</v>
@@ -4647,7 +4647,7 @@
         <v>121</v>
       </c>
       <c r="J73" s="23" t="s">
-        <v>413</v>
+        <v>407</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4655,10 +4655,10 @@
         <v>35</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>428</v>
+        <v>422</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>429</v>
+        <v>423</v>
       </c>
       <c r="D74" s="24" t="b">
         <v>0</v>
@@ -4676,10 +4676,10 @@
         <v>0</v>
       </c>
       <c r="I74" s="23" t="s">
-        <v>430</v>
+        <v>424</v>
       </c>
       <c r="J74" s="24" t="s">
-        <v>431</v>
+        <v>425</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4687,10 +4687,10 @@
         <v>63</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>432</v>
+        <v>426</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="D75" s="24" t="b">
         <v>0</v>
@@ -4711,7 +4711,7 @@
         <v>64</v>
       </c>
       <c r="J75" s="23" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4719,10 +4719,10 @@
         <v>36</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>438</v>
+        <v>432</v>
       </c>
       <c r="C76" s="23" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D76" s="25" t="b">
         <v>0</v>
@@ -4740,10 +4740,10 @@
         <v>1</v>
       </c>
       <c r="I76" s="23" t="s">
-        <v>436</v>
+        <v>430</v>
       </c>
       <c r="J76" s="23" t="s">
-        <v>435</v>
+        <v>429</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4751,10 +4751,10 @@
         <v>37</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>439</v>
+        <v>433</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>440</v>
+        <v>434</v>
       </c>
       <c r="D77" s="25" t="b">
         <v>0</v>
@@ -4772,10 +4772,10 @@
         <v>1</v>
       </c>
       <c r="I77" s="23" t="s">
-        <v>437</v>
+        <v>431</v>
       </c>
       <c r="J77" s="23" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4783,10 +4783,10 @@
         <v>122</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>445</v>
+        <v>439</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>443</v>
+        <v>437</v>
       </c>
       <c r="D78" s="25" t="b">
         <v>0</v>
@@ -4807,7 +4807,7 @@
         <v>123</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4815,10 +4815,10 @@
         <v>124</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>446</v>
+        <v>440</v>
       </c>
       <c r="D79" s="24" t="b">
         <v>1</v>
@@ -4836,10 +4836,10 @@
         <v>0</v>
       </c>
       <c r="I79" s="23" t="s">
-        <v>447</v>
+        <v>441</v>
       </c>
       <c r="J79" s="23" t="s">
-        <v>448</v>
+        <v>442</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="43" x14ac:dyDescent="0.2">
@@ -4847,10 +4847,10 @@
         <v>38</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>449</v>
+        <v>443</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>450</v>
+        <v>444</v>
       </c>
       <c r="D80" s="25" t="b">
         <v>0</v>
@@ -4871,7 +4871,7 @@
         <v>39</v>
       </c>
       <c r="J80" s="23" t="s">
-        <v>451</v>
+        <v>445</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4900,10 +4900,10 @@
         <v>1</v>
       </c>
       <c r="I81" s="23" t="s">
-        <v>454</v>
+        <v>448</v>
       </c>
       <c r="J81" s="23" t="s">
-        <v>452</v>
+        <v>446</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4914,7 +4914,7 @@
         <v>126</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>456</v>
+        <v>450</v>
       </c>
       <c r="D82" s="24" t="b">
         <v>0</v>
@@ -4932,10 +4932,10 @@
         <v>1</v>
       </c>
       <c r="I82" s="23" t="s">
-        <v>455</v>
+        <v>449</v>
       </c>
       <c r="J82" s="23" t="s">
-        <v>453</v>
+        <v>447</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4946,7 +4946,7 @@
         <v>128</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>457</v>
+        <v>451</v>
       </c>
       <c r="D83" s="25" t="b">
         <v>0</v>
@@ -4967,7 +4967,7 @@
         <v>129</v>
       </c>
       <c r="J83" s="23" t="s">
-        <v>458</v>
+        <v>452</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
@@ -4975,10 +4975,10 @@
         <v>215</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>460</v>
+        <v>454</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="D84" s="24" t="b">
         <v>1</v>
@@ -4999,7 +4999,7 @@
         <v>68</v>
       </c>
       <c r="J84" s="23" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -5007,10 +5007,10 @@
         <v>4</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>459</v>
+        <v>453</v>
       </c>
       <c r="D85" s="24" t="b">
         <v>1</v>
@@ -5031,7 +5031,7 @@
         <v>68</v>
       </c>
       <c r="J85" s="23" t="s">
-        <v>411</v>
+        <v>405</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -5042,7 +5042,7 @@
         <v>131</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>463</v>
+        <v>457</v>
       </c>
       <c r="D86" s="25" t="b">
         <v>0</v>
@@ -5060,10 +5060,10 @@
         <v>0</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>462</v>
+        <v>456</v>
       </c>
       <c r="J86" s="23" t="s">
-        <v>461</v>
+        <v>455</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -5074,7 +5074,7 @@
         <v>133</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>466</v>
+        <v>460</v>
       </c>
       <c r="D87" s="24" t="b">
         <v>1</v>
@@ -5092,10 +5092,10 @@
         <v>0</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>465</v>
+        <v>459</v>
       </c>
       <c r="J87" s="23" t="s">
-        <v>464</v>
+        <v>458</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -5135,10 +5135,10 @@
         <v>139</v>
       </c>
       <c r="B89" s="29" t="s">
-        <v>467</v>
+        <v>461</v>
       </c>
       <c r="C89" s="29" t="s">
-        <v>468</v>
+        <v>462</v>
       </c>
       <c r="D89" s="24" t="b">
         <v>1</v>
@@ -5156,10 +5156,10 @@
         <v>0</v>
       </c>
       <c r="I89" s="29" t="s">
-        <v>469</v>
+        <v>463</v>
       </c>
       <c r="J89" s="23" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="14" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
fixed a lot of metadata issues. almost error free now
</commit_message>
<xml_diff>
--- a/metadata/binddata.xlsx
+++ b/metadata/binddata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ual895/Git/newdictionary/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411421A2-71ED-0A44-BDC0-9752E64698C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E5F107F-2ED1-4C4F-8F10-82CA5FFAA830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="500" windowWidth="27820" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,9 +349,6 @@
     <t>and</t>
   </si>
   <si>
-    <t>any?</t>
-  </si>
-  <si>
     <t>breed</t>
   </si>
   <si>
@@ -391,9 +388,6 @@
     <t>n-of</t>
   </si>
   <si>
-    <t>one-of, count, any?, all?</t>
-  </si>
-  <si>
     <t>of</t>
   </si>
   <si>
@@ -439,9 +433,6 @@
     <t>ask</t>
   </si>
   <si>
-    <t>clear-all</t>
-  </si>
-  <si>
     <t>clear-patches</t>
   </si>
   <si>
@@ -454,21 +445,12 @@
     <t>create-turtles</t>
   </si>
   <si>
-    <t>hatch, sprout, ask, turtles-own, breeds</t>
-  </si>
-  <si>
     <t>facexy</t>
   </si>
   <si>
-    <t>face, setxy, heading, towards</t>
-  </si>
-  <si>
     <t>forward</t>
   </si>
   <si>
-    <t>right, heading, turtles, move-to</t>
-  </si>
-  <si>
     <t>move-to</t>
   </si>
   <si>
@@ -523,9 +505,6 @@
     <t>ask, turtles-own, patches, links</t>
   </si>
   <si>
-    <t>all?</t>
-  </si>
-  <si>
     <t>ceiling</t>
   </si>
   <si>
@@ -547,9 +526,6 @@
     <t>face</t>
   </si>
   <si>
-    <t>towards, facexy, heading, right</t>
-  </si>
-  <si>
     <t>floor</t>
   </si>
   <si>
@@ -565,9 +541,6 @@
     <t>if</t>
   </si>
   <si>
-    <t>ifelse, ifelse-value, any?, all?</t>
-  </si>
-  <si>
     <t>left</t>
   </si>
   <si>
@@ -616,9 +589,6 @@
     <t>mod</t>
   </si>
   <si>
-    <t>mean, count, if, any?</t>
-  </si>
-  <si>
     <t>myself</t>
   </si>
   <si>
@@ -667,15 +637,9 @@
     <t>Sets the tick counter to 0.</t>
   </si>
   <si>
-    <t>tick, to, ask, clear-all</t>
-  </si>
-  <si>
     <t>right</t>
   </si>
   <si>
-    <t>left, heading, towards, face</t>
-  </si>
-  <si>
     <t>set</t>
   </si>
   <si>
@@ -700,18 +664,12 @@
     <t>towards</t>
   </si>
   <si>
-    <t>Reports the angle of the caller towards an agent.</t>
-  </si>
-  <si>
     <t>face, right, left, heading</t>
   </si>
   <si>
     <t>turtles-here</t>
   </si>
   <si>
-    <t>Reports the agentset of all the turtles on a caller's patch.</t>
-  </si>
-  <si>
     <t>turtles-own</t>
   </si>
   <si>
@@ -725,12 +683,6 @@
   </si>
   <si>
     <t>loop</t>
-  </si>
-  <si>
-    <t>if, if-else, repeat, tick</t>
-  </si>
-  <si>
-    <t>Moths, Traffic Basic, Shepherds</t>
   </si>
   <si>
     <t>with</t>
@@ -916,15 +868,9 @@
     <t>NetLogo's Models Library is an invaluable resource. Learn how to access it.</t>
   </si>
   <si>
-    <t>Checks if a reporter is true for all agents in an agentset.</t>
-  </si>
-  <si>
     <t>Checks if both provided conditions are true.</t>
   </si>
   <si>
-    <t>Checks if there are any agents in an agentset.</t>
-  </si>
-  <si>
     <t>Asks agents do things.</t>
   </si>
   <si>
@@ -934,6 +880,738 @@
     <t>Rounds a number up to the nearest integer.</t>
   </si>
   <si>
+    <t>Counts the number of agents in an agentset.</t>
+  </si>
+  <si>
+    <t>Creates links with every agent in an agentset.</t>
+  </si>
+  <si>
+    <t>Creates turtles with random colors and headings at the center of the world.</t>
+  </si>
+  <si>
+    <t>Removes a turtle or link from the world.</t>
+  </si>
+  <si>
+    <t>Concludes a procedure.</t>
+  </si>
+  <si>
+    <t>Rounds a number down to the nearest integer.</t>
+  </si>
+  <si>
+    <t>Picks a value based on a provided list of condition-value pairs.</t>
+  </si>
+  <si>
+    <t>fd</t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>crt</t>
+  </si>
+  <si>
+    <t>turtle</t>
+  </si>
+  <si>
+    <t>Reports members of an agentset within a certain radius of an agent.</t>
+  </si>
+  <si>
+    <t>Reports members of an agentset within a "cone-of-vision" of an agent.</t>
+  </si>
+  <si>
+    <t>Places turtles in a circle circle around the center of the world.</t>
+  </si>
+  <si>
+    <t>Turns a turtle certain amount of degrees to the left.</t>
+  </si>
+  <si>
+    <t>Reports the highest value in a provided list.</t>
+  </si>
+  <si>
+    <t>Reports a list of top values in a provided list.</t>
+  </si>
+  <si>
+    <t>Reports the average of a provided list of numerical values.</t>
+  </si>
+  <si>
+    <t>Reports true if a value is within a list or if an agent is in an agentset.</t>
+  </si>
+  <si>
+    <t>Moves a turtle to set its x and y coordinates to be the same as another turtle or patch.</t>
+  </si>
+  <si>
+    <t>Reports the original turtle that asked another turtle to follow some rules.</t>
+  </si>
+  <si>
+    <t>Reports an agentset containing the eight neighboring patches.</t>
+  </si>
+  <si>
+    <t>Reports an agentset containing the four neighboring patches in cardinal directions (north, west, south, east).</t>
+  </si>
+  <si>
+    <t>A special value that helps checking if an agent exists or not.</t>
+  </si>
+  <si>
+    <t>Reports the value of an agent-owned variable.</t>
+  </si>
+  <si>
+    <t>Checks if either of two provided conditions is true.</t>
+  </si>
+  <si>
+    <t>Reports an agentset which is the same as the input agentset but omits the agent that used this primitive.</t>
+  </si>
+  <si>
+    <t>Reports a specific patch at the provided (x,y) conditions.</t>
+  </si>
+  <si>
+    <t>Reports the single patch that is the given distance “ahead” of this turtle</t>
+  </si>
+  <si>
+    <t>Autumn, Shepherds, Scatter, Party</t>
+  </si>
+  <si>
+    <t>both, boolean, true, false, combine</t>
+  </si>
+  <si>
+    <t>Anisogamy, Fur, Mammoths, Fireworks</t>
+  </si>
+  <si>
+    <t>Ants, Mimicry, Moths, Tumor</t>
+  </si>
+  <si>
+    <t>do, commands, rules, behavior</t>
+  </si>
+  <si>
+    <t>kind, type, subset, custom</t>
+  </si>
+  <si>
+    <t>Bacterial Infection, Disease Solo, Rabbit Grass Weeds, Wolf Sheep Predation</t>
+  </si>
+  <si>
+    <t>floor, round, mean, count</t>
+  </si>
+  <si>
+    <t>GasLab Circular Particles, Traffic 2 Lanes, Chaos in a Box, Decay</t>
+  </si>
+  <si>
+    <t>Flocking, Fur, Daisyworld, Wolf Sheep Predation, Follower</t>
+  </si>
+  <si>
+    <t>clear, erase, remove, delete, clean, new, fresh, refresh, reset, restart, reboot, recreate</t>
+  </si>
+  <si>
+    <t>Disease Solo, Turbulence, Simple Kinetics 3, Simple Birth Rates</t>
+  </si>
+  <si>
+    <t>Sunflower, Mammoths, Bacterial Infection, Tumor</t>
+  </si>
+  <si>
+    <t>color, pencil, change, turtle, link, look, style, design, visual, hue, rgb, hex</t>
+  </si>
+  <si>
+    <t>Mimicry, Peppered Moths, Virus, Plant Growth</t>
+  </si>
+  <si>
+    <t>Team Assembly, CRISPR Bacterium, Membrane Formation, Virus on a Network</t>
+  </si>
+  <si>
+    <t>make, more, turtle, new, agent</t>
+  </si>
+  <si>
+    <t>create, make, more, turtle, new, agent</t>
+  </si>
+  <si>
+    <t>Sunflower, Wolf Sheep Predation, Virus, Plant Growth</t>
+  </si>
+  <si>
+    <t>Wolf Sheep Predation, Virus, Tumor, Bug Hunt Camouflage</t>
+  </si>
+  <si>
+    <t>turtles, links, patches, create-turtles</t>
+  </si>
+  <si>
+    <t>remove, end, kill, erase, death, disappear, eliminate, discard</t>
+  </si>
+  <si>
+    <t>Spreads a patch characteristic to its neighbors.</t>
+  </si>
+  <si>
+    <t>spread, share, disperse, radiate, propagate, broadcast</t>
+  </si>
+  <si>
+    <t>Ants, Slime, Heatbugs, Honeycomb</t>
+  </si>
+  <si>
+    <t>Flocking Vee Formations, Fur, BeeSmart Hive Finding, Autumn</t>
+  </si>
+  <si>
+    <t>facexy, min-pxcor, patch-ahead, setxy</t>
+  </si>
+  <si>
+    <t>length, far, measure, range, gap, separation, space</t>
+  </si>
+  <si>
+    <t>Reports the distance from one turtle/patch agent to another.</t>
+  </si>
+  <si>
+    <t>finish, complete, close, finalize, wrap, terminate, define</t>
+  </si>
+  <si>
+    <t>Rock Paper Scissors, El Farol, Paths, Traffic Grid</t>
+  </si>
+  <si>
+    <t>turn, spin, look, confront, watch, glare, stare, direction, angle</t>
+  </si>
+  <si>
+    <t>Changes a turtle's heading towards another turtle or patch.</t>
+  </si>
+  <si>
+    <t>Changes a turtle's heading towards a specific point (x, y) in the world.</t>
+  </si>
+  <si>
+    <t>Ant Lines, Scatter, Bidding Market, Thermostat</t>
+  </si>
+  <si>
+    <t>round, up, integer, decimal, floating, math, calculate</t>
+  </si>
+  <si>
+    <t>Bidding Market, Vector Fields, CRISPR Ecosystem, Wolf Sheep Predation</t>
+  </si>
+  <si>
+    <t>variable, scope, universal, constant</t>
+  </si>
+  <si>
+    <t>turtles-own, patches-own, set, let</t>
+  </si>
+  <si>
+    <t>Shepherds, HIV, Giant Component, Fruit Wars</t>
+  </si>
+  <si>
+    <t>Chaos in a Box, Reactor Top Down, Voronoi, Galton Box</t>
+  </si>
+  <si>
+    <t>birth, new, create, conceive, spawn, generate, make, parent</t>
+  </si>
+  <si>
+    <t>Carries out a provided set of rules (code) if a given condition is true. Does nothing if a given condition is false.</t>
+  </si>
+  <si>
+    <t>Carries out one set of rules if a given condition is true, and another set of rules if a given condition is false.</t>
+  </si>
+  <si>
+    <t>condition, true, false, branch</t>
+  </si>
+  <si>
+    <t>condition, true, false, branch, otherwise</t>
+  </si>
+  <si>
+    <t>if, ifelse-value, or, and</t>
+  </si>
+  <si>
+    <t>switch, case, condition, otherwise</t>
+  </si>
+  <si>
+    <t>Echo, Virus, Sunflower Emergent, DLA Alternate</t>
+  </si>
+  <si>
+    <t>Flocking Vee Formations, BeeSmart Hive Finding, Bug Hunt Speeds, Flocking</t>
+  </si>
+  <si>
+    <t>around, near, circle, detect, see, vision</t>
+  </si>
+  <si>
+    <t>see, vision, detect, near</t>
+  </si>
+  <si>
+    <t>in-cone, other, neighbors, with</t>
+  </si>
+  <si>
+    <t>GasLab Circular Particles, Paths, Fruit Wars, Fairy Circles</t>
+  </si>
+  <si>
+    <t>formation, arrangement, ring, link</t>
+  </si>
+  <si>
+    <t>right, set, face, forward</t>
+  </si>
+  <si>
+    <t>Mammoths, Tumor, Flocking, Slime</t>
+  </si>
+  <si>
+    <t>Creates a local variable that only exists within just one procedure or a statement surrended with brackets (`[  ]`).</t>
+  </si>
+  <si>
+    <t>variable, local, declare, value, constant, temporary</t>
+  </si>
+  <si>
+    <t>Disease Solo, Sand, Lennard-Jones, Boiling</t>
+  </si>
+  <si>
+    <t>link-neighbors, turtles, patches, create-links-with</t>
+  </si>
+  <si>
+    <t>social, connect, network, web, complex, relation</t>
+  </si>
+  <si>
+    <t>connect, network, web, complex, relation, social</t>
+  </si>
+  <si>
+    <t>Simple Economy, Simple Viral Marketing</t>
+  </si>
+  <si>
+    <t>patch, coordinate, x, axis, world, view, west</t>
+  </si>
+  <si>
+    <t>patch, coordinate, y, axis, world, view, north</t>
+  </si>
+  <si>
+    <t>average, list, array, median, medium, middle</t>
+  </si>
+  <si>
+    <t>Mimicry, Flocking, Scatter, CRISPR Ecosystem</t>
+  </si>
+  <si>
+    <t>big, high, largest, most, top</t>
+  </si>
+  <si>
+    <t>patch, coordinate, x, axis, world, view, east</t>
+  </si>
+  <si>
+    <t>patch, coordinate, x, axis, world, view, south</t>
+  </si>
+  <si>
+    <t>Fire, Tumor, Blood Sugar Regulation, Ant Lines</t>
+  </si>
+  <si>
+    <t>Autumn, Fireworks, Galton Box, Rugby</t>
+  </si>
+  <si>
+    <t>Performs the modulo operation; reports the remainder from the division of the first number by the second number.</t>
+  </si>
+  <si>
+    <t>remainder, divide, math, calculate, arithmetic</t>
+  </si>
+  <si>
+    <t>Sunflower, Flocking Vee Formations, Voronoi, Fruit Wars</t>
+  </si>
+  <si>
+    <t>jump, travel, relocate, shift, transport, hop</t>
+  </si>
+  <si>
+    <t>move, motion, straight, go, around, position, location, step, walk, jog</t>
+  </si>
+  <si>
+    <t>Sunflower Biomorphs, Mammoths, Autumn, Fairy Circles</t>
+  </si>
+  <si>
+    <t>Reports "n" randomly picked agents from an agentset or items from a list.</t>
+  </si>
+  <si>
+    <t>subset, random, batch, portion, fragment</t>
+  </si>
+  <si>
+    <t>Virus, Heatbugs, Voronoi, Virus on a Network</t>
+  </si>
+  <si>
+    <t>surrounding, nearby, around, directions, next, border, adjoin, touch</t>
+  </si>
+  <si>
+    <t>neighbors4, patch-ahead, turtles-here, patches</t>
+  </si>
+  <si>
+    <t>Fur, DLA, Segregation, Daisyworld</t>
+  </si>
+  <si>
+    <t>neighbors, patch-ahead, turtles-here, patches</t>
+  </si>
+  <si>
+    <t>Fire, Life, Sandpile, Altruism</t>
+  </si>
+  <si>
+    <t>none, empty, dead, exist, nothing</t>
+  </si>
+  <si>
+    <t>Tumor, Heatbugs, Shepherds, HIV</t>
+  </si>
+  <si>
+    <t>variable, characteristic, property, feature</t>
+  </si>
+  <si>
+    <t>Urban Suite - Recycling, Paths, Slime, Language Change</t>
+  </si>
+  <si>
+    <t>Reports one randomly picked member from a provided agentset or list.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pick, select, draw, lottery </t>
+  </si>
+  <si>
+    <t>n-of, random, max-n-of, let</t>
+  </si>
+  <si>
+    <t>Mammoths, Ants, Shepherds, Fairy Circles</t>
+  </si>
+  <si>
+    <t>either, boolean, true, false, condition, compare</t>
+  </si>
+  <si>
+    <t>Lennard-Jones, GasLab Atmosphere, Bidding Market, Wealth Distribution</t>
+  </si>
+  <si>
+    <t>omit, exclude</t>
+  </si>
+  <si>
+    <t>Virus, Flocking, Scatter, Fruit Wars</t>
+  </si>
+  <si>
+    <t>square, background, world</t>
+  </si>
+  <si>
+    <t>Ant Lines, Autumn, SmoothLife, Rumor Mill</t>
+  </si>
+  <si>
+    <t>before, see, detect, lead, onward</t>
+  </si>
+  <si>
+    <t>neighbors, in-radius, in-cone, nobody</t>
+  </si>
+  <si>
+    <t>Mammoths, Slime, Climate Change, Traffic Intersection</t>
+  </si>
+  <si>
+    <t>Defines custom characteristics (variables) for patches. Each custom characteristic can have a different value for each patch.</t>
+  </si>
+  <si>
+    <t>Reports a patch's color and changes a patch's color when used with the set primitive.</t>
+  </si>
+  <si>
+    <t>patch, square, world, background, paint</t>
+  </si>
+  <si>
+    <t>Starts tracing the movement of the turtle on patches.</t>
+  </si>
+  <si>
+    <t>trace, draw, mark, paint, engrave, sketch</t>
+  </si>
+  <si>
+    <t>Turtles Circling, Bidding Market, GasLab Single Collision, Pendulum</t>
+  </si>
+  <si>
+    <t>Reports a random whole number between 0 and a specified number.</t>
+  </si>
+  <si>
+    <t>probability, chance, lottery, luck, toss, pick</t>
+  </si>
+  <si>
+    <t>Reports a random number with decimal points between 0 and a specified number.</t>
+  </si>
+  <si>
+    <t>decimal, floating, probability, chance, lottery, luck, toss, pick</t>
+  </si>
+  <si>
+    <t>Fire, Climate Change, Galton Box, Daisyworld</t>
+  </si>
+  <si>
+    <t>Reports a random number with decimal points that is picked from over a normal distribution with a specified mean and standard deviation.</t>
+  </si>
+  <si>
+    <t>distribution, bell, curve, chance, probability, lottery, luck, toss, pick</t>
+  </si>
+  <si>
+    <t>random, random-float, mean, set</t>
+  </si>
+  <si>
+    <t>Performs a provided set of rules (commands) repeatedly for a specified number of times.</t>
+  </si>
+  <si>
+    <t>repetition, again, multiple, loop, for, execute</t>
+  </si>
+  <si>
+    <t>ask, to, end, while</t>
+  </si>
+  <si>
+    <t>Disease Solo, Flocking Vee Formations, Peppered Moths, Ant Lines</t>
+  </si>
+  <si>
+    <t>counter, time, restart, clock, watch</t>
+  </si>
+  <si>
+    <t>Wolf Sheep Predation, Fire, Autumn, Climate Change</t>
+  </si>
+  <si>
+    <t>Changes a turtle's heading a certain amount of degrees to the right.</t>
+  </si>
+  <si>
+    <t>turn, angle, direction, orientation, twist, rotate</t>
+  </si>
+  <si>
+    <t>turn, spin, rotate, angle, direction, orientation</t>
+  </si>
+  <si>
+    <t>Reports the integer that is nearest to a specified value.</t>
+  </si>
+  <si>
+    <t>decimal, floating, near, approximate, roughly</t>
+  </si>
+  <si>
+    <t>shade, legend, tint, paint, tone, saturation, gradient</t>
+  </si>
+  <si>
+    <t>Moths, Ants, Honeycomb, Autumn</t>
+  </si>
+  <si>
+    <t>comment, note</t>
+  </si>
+  <si>
+    <t>Changes the value of a variable (global, local, or agent-owned).</t>
+  </si>
+  <si>
+    <t>variable, value, change, modify, alter</t>
+  </si>
+  <si>
+    <t>Moves a turtle to the exact location defined by the provided x and y coordinates.</t>
+  </si>
+  <si>
+    <t>position, coordinate, location, move, jump, transport</t>
+  </si>
+  <si>
+    <t>move-to, min-pxcor, max-pycor, neighbors</t>
+  </si>
+  <si>
+    <t>Vision Evolution, Tumor, Virus, Flocking</t>
+  </si>
+  <si>
+    <t>Reports a turtles or link's shape and changes a turtle's or link's shape when used with the set primitive.</t>
+  </si>
+  <si>
+    <t>look, design, style, outline, image, bitmap, vector, picture, icon, appearance, figure, photo</t>
+  </si>
+  <si>
+    <t>Urban Suite - Pollution, Traffic Intersection, Mimicry, Ant Lines</t>
+  </si>
+  <si>
+    <t>sort-on, count, mean, ask</t>
+  </si>
+  <si>
+    <t>sort-by, count, mean, ask</t>
+  </si>
+  <si>
+    <t>Reports a sorted version of a provided list based on a user-defined comparison.</t>
+  </si>
+  <si>
+    <t>Reports a sorted version of a provided agentset based on a user-defined comparison.</t>
+  </si>
+  <si>
+    <t>list, array, order, arrange, sift, cull, assort</t>
+  </si>
+  <si>
+    <t>Birthdays, Dice, DNA Protein Synthesis, Rnd Example</t>
+  </si>
+  <si>
+    <t>Daisyworld, Ant Lines, Heatbugs, Fairy Circles</t>
+  </si>
+  <si>
+    <t>create, birth, new, turtle, grow, germinate, spring, vegetate, root</t>
+  </si>
+  <si>
+    <t>Advances the tick counter by 1.</t>
+  </si>
+  <si>
+    <t>Creates new turtles at the center of a patch.</t>
+  </si>
+  <si>
+    <t>time, counter, clock, watch</t>
+  </si>
+  <si>
+    <t>Flocking, BeeSmart Hive Finding, Slime, Shepherds</t>
+  </si>
+  <si>
+    <t>Turns a link between two turtles into a rigid connection so that the movement of one turtle impacts the movement of the other.</t>
+  </si>
+  <si>
+    <t>link, connection, attachment, lock, hook, anchor</t>
+  </si>
+  <si>
+    <t>Vision Evolution, DNA Replication Fork, Bug Hunt Environmental Changes, Connected Chemistry 8 Gas Particle Sandbox</t>
+  </si>
+  <si>
+    <t>Wolf Sheep Predation, Fire, Ants, Segregation</t>
+  </si>
+  <si>
+    <t>Mimicry, Moths, Rock Paper Scissors, HIV</t>
+  </si>
+  <si>
+    <t>to-report, end, ask, create-turtles</t>
+  </si>
+  <si>
+    <t>to, end, ask, if</t>
+  </si>
+  <si>
+    <t>procedure, function, return, calculate, transform, input, output</t>
+  </si>
+  <si>
+    <t>turn, angle, face, direction, twist, spin</t>
+  </si>
+  <si>
+    <t>Chaos in a Box, Bug Hunt Coevolution, GenEvo 1 Genetic Switch, Traffic 2 Lanes</t>
+  </si>
+  <si>
+    <t>shape, triangle, mobile, agent, tortoise, animal, person, people, object, thing</t>
+  </si>
+  <si>
+    <t>Reports a specific turtle that has the provided who number.</t>
+  </si>
+  <si>
+    <t>El Farol, Party, Segregation, Chemical Equilibrium</t>
+  </si>
+  <si>
+    <t>neighbors, patches, other, in-radius</t>
+  </si>
+  <si>
+    <t>touch, contact, near, communicate, rub, tangent, tap, collide, notice, recognize, sense</t>
+  </si>
+  <si>
+    <t>Disease Solo, Flocking Vee Formations, Tumor, Wolf Sheep Predation</t>
+  </si>
+  <si>
+    <t>variable, declare, characteristic, property, attribute, trait, quality, phenotype</t>
+  </si>
+  <si>
+    <t>Reports a subset of the original agentset that only contains the agents with specified characteristics.</t>
+  </si>
+  <si>
+    <t>specific, agentset, query, narrow, subset, reduce, fragment, select</t>
+  </si>
+  <si>
+    <t>if, of, turtles-own, patches-own</t>
+  </si>
+  <si>
+    <t>Fur, Mimicry, Ants, Heatbugs</t>
+  </si>
+  <si>
+    <t>count, if, n-of, with</t>
+  </si>
+  <si>
+    <t>Reports the largest x-coordinate of the patches in a model.</t>
+  </si>
+  <si>
+    <t>Reports the largest y-coordinate of the patches in a model.</t>
+  </si>
+  <si>
+    <t>any?</t>
+  </si>
+  <si>
+    <t>all?</t>
+  </si>
+  <si>
+    <t>Grand Canyon, Disease Solo, CA 1D Elementary, Simple Birth Rates</t>
+  </si>
+  <si>
+    <t>Mimicry, Ant Lines, Grand Canyon, Fruit Wars</t>
+  </si>
+  <si>
+    <t>Heatbugs, Shepherds, Membrane Formation, Grand Canyon</t>
+  </si>
+  <si>
+    <t>Autumn, Fur, Flocking, Small Worlds</t>
+  </si>
+  <si>
+    <t>Fairy Circles, Small Worlds, Party, Traffic Grid Goal</t>
+  </si>
+  <si>
+    <t>within, count, agentset, remaining</t>
+  </si>
+  <si>
+    <t>check, agents, agentset, exist</t>
+  </si>
+  <si>
+    <t>number, agents, many, turtles, links, patches, amount, total, sum</t>
+  </si>
+  <si>
+    <t>turtles, patches, links, with</t>
+  </si>
+  <si>
+    <t>create-turtles, turtles-own, die, ask</t>
+  </si>
+  <si>
+    <t>clear-patches, clear-turtles, die, reset-ticks</t>
+  </si>
+  <si>
+    <t>clear-all, clear-turtles, die, reset-ticks</t>
+  </si>
+  <si>
+    <t>clear-all, clear-patches, die, reset-ticks</t>
+  </si>
+  <si>
+    <t>pcolor, scale-color, turtles-own, of</t>
+  </si>
+  <si>
+    <t>hatch, sprout, ask, turtles-own</t>
+  </si>
+  <si>
+    <t>patches-own, patches, globals, neighbors</t>
+  </si>
+  <si>
+    <t>links, create-links-with, setxy, move-to</t>
+  </si>
+  <si>
+    <t>pen-up, clear-all, forward, right</t>
+  </si>
+  <si>
+    <t>pen-down, clear-all, forward, right</t>
+  </si>
+  <si>
+    <t>reset-ticks, ask, to, clear-all</t>
+  </si>
+  <si>
+    <t>nobody, count, if, any</t>
+  </si>
+  <si>
+    <t>all, if, other, nobody</t>
+  </si>
+  <si>
+    <t>ifelse, ifelse-value, any, all</t>
+  </si>
+  <si>
+    <t>if, ifelse, or, globals</t>
+  </si>
+  <si>
+    <t>create-links-with, links, any, count</t>
+  </si>
+  <si>
+    <t>mean, count, if, any</t>
+  </si>
+  <si>
+    <t>one-of, count, any, all</t>
+  </si>
+  <si>
+    <t>any, member, n-of, let</t>
+  </si>
+  <si>
+    <t>any, turtles-here, in-radius, patches</t>
+  </si>
+  <si>
+    <t>if, ifelse, and, of</t>
+  </si>
+  <si>
+    <t>tick, to, ask, clear-all</t>
+  </si>
+  <si>
+    <t>if, ifelse, repeat, tick</t>
+  </si>
+  <si>
+    <t>Checks if there is at least one agent in an agentset.</t>
+  </si>
+  <si>
+    <t>Makes a turtle move in any number of units on a straight path.</t>
+  </si>
+  <si>
+    <t>Makes a turtle make any number of new turtles that are identical to itself.</t>
+  </si>
+  <si>
+    <t>Starts a comments to take notes on a line of code. anything that follows a semicolon (;) will not be considered code.</t>
+  </si>
+  <si>
     <t>Clears all the drawings, turtles, plots, etc., leaving a blank slate.</t>
   </si>
   <si>
@@ -943,805 +1621,127 @@
     <t>Removes all the turtles as well as resets the numbering of turtles.</t>
   </si>
   <si>
-    <t>Counts the number of agents in an agentset.</t>
-  </si>
-  <si>
-    <t>Creates links with every agent in an agentset.</t>
-  </si>
-  <si>
-    <t>Creates turtles with random colors and headings at the center of the world.</t>
-  </si>
-  <si>
-    <t>Removes a turtle or link from the world.</t>
-  </si>
-  <si>
-    <t>Concludes a procedure.</t>
-  </si>
-  <si>
-    <t>Rounds a number down to the nearest integer.</t>
-  </si>
-  <si>
-    <t>Allows turtles to move in any number of units on a straight path.</t>
-  </si>
-  <si>
-    <t>Picks a value based on a provided list of condition-value pairs.</t>
-  </si>
-  <si>
-    <t>fd</t>
-  </si>
-  <si>
-    <t>ca</t>
-  </si>
-  <si>
-    <t>crt</t>
-  </si>
-  <si>
-    <t>turtle</t>
-  </si>
-  <si>
-    <t>Reports members of an agentset within a certain radius of an agent.</t>
-  </si>
-  <si>
-    <t>Reports members of an agentset within a "cone-of-vision" of an agent.</t>
-  </si>
-  <si>
-    <t>Places turtles in a circle circle around the center of the world.</t>
-  </si>
-  <si>
-    <t>Turns a turtle certain amount of degrees to the left.</t>
+    <t>Built-in turtle characteristic that the color of a turtle and allows us to change it.</t>
+  </si>
+  <si>
+    <t>Defines variables that can be accessed throughout the whole model and has the same value for all the agents.</t>
+  </si>
+  <si>
+    <t>Crystallization Basic, Rebellion, Hotelling's Law, Traffic Grid</t>
   </si>
   <si>
     <t>Reports all agents connected to a turtle with links.</t>
   </si>
   <si>
+    <t>Virus on a Network, Preferential Attachment, Team Assembly, Small Worlds</t>
+  </si>
+  <si>
+    <t>Reports the smallest x-coordinate of the patches in a model.</t>
+  </si>
+  <si>
+    <t>Reports the smallest y-coordinate of the patches in a model.</t>
+  </si>
+  <si>
+    <t>interaction, caller, original, nested, refer, talk</t>
+  </si>
+  <si>
+    <t>Reports an agentset that contains all the patches in a model.</t>
+  </si>
+  <si>
+    <t>Reports a shade of a base hue (color) based on where a speficied value falls is within a specified range (min-max).</t>
+  </si>
+  <si>
+    <t>Reports the angle of the caller towards an agent.</t>
+  </si>
+  <si>
+    <t>Reports the agentset of all the turtles on a caller's patch.</t>
+  </si>
+  <si>
+    <t>Checks if a reporter is true for all the agents in an agentset.</t>
+  </si>
+  <si>
+    <t>Membrane Formation, Giant Component, Small Worlds, Language Change</t>
+  </si>
+  <si>
+    <t>Reports an agentset that contains all the turtles in a model.</t>
+  </si>
+  <si>
     <t>Reports an agentset that contains all the links in a model.</t>
   </si>
   <si>
-    <t>Reports the highest value in a provided list.</t>
-  </si>
-  <si>
-    <t>Reports a list of top values in a provided list.</t>
-  </si>
-  <si>
-    <t>Reports the average of a provided list of numerical values.</t>
-  </si>
-  <si>
-    <t>Reports true if a value is within a list or if an agent is in an agentset.</t>
-  </si>
-  <si>
-    <t>Moves a turtle to set its x and y coordinates to be the same as another turtle or patch.</t>
-  </si>
-  <si>
-    <t>Reports the original turtle that asked another turtle to follow some rules.</t>
-  </si>
-  <si>
-    <t>Reports an agentset containing the eight neighboring patches.</t>
-  </si>
-  <si>
-    <t>Reports an agentset containing the four neighboring patches in cardinal directions (north, west, south, east).</t>
-  </si>
-  <si>
-    <t>A special value that helps checking if an agent exists or not.</t>
-  </si>
-  <si>
-    <t>Reports the value of an agent-owned variable.</t>
-  </si>
-  <si>
-    <t>Checks if either of two provided conditions is true.</t>
-  </si>
-  <si>
-    <t>Reports an agentset which is the same as the input agentset but omits the agent that used this primitive.</t>
-  </si>
-  <si>
-    <t>Reports a specific patch at the provided (x,y) conditions.</t>
-  </si>
-  <si>
-    <t>Reports the single patch that is the given distance “ahead” of this turtle</t>
-  </si>
-  <si>
-    <t>all, check, agents, agentset, exist</t>
-  </si>
-  <si>
-    <t>any?, nobody, count, not, if</t>
-  </si>
-  <si>
-    <t>Autumn, Shepherds, Scatter, Party</t>
-  </si>
-  <si>
-    <t>Autumn, Fur, Flocking, Small Worlds</t>
-  </si>
-  <si>
-    <t>if, or, if-else, ifelse-value, not</t>
-  </si>
-  <si>
-    <t>both, boolean, true, false, combine</t>
-  </si>
-  <si>
-    <t>all?, count, if, other, nobody</t>
-  </si>
-  <si>
-    <t>Anisogamy, Fur, Mammoths, Fireworks</t>
-  </si>
-  <si>
-    <t>Ants, Mimicry, Moths, Tumor</t>
-  </si>
-  <si>
-    <t>turtles, patches, links, with, n-of, one-of</t>
-  </si>
-  <si>
-    <t>do, commands, rules, behavior</t>
-  </si>
-  <si>
-    <t>kind, type, subset, custom</t>
-  </si>
-  <si>
-    <t>create-turtles, turtles-own, die, ask, hatch</t>
-  </si>
-  <si>
-    <t>Bacterial Infection, Disease Solo, Rabbit Grass Weeds, Wolf Sheep Predation</t>
-  </si>
-  <si>
-    <t>floor, round, mean, count</t>
-  </si>
-  <si>
-    <t>GasLab Circular Particles, Traffic 2 Lanes, Chaos in a Box, Decay</t>
-  </si>
-  <si>
-    <t>Flocking, Fur, Daisyworld, Wolf Sheep Predation, Follower</t>
-  </si>
-  <si>
-    <t>clear-patches, clear-turtles, die, reset-ticks, globals, create-turtles</t>
-  </si>
-  <si>
-    <t>clear, erase, remove, delete, clean, new, fresh, refresh, reset, restart, reboot, recreate</t>
-  </si>
-  <si>
-    <t>clear-all, clear-turtles, neighbors, pcolor, reset-ticks, globals, create-turtles</t>
-  </si>
-  <si>
-    <t>die, clear-all, clear-patches, reset-ticks, globals, create-turtles</t>
-  </si>
-  <si>
-    <t>Disease Solo, Turbulence, Simple Kinetics 3, Simple Birth Rates</t>
-  </si>
-  <si>
-    <t>Grand Canyon, Disease Solo, CA 1D Elementary, Simple Birth Rates</t>
-  </si>
-  <si>
-    <t>pcolor, scale-color, turtles-own, of, with</t>
-  </si>
-  <si>
-    <t>Sunflower, Mammoths, Bacterial Infection, Tumor</t>
-  </si>
-  <si>
-    <t>color, pencil, change, turtle, link, look, style, design, visual, hue, rgb, hex</t>
-  </si>
-  <si>
-    <t>number, agents, many, turtles, links, patches, amount, total, sum</t>
-  </si>
-  <si>
-    <t>mean, mod, if, if-else, any?, all, turtles, patches</t>
-  </si>
-  <si>
-    <t>Mimicry, Peppered Moths, Virus, Plant Growth</t>
-  </si>
-  <si>
-    <t>Team Assembly, CRISPR Bacterium, Membrane Formation, Virus on a Network</t>
-  </si>
-  <si>
-    <t>make, more, turtle, new, agent</t>
-  </si>
-  <si>
-    <t>create, make, more, turtle, new, agent</t>
-  </si>
-  <si>
-    <t>Sunflower, Wolf Sheep Predation, Virus, Plant Growth</t>
-  </si>
-  <si>
-    <t>Wolf Sheep Predation, Virus, Tumor, Bug Hunt Camouflage</t>
-  </si>
-  <si>
-    <t>turtles, links, patches, create-turtles</t>
-  </si>
-  <si>
-    <t>remove, end, kill, erase, death, disappear, eliminate, discard</t>
-  </si>
-  <si>
-    <t>Built-in turtle characteristic that the color of a turtle and allows us to change it.</t>
-  </si>
-  <si>
-    <t>Spreads a patch characteristic to its neighbors.</t>
-  </si>
-  <si>
-    <t>spread, share, disperse, radiate, propagate, broadcast</t>
-  </si>
-  <si>
-    <t>patches-own, patches, globals, neighbors, neighbors4</t>
-  </si>
-  <si>
-    <t>Ants, Slime, Heatbugs, Honeycomb</t>
-  </si>
-  <si>
-    <t>Flocking Vee Formations, Fur, BeeSmart Hive Finding, Autumn</t>
-  </si>
-  <si>
-    <t>facexy, min-pxcor, patch-ahead, setxy</t>
-  </si>
-  <si>
-    <t>length, far, measure, range, gap, separation, space</t>
-  </si>
-  <si>
-    <t>Reports the distance from one turtle/patch agent to another.</t>
-  </si>
-  <si>
-    <t>finish, complete, close, finalize, wrap, terminate, define</t>
-  </si>
-  <si>
-    <t>Rock Paper Scissors, El Farol, Paths, Traffic Grid</t>
-  </si>
-  <si>
-    <t>Disease Solo, Heatbugs, Voronoi - Emergent, Vants, Wealth Distribution</t>
-  </si>
-  <si>
-    <t>turn, spin, look, confront, watch, glare, stare, direction, angle</t>
-  </si>
-  <si>
-    <t>Changes a turtle's heading towards another turtle or patch.</t>
-  </si>
-  <si>
-    <t>Changes a turtle's heading towards a specific point (x, y) in the world.</t>
-  </si>
-  <si>
-    <t>Ant Lines, Scatter, Bidding Market, Thermostat</t>
-  </si>
-  <si>
-    <t>Daisyworld, Simple Birth Rates, Traffic Grid</t>
-  </si>
-  <si>
-    <t>round, up, integer, decimal, floating, math, calculate</t>
-  </si>
-  <si>
-    <t>Bidding Market, Vector Fields, CRISPR Ecosystem, Wolf Sheep Predation</t>
-  </si>
-  <si>
-    <t>Defines variables that can be accessed throughout the whole model and has the same value for all the agents.</t>
-  </si>
-  <si>
-    <t>variable, scope, universal, constant</t>
-  </si>
-  <si>
-    <t>turtles-own, patches-own, set, let</t>
-  </si>
-  <si>
-    <t>Shepherds, HIV, Giant Component, Fruit Wars</t>
-  </si>
-  <si>
-    <t>Chaos in a Box, Reactor Top Down, Voronoi, Galton Box</t>
-  </si>
-  <si>
-    <t>birth, new, create, conceive, spawn, generate, make, parent</t>
-  </si>
-  <si>
-    <t>Allows a turtle to make any number of new turtles that are identical to itself.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reactor X-Section, Sand, DLA Alternate Linear, </t>
-  </si>
-  <si>
-    <t>Carries out a provided set of rules (code) if a given condition is true. Does nothing if a given condition is false.</t>
-  </si>
-  <si>
-    <t>Carries out one set of rules if a given condition is true, and another set of rules if a given condition is false.</t>
-  </si>
-  <si>
-    <t>condition, true, false, branch</t>
-  </si>
-  <si>
-    <t>condition, true, false, branch, otherwise</t>
-  </si>
-  <si>
-    <t>if, ifelse-value, or, and</t>
-  </si>
-  <si>
-    <t>Crystallization Basic, Rebellion, Hotelling's Law, Traffic Grid</t>
-  </si>
-  <si>
-    <t>switch, case, condition, otherwise</t>
-  </si>
-  <si>
-    <t>if, if-else, or, globals</t>
-  </si>
-  <si>
-    <t>Echo, Virus, Sunflower Emergent, DLA Alternate</t>
-  </si>
-  <si>
-    <t>Flocking Vee Formations, BeeSmart Hive Finding, Bug Hunt Speeds, Flocking</t>
-  </si>
-  <si>
-    <t>around, near, circle, detect, see, vision</t>
-  </si>
-  <si>
-    <t>see, vision, detect, near</t>
-  </si>
-  <si>
-    <t>in-cone, other, neighbors, with</t>
-  </si>
-  <si>
-    <t>GasLab Circular Particles, Paths, Fruit Wars, Fairy Circles</t>
-  </si>
-  <si>
-    <t>formation, arrangement, ring, link</t>
-  </si>
-  <si>
-    <t>links, link-neighbors, create-links-with, setxy, move-to</t>
-  </si>
-  <si>
-    <t>Planarity, Giant Component, Small Worlds</t>
-  </si>
-  <si>
-    <t>right, set, face, forward</t>
-  </si>
-  <si>
-    <t>Mammoths, Tumor, Flocking, Slime</t>
-  </si>
-  <si>
-    <t>Creates a local variable that only exists within just one procedure or a statement surrended with brackets (`[  ]`).</t>
-  </si>
-  <si>
-    <t>variable, local, declare, value, constant, temporary</t>
-  </si>
-  <si>
-    <t>Disease Solo, Sand, Lennard-Jones, Boiling</t>
-  </si>
-  <si>
-    <t>Membrane Formation, Giant Component, Small Worlds, Language Change</t>
-  </si>
-  <si>
-    <t>create-links-with, links, any?, count</t>
-  </si>
-  <si>
-    <t>link-neighbors, turtles, patches, create-links-with</t>
-  </si>
-  <si>
-    <t>social, connect, network, web, complex, relation</t>
-  </si>
-  <si>
-    <t>connect, network, web, complex, relation, social</t>
-  </si>
-  <si>
-    <t>Virus on a Network, Preferential Attachment, Team Assembly, Small Worlds</t>
-  </si>
-  <si>
-    <t>count, min, mean, mod</t>
-  </si>
-  <si>
-    <t>Mimicry, Ant Lines, Grand Canyon, Fruit Wars</t>
-  </si>
-  <si>
-    <t>one-of, max, min, count</t>
-  </si>
-  <si>
-    <t>Simple Economy, Simple Viral Marketing</t>
-  </si>
-  <si>
-    <t>patch, coordinate, x, axis, world, view, west</t>
-  </si>
-  <si>
-    <t>patch, coordinate, y, axis, world, view, north</t>
-  </si>
-  <si>
-    <t>Urban Suite - Economic Disparity, DLA, Traffic Grid Goal</t>
-  </si>
-  <si>
-    <t>Fruit Wars, Ants, Sunflower Biomorphs, Random Balls</t>
-  </si>
-  <si>
-    <t>average, list, array, median, medium, middle</t>
-  </si>
-  <si>
-    <t>Mimicry, Flocking, Scatter, CRISPR Ecosystem</t>
-  </si>
-  <si>
-    <t>Fairy Circles, Small Worlds, Party, Traffic Grid Goal</t>
-  </si>
-  <si>
-    <t>big, high, largest, most, top</t>
-  </si>
-  <si>
-    <t>patch, coordinate, x, axis, world, view, east</t>
-  </si>
-  <si>
-    <t>patch, coordinate, x, axis, world, view, south</t>
-  </si>
-  <si>
-    <t>Fire, Tumor, Blood Sugar Regulation, Ant Lines</t>
-  </si>
-  <si>
-    <t>Autumn, Fireworks, Galton Box, Rugby</t>
-  </si>
-  <si>
-    <t>Performs the modulo operation; reports the remainder from the division of the first number by the second number.</t>
-  </si>
-  <si>
-    <t>remainder, divide, math, calculate, arithmetic</t>
-  </si>
-  <si>
-    <t>Sunflower, Flocking Vee Formations, Voronoi, Fruit Wars</t>
-  </si>
-  <si>
-    <t>jump, travel, relocate, shift, transport, hop</t>
-  </si>
-  <si>
-    <t>move, motion, straight, go, around, position, location, step, walk, jog</t>
-  </si>
-  <si>
-    <t>setxy, set, pxcor, patches</t>
-  </si>
-  <si>
-    <t>Heatbugs, Shepherds, Membrane Formation, Grand Canyon</t>
-  </si>
-  <si>
-    <t>interaction, caller, original, nested, refer, talk</t>
-  </si>
-  <si>
-    <t>Sunflower Biomorphs, Mammoths, Autumn, Fairy Circles</t>
-  </si>
-  <si>
-    <t>Reports "n" randomly picked agents from an agentset or items from a list.</t>
-  </si>
-  <si>
-    <t>subset, random, batch, portion, fragment</t>
-  </si>
-  <si>
-    <t>Virus, Heatbugs, Voronoi, Virus on a Network</t>
-  </si>
-  <si>
-    <t>surrounding, nearby, around, directions, next, border, adjoin, touch</t>
-  </si>
-  <si>
-    <t>neighbors4, patch-ahead, turtles-here, patches</t>
-  </si>
-  <si>
-    <t>Fur, DLA, Segregation, Daisyworld</t>
-  </si>
-  <si>
-    <t>neighbors, patch-ahead, turtles-here, patches</t>
-  </si>
-  <si>
-    <t>Fire, Life, Sandpile, Altruism</t>
-  </si>
-  <si>
-    <t>none, empty, dead, exist, nothing</t>
-  </si>
-  <si>
-    <t>any?, member?, n-of, let</t>
-  </si>
-  <si>
-    <t>Tumor, Heatbugs, Shepherds, HIV</t>
-  </si>
-  <si>
-    <t>variable, characteristic, property, feature</t>
-  </si>
-  <si>
-    <t>Urban Suite - Recycling, Paths, Slime, Language Change</t>
-  </si>
-  <si>
-    <t>Reports one randomly picked member from a provided agentset or list.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pick, select, draw, lottery </t>
-  </si>
-  <si>
-    <t>n-of, random, max-n-of, let</t>
-  </si>
-  <si>
-    <t>Mammoths, Ants, Shepherds, Fairy Circles</t>
-  </si>
-  <si>
-    <t>either, boolean, true, false, condition, compare</t>
-  </si>
-  <si>
-    <t>if, if-else, and, of</t>
-  </si>
-  <si>
-    <t>Lennard-Jones, GasLab Atmosphere, Bidding Market, Wealth Distribution</t>
-  </si>
-  <si>
-    <t>omit, exclude</t>
-  </si>
-  <si>
-    <t>any?, turtles-here, in-radius, patches</t>
-  </si>
-  <si>
-    <t>Virus, Flocking, Scatter, Fruit Wars</t>
-  </si>
-  <si>
-    <t>square, background, world</t>
-  </si>
-  <si>
-    <t>Ant Lines, Autumn, SmoothLife, Rumor Mill</t>
-  </si>
-  <si>
-    <t>before, see, detect, lead, onward</t>
-  </si>
-  <si>
-    <t>neighbors, in-radius, in-cone, nobody</t>
-  </si>
-  <si>
-    <t>Mammoths, Slime, Climate Change, Traffic Intersection</t>
-  </si>
-  <si>
-    <t>Reports an agentset that contains all the patches in a model.</t>
-  </si>
-  <si>
-    <t>Reports an agentset that contains all the turtles in a model.</t>
-  </si>
-  <si>
-    <t>Peppered Moths, Blood Sugar Regulation, Honeycomb</t>
-  </si>
-  <si>
-    <t>Defines custom characteristics (variables) for patches. Each custom characteristic can have a different value for each patch.</t>
-  </si>
-  <si>
-    <t>Diffusion Graphics, Grand Canyon, Life, Hoteling's Law</t>
-  </si>
-  <si>
-    <t>Reports a patch's color and changes a patch's color when used with the set primitive.</t>
-  </si>
-  <si>
-    <t>patch, square, world, background, paint</t>
-  </si>
-  <si>
-    <t>Vision Evolution, Rock Paper Scissors, Wolf Sheep Predation</t>
-  </si>
-  <si>
-    <t>Starts tracing the movement of the turtle on patches.</t>
-  </si>
-  <si>
-    <t>trace, draw, mark, paint, engrave, sketch</t>
-  </si>
-  <si>
-    <t>pen-up, clear-all, forward, right</t>
-  </si>
-  <si>
-    <t>Turtles Circling, Bidding Market, GasLab Single Collision, Pendulum</t>
-  </si>
-  <si>
-    <t>pen-down, clear-all, forward, right</t>
-  </si>
-  <si>
-    <t>Reports a random whole number between 0 and a specified number.</t>
-  </si>
-  <si>
-    <t>probability, chance, lottery, luck, toss, pick</t>
-  </si>
-  <si>
-    <t>Reports a random number with decimal points between 0 and a specified number.</t>
-  </si>
-  <si>
-    <t>decimal, floating, probability, chance, lottery, luck, toss, pick</t>
-  </si>
-  <si>
-    <t>Fire, Climate Change, Galton Box, Daisyworld</t>
-  </si>
-  <si>
-    <t>Reports a random number with decimal points that is picked from over a normal distribution with a specified mean and standard deviation.</t>
-  </si>
-  <si>
-    <t>distribution, bell, curve, chance, probability, lottery, luck, toss, pick</t>
-  </si>
-  <si>
-    <t>random, random-float, mean, set</t>
-  </si>
-  <si>
-    <t>Anisogamy, Autumn, Epidem Basic, Echo</t>
-  </si>
-  <si>
-    <t>Performs a provided set of rules (commands) repeatedly for a specified number of times.</t>
-  </si>
-  <si>
-    <t>repetition, again, multiple, loop, for, execute</t>
-  </si>
-  <si>
-    <t>ask, to, end, while</t>
-  </si>
-  <si>
-    <t>Disease Solo, Flocking Vee Formations, Peppered Moths, Ant Lines</t>
-  </si>
-  <si>
-    <t>counter, time, restart, clock, watch</t>
-  </si>
-  <si>
-    <t>Wolf Sheep Predation, Fire, Autumn, Climate Change</t>
-  </si>
-  <si>
-    <t>Changes a turtle's heading a certain amount of degrees to the right.</t>
-  </si>
-  <si>
-    <t>turn, angle, direction, orientation, twist, rotate</t>
-  </si>
-  <si>
-    <t>turn, spin, rotate, angle, direction, orientation</t>
-  </si>
-  <si>
-    <t>Wolf Sheep Simple, Mammoths, Anisogamy, DLA Simple</t>
-  </si>
-  <si>
-    <t>Reports the integer that is nearest to a specified value.</t>
-  </si>
-  <si>
-    <t>decimal, floating, near, approximate, roughly</t>
-  </si>
-  <si>
-    <t>Sex Ratio Equilibrium, Bug Hunt Camouflage, GenDrift T Interact, Blood Sugar Regulation</t>
-  </si>
-  <si>
-    <t>Reports a shade of a base hue (color) based on where a speficied value falls is within a specified range (min-max).</t>
-  </si>
-  <si>
-    <t>shade, legend, tint, paint, tone, saturation, gradient</t>
-  </si>
-  <si>
-    <t>Moths, Ants, Honeycomb, Autumn</t>
-  </si>
-  <si>
-    <t>Starts a comments to take notes on a line of code. Anything that follows a semicolon (;) will not be considered code.</t>
-  </si>
-  <si>
-    <t>comment, note</t>
-  </si>
-  <si>
-    <t>Changes the value of a variable (global, local, or agent-owned).</t>
-  </si>
-  <si>
-    <t>variable, value, change, modify, alter</t>
-  </si>
-  <si>
-    <t>Moves a turtle to the exact location defined by the provided x and y coordinates.</t>
-  </si>
-  <si>
-    <t>position, coordinate, location, move, jump, transport</t>
-  </si>
-  <si>
-    <t>move-to, min-pxcor, max-pycor, neighbors</t>
-  </si>
-  <si>
-    <t>Vision Evolution, Tumor, Virus, Flocking</t>
-  </si>
-  <si>
-    <t>Reports a turtles or link's shape and changes a turtle's or link's shape when used with the set primitive.</t>
-  </si>
-  <si>
-    <t>look, design, style, outline, image, bitmap, vector, picture, icon, appearance, figure, photo</t>
-  </si>
-  <si>
-    <t>Urban Suite - Pollution, Traffic Intersection, Mimicry, Ant Lines</t>
-  </si>
-  <si>
-    <t>Hoteling's Law, GasLab Circular Particles, CRISPR Bacterium, Ask Ordering Example</t>
-  </si>
-  <si>
-    <t>sort-on, count, mean, ask</t>
-  </si>
-  <si>
-    <t>sort-by, count, mean, ask</t>
-  </si>
-  <si>
-    <t>Reports a sorted version of a provided list based on a user-defined comparison.</t>
-  </si>
-  <si>
-    <t>Reports a sorted version of a provided agentset based on a user-defined comparison.</t>
-  </si>
-  <si>
-    <t>list, array, order, arrange, sift, cull, assort</t>
-  </si>
-  <si>
-    <t>Birthdays, Dice, DNA Protein Synthesis, Rnd Example</t>
-  </si>
-  <si>
-    <t>Daisyworld, Ant Lines, Heatbugs, Fairy Circles</t>
-  </si>
-  <si>
-    <t>create, birth, new, turtle, grow, germinate, spring, vegetate, root</t>
-  </si>
-  <si>
-    <t>Advances the tick counter by 1.</t>
-  </si>
-  <si>
-    <t>Creates new turtles at the center of a patch.</t>
-  </si>
-  <si>
-    <t>time, counter, clock, watch</t>
-  </si>
-  <si>
-    <t>reset-ticks, ask, to, clear-all</t>
-  </si>
-  <si>
-    <t>Flocking, BeeSmart Hive Finding, Slime, Shepherds</t>
-  </si>
-  <si>
-    <t>Turns a link between two turtles into a rigid connection so that the movement of one turtle impacts the movement of the other.</t>
-  </si>
-  <si>
-    <t>link, connection, attachment, lock, hook, anchor</t>
-  </si>
-  <si>
-    <t>Vision Evolution, DNA Replication Fork, Bug Hunt Environmental Changes, Connected Chemistry 8 Gas Particle Sandbox</t>
-  </si>
-  <si>
-    <t>Wolf Sheep Predation, Fire, Ants, Segregation</t>
-  </si>
-  <si>
-    <t>Mimicry, Moths, Rock Paper Scissors, HIV</t>
-  </si>
-  <si>
-    <t>to-report, end, ask, create-turtles</t>
-  </si>
-  <si>
-    <t>to, end, ask, if</t>
-  </si>
-  <si>
-    <t>procedure, function, return, calculate, transform, input, output</t>
-  </si>
-  <si>
-    <t>turn, angle, face, direction, twist, spin</t>
-  </si>
-  <si>
-    <t>Chaos in a Box, Bug Hunt Coevolution, GenEvo 1 Genetic Switch, Traffic 2 Lanes</t>
-  </si>
-  <si>
-    <t>shape, triangle, mobile, agent, tortoise, animal, person, people, object, thing</t>
-  </si>
-  <si>
-    <t>Reports a specific turtle that has the provided who number.</t>
-  </si>
-  <si>
-    <t>El Farol, Party, Segregation, Chemical Equilibrium</t>
-  </si>
-  <si>
-    <t>neighbors, patches, other, in-radius</t>
-  </si>
-  <si>
-    <t>touch, contact, near, communicate, rub, tangent, tap, collide, notice, recognize, sense</t>
-  </si>
-  <si>
-    <t>Disease Solo, Flocking Vee Formations, Tumor, Wolf Sheep Predation</t>
-  </si>
-  <si>
-    <t>set, globals, patches-own, with, of</t>
-  </si>
-  <si>
-    <t>variable, declare, characteristic, property, attribute, trait, quality, phenotype</t>
-  </si>
-  <si>
-    <t>Reports a subset of the original agentset that only contains the agents with specified characteristics.</t>
-  </si>
-  <si>
-    <t>specific, agentset, query, narrow, subset, reduce, fragment, select</t>
-  </si>
-  <si>
-    <t>if, of, turtles-own, patches-own</t>
-  </si>
-  <si>
-    <t>Fur, Mimicry, Ants, Heatbugs</t>
-  </si>
-  <si>
-    <t>count, if, n-of, with</t>
-  </si>
-  <si>
-    <t>Reports the largest x-coordinate of the patches in a model.</t>
-  </si>
-  <si>
-    <t>Reports the largest y-coordinate of the patches in a model.</t>
-  </si>
-  <si>
-    <t>Reports the smallest x-coordinate of the patches in a model.</t>
-  </si>
-  <si>
-    <t>Reports the smallest y-coordinate of the patches in a model.</t>
-  </si>
-  <si>
-    <t>any, within, count, agentset, remaining</t>
+    <t>mean, mod, if, ifelse</t>
+  </si>
+  <si>
+    <t>clear-all</t>
+  </si>
+  <si>
+    <t>if, or, ifelse, with</t>
+  </si>
+  <si>
+    <t>Disease Solo, Heatbugs, Voronoi - Emergent, Vants</t>
+  </si>
+  <si>
+    <t>face, setxy, max-pxcor, towards</t>
+  </si>
+  <si>
+    <t>right, random, turtles, move-to</t>
+  </si>
+  <si>
+    <t>Daisyworld, Simple Birth Rates, Traffic Grid, CRISPR Bacterium</t>
+  </si>
+  <si>
+    <t>towards, facexy, forward, right</t>
+  </si>
+  <si>
+    <t>Reactor X-Section, Sand, DLA Alternate Linear, Fire</t>
+  </si>
+  <si>
+    <t>Planarity, Giant Component, Small Worlds, Spread of Disease</t>
+  </si>
+  <si>
+    <t>count, mean, mod, of</t>
+  </si>
+  <si>
+    <t>one-of, max, of, count</t>
+  </si>
+  <si>
+    <t>Urban Suite - Economic Disparity, DLA, Traffic Grid Goal, Blood Sugar Regulation</t>
+  </si>
+  <si>
+    <t>Fruit Wars, Ants, Sunflower Biomorphs, Galton Box</t>
+  </si>
+  <si>
+    <t>setxy, set, max-pxcor, patches</t>
+  </si>
+  <si>
+    <t>Peppered Moths, Blood Sugar Regulation, Honeycomb, Rock Paper Scissors</t>
+  </si>
+  <si>
+    <t>Diffusion Graphics, Grand Canyon, Life, Paths</t>
+  </si>
+  <si>
+    <t>Vision Evolution, Rock Paper Scissors, Wolf Sheep Predation, Bacterial Infection</t>
+  </si>
+  <si>
+    <t>Anisogamy, Autumn, Echo, Sex Ratio Equilibrium</t>
+  </si>
+  <si>
+    <t>Bacteria Hunt Speeds, Mammoths, Anisogamy, DLA Simple</t>
+  </si>
+  <si>
+    <t>Sex Ratio Equilibrium, Bug Hunt Camouflage, Bacterial Infection, Blood Sugar Regulation</t>
+  </si>
+  <si>
+    <t>4 Block Stalagmites, GasLab Circular Particles, CRISPR Bacterium, Ask Ordering Example</t>
+  </si>
+  <si>
+    <t>left, forward, towards, face</t>
+  </si>
+  <si>
+    <t>set, globals, patches-own, with</t>
+  </si>
+  <si>
+    <t>Moths, Traffic Basic, Shepherds, Sunflower Biomorphs</t>
   </si>
 </sst>
 </file>
@@ -2279,9 +2279,9 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A80" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J89" sqref="J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2348,13 +2348,13 @@
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>69</v>
+        <v>390</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>195</v>
+        <v>442</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>236</v>
+        <v>397</v>
       </c>
       <c r="D2" s="24" t="b">
         <v>0</v>
@@ -2372,10 +2372,10 @@
         <v>1</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>237</v>
+        <v>411</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2383,10 +2383,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>196</v>
+        <v>179</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>241</v>
+        <v>213</v>
       </c>
       <c r="D3" s="24" t="b">
         <v>0</v>
@@ -2404,21 +2404,21 @@
         <v>1</v>
       </c>
       <c r="I3" s="23" t="s">
-        <v>240</v>
+        <v>448</v>
       </c>
       <c r="J3" s="23" t="s">
-        <v>239</v>
+        <v>394</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>11</v>
+        <v>389</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>197</v>
+        <v>423</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>470</v>
+        <v>396</v>
       </c>
       <c r="D4" s="25" t="b">
         <v>0</v>
@@ -2436,21 +2436,21 @@
         <v>1</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>242</v>
+        <v>412</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>243</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>246</v>
+        <v>216</v>
       </c>
       <c r="D5" s="24" t="b">
         <v>1</v>
@@ -2468,21 +2468,21 @@
         <v>0</v>
       </c>
       <c r="I5" s="23" t="s">
-        <v>245</v>
+        <v>399</v>
       </c>
       <c r="J5" s="23" t="s">
-        <v>244</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>247</v>
+        <v>217</v>
       </c>
       <c r="D6" s="24" t="b">
         <v>1</v>
@@ -2500,21 +2500,21 @@
         <v>0</v>
       </c>
       <c r="I6" s="23" t="s">
-        <v>248</v>
+        <v>400</v>
       </c>
       <c r="J6" s="23" t="s">
-        <v>249</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>200</v>
+        <v>182</v>
       </c>
       <c r="C7" s="23" t="s">
-        <v>289</v>
+        <v>247</v>
       </c>
       <c r="D7" s="24" t="b">
         <v>0</v>
@@ -2532,21 +2532,21 @@
         <v>1</v>
       </c>
       <c r="I7" s="23" t="s">
-        <v>250</v>
+        <v>219</v>
       </c>
       <c r="J7" s="23" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>201</v>
+        <v>427</v>
       </c>
       <c r="C8" s="23" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
       <c r="D8" s="24" t="b">
         <v>1</v>
@@ -2564,21 +2564,21 @@
         <v>0</v>
       </c>
       <c r="I8" s="23" t="s">
-        <v>253</v>
+        <v>401</v>
       </c>
       <c r="J8" s="23" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>41</v>
+        <v>447</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>201</v>
+        <v>427</v>
       </c>
       <c r="C9" s="23" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
       <c r="D9" s="24" t="b">
         <v>1</v>
@@ -2596,21 +2596,21 @@
         <v>0</v>
       </c>
       <c r="I9" s="23" t="s">
-        <v>253</v>
+        <v>401</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>202</v>
+        <v>428</v>
       </c>
       <c r="C10" s="23" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
       <c r="D10" s="24" t="b">
         <v>1</v>
@@ -2628,21 +2628,21 @@
         <v>0</v>
       </c>
       <c r="I10" s="23" t="s">
-        <v>255</v>
+        <v>402</v>
       </c>
       <c r="J10" s="23" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>203</v>
+        <v>429</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
       <c r="D11" s="24" t="b">
         <v>1</v>
@@ -2660,21 +2660,21 @@
         <v>0</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>256</v>
+        <v>403</v>
       </c>
       <c r="J11" s="23" t="s">
-        <v>258</v>
+        <v>391</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B12" s="27" t="s">
-        <v>272</v>
+        <v>430</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
       <c r="D12" s="24" t="b">
         <v>0</v>
@@ -2692,21 +2692,21 @@
         <v>0</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>259</v>
+        <v>404</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B13" s="23" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>262</v>
+        <v>398</v>
       </c>
       <c r="D13" s="24" t="b">
         <v>0</v>
@@ -2724,53 +2724,53 @@
         <v>1</v>
       </c>
       <c r="I13" s="23" t="s">
-        <v>263</v>
+        <v>446</v>
       </c>
       <c r="J13" s="23" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A14" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>184</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>273</v>
+      </c>
+      <c r="D14" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E14" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>324</v>
-      </c>
-      <c r="D14" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E14" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F14" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G14" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H14" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>14</v>
-      </c>
       <c r="J14" s="23" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A15" s="22" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="D15" s="24" t="b">
         <v>1</v>
@@ -2788,21 +2788,21 @@
         <v>0</v>
       </c>
       <c r="I15" s="23" t="s">
-        <v>46</v>
+        <v>405</v>
       </c>
       <c r="J15" s="23" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A16" s="22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B16" s="27" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="D16" s="24" t="b">
         <v>1</v>
@@ -2820,21 +2820,21 @@
         <v>0</v>
       </c>
       <c r="I16" s="23" t="s">
-        <v>46</v>
+        <v>405</v>
       </c>
       <c r="J16" s="23" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B17" s="23" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>271</v>
+        <v>233</v>
       </c>
       <c r="D17" s="25" t="b">
         <v>0</v>
@@ -2852,21 +2852,21 @@
         <v>0</v>
       </c>
       <c r="I17" s="23" t="s">
-        <v>270</v>
+        <v>232</v>
       </c>
       <c r="J17" s="23" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="29" x14ac:dyDescent="0.2">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="23" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>274</v>
+        <v>235</v>
       </c>
       <c r="D18" s="25" t="b">
         <v>0</v>
@@ -2884,21 +2884,21 @@
         <v>0</v>
       </c>
       <c r="I18" s="23" t="s">
-        <v>275</v>
+        <v>406</v>
       </c>
       <c r="J18" s="23" t="s">
-        <v>276</v>
+        <v>236</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B19" s="23" t="s">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>279</v>
+        <v>239</v>
       </c>
       <c r="D19" s="25" t="b">
         <v>0</v>
@@ -2916,21 +2916,21 @@
         <v>0</v>
       </c>
       <c r="I19" s="23" t="s">
-        <v>278</v>
+        <v>238</v>
       </c>
       <c r="J19" s="23" t="s">
-        <v>277</v>
+        <v>237</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="B20" s="23" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>281</v>
+        <v>241</v>
       </c>
       <c r="D20" s="24" t="b">
         <v>1</v>
@@ -2948,21 +2948,21 @@
         <v>0</v>
       </c>
       <c r="I20" s="23" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="J20" s="23" t="s">
-        <v>282</v>
+        <v>242</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B21" s="23" t="s">
-        <v>285</v>
+        <v>244</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>284</v>
+        <v>243</v>
       </c>
       <c r="D21" s="25" t="b">
         <v>0</v>
@@ -2980,21 +2980,21 @@
         <v>0</v>
       </c>
       <c r="I21" s="23" t="s">
-        <v>77</v>
+        <v>453</v>
       </c>
       <c r="J21" s="23" t="s">
-        <v>283</v>
+        <v>449</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B22" s="23" t="s">
-        <v>286</v>
+        <v>245</v>
       </c>
       <c r="C22" s="23" t="s">
-        <v>284</v>
+        <v>243</v>
       </c>
       <c r="D22" s="24" t="b">
         <v>0</v>
@@ -3012,21 +3012,21 @@
         <v>0</v>
       </c>
       <c r="I22" s="23" t="s">
-        <v>48</v>
+        <v>450</v>
       </c>
       <c r="J22" s="23" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="22" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B23" s="23" t="s">
-        <v>209</v>
+        <v>188</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>289</v>
+        <v>247</v>
       </c>
       <c r="D23" s="24" t="b">
         <v>0</v>
@@ -3044,21 +3044,21 @@
         <v>1</v>
       </c>
       <c r="I23" s="23" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="J23" s="23" t="s">
-        <v>288</v>
+        <v>452</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A24" s="28" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B24" s="27" t="s">
-        <v>210</v>
+        <v>424</v>
       </c>
       <c r="C24" s="23" t="s">
-        <v>347</v>
+        <v>289</v>
       </c>
       <c r="D24" s="24" t="b">
         <v>0</v>
@@ -3076,21 +3076,21 @@
         <v>0</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>50</v>
+        <v>451</v>
       </c>
       <c r="J24" s="23" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A25" s="28" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>210</v>
+        <v>424</v>
       </c>
       <c r="C25" s="23" t="s">
-        <v>347</v>
+        <v>289</v>
       </c>
       <c r="D25" s="24" t="b">
         <v>0</v>
@@ -3108,21 +3108,21 @@
         <v>0</v>
       </c>
       <c r="I25" s="23" t="s">
-        <v>50</v>
+        <v>451</v>
       </c>
       <c r="J25" s="23" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="23" t="s">
-        <v>291</v>
+        <v>431</v>
       </c>
       <c r="C26" s="23" t="s">
-        <v>292</v>
+        <v>249</v>
       </c>
       <c r="D26" s="24" t="b">
         <v>1</v>
@@ -3140,21 +3140,21 @@
         <v>0</v>
       </c>
       <c r="I26" s="23" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="J26" s="23" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A27" s="22" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>297</v>
+        <v>425</v>
       </c>
       <c r="C27" s="23" t="s">
-        <v>296</v>
+        <v>253</v>
       </c>
       <c r="D27" s="25" t="b">
         <v>0</v>
@@ -3172,21 +3172,21 @@
         <v>0</v>
       </c>
       <c r="I27" s="23" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="J27" s="23" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A28" s="22" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B28" s="23" t="s">
-        <v>299</v>
+        <v>254</v>
       </c>
       <c r="C28" s="23" t="s">
-        <v>301</v>
+        <v>256</v>
       </c>
       <c r="D28" s="24" t="b">
         <v>0</v>
@@ -3204,21 +3204,21 @@
         <v>1</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>83</v>
+        <v>413</v>
       </c>
       <c r="J28" s="23" t="s">
-        <v>298</v>
+        <v>454</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A29" s="28" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B29" s="23" t="s">
-        <v>300</v>
+        <v>255</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>302</v>
+        <v>257</v>
       </c>
       <c r="D29" s="25" t="b">
         <v>0</v>
@@ -3236,21 +3236,21 @@
         <v>1</v>
       </c>
       <c r="I29" s="23" t="s">
-        <v>303</v>
+        <v>258</v>
       </c>
       <c r="J29" s="23" t="s">
-        <v>304</v>
+        <v>432</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B30" s="23" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>305</v>
+        <v>259</v>
       </c>
       <c r="D30" s="25" t="b">
         <v>0</v>
@@ -3268,53 +3268,53 @@
         <v>1</v>
       </c>
       <c r="I30" s="23" t="s">
-        <v>306</v>
+        <v>414</v>
       </c>
       <c r="J30" s="29" t="s">
-        <v>307</v>
+        <v>260</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A31" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>263</v>
+      </c>
+      <c r="D31" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" s="24" t="b">
+        <v>1</v>
+      </c>
+      <c r="F31" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="G31" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="H31" s="25" t="b">
+        <v>0</v>
+      </c>
+      <c r="I31" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="C31" s="23" t="s">
-        <v>310</v>
-      </c>
-      <c r="D31" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="E31" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="F31" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="G31" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="H31" s="25" t="b">
-        <v>0</v>
-      </c>
-      <c r="I31" s="23" t="s">
-        <v>20</v>
-      </c>
       <c r="J31" s="23" t="s">
-        <v>308</v>
+        <v>261</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A32" s="22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B32" s="23" t="s">
-        <v>216</v>
+        <v>194</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>309</v>
+        <v>262</v>
       </c>
       <c r="D32" s="25" t="b">
         <v>0</v>
@@ -3332,21 +3332,21 @@
         <v>0</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>311</v>
+        <v>264</v>
       </c>
       <c r="J32" s="23" t="s">
-        <v>312</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B33" s="23" t="s">
-        <v>218</v>
+        <v>196</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>313</v>
+        <v>266</v>
       </c>
       <c r="D33" s="24" t="b">
         <v>1</v>
@@ -3364,21 +3364,21 @@
         <v>0</v>
       </c>
       <c r="I33" s="23" t="s">
-        <v>314</v>
+        <v>407</v>
       </c>
       <c r="J33" s="23" t="s">
-        <v>315</v>
+        <v>455</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="22" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B34" s="23" t="s">
-        <v>219</v>
+        <v>197</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>409</v>
+        <v>337</v>
       </c>
       <c r="D34" s="25" t="b">
         <v>0</v>
@@ -3396,21 +3396,21 @@
         <v>0</v>
       </c>
       <c r="I34" s="23" t="s">
-        <v>316</v>
+        <v>267</v>
       </c>
       <c r="J34" s="23" t="s">
-        <v>317</v>
+        <v>268</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="22" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="B35" s="23" t="s">
-        <v>318</v>
+        <v>269</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>319</v>
+        <v>270</v>
       </c>
       <c r="D35" s="24" t="b">
         <v>0</v>
@@ -3428,21 +3428,21 @@
         <v>1</v>
       </c>
       <c r="I35" s="23" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="J35" s="23" t="s">
-        <v>320</v>
+        <v>271</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A36" s="22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="23" t="s">
-        <v>220</v>
+        <v>433</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>325</v>
+        <v>274</v>
       </c>
       <c r="D36" s="25" t="b">
         <v>0</v>
@@ -3460,10 +3460,10 @@
         <v>0</v>
       </c>
       <c r="I36" s="23" t="s">
-        <v>322</v>
+        <v>415</v>
       </c>
       <c r="J36" s="23" t="s">
-        <v>321</v>
+        <v>443</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3471,10 +3471,10 @@
         <v>6</v>
       </c>
       <c r="B37" s="23" t="s">
-        <v>221</v>
+        <v>445</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>325</v>
+        <v>274</v>
       </c>
       <c r="D37" s="25" t="b">
         <v>0</v>
@@ -3492,21 +3492,21 @@
         <v>0</v>
       </c>
       <c r="I37" s="23" t="s">
-        <v>323</v>
+        <v>272</v>
       </c>
       <c r="J37" s="23" t="s">
-        <v>326</v>
+        <v>434</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="B38" s="23" t="s">
-        <v>222</v>
+        <v>198</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>338</v>
+        <v>280</v>
       </c>
       <c r="D38" s="24" t="b">
         <v>0</v>
@@ -3524,21 +3524,21 @@
         <v>1</v>
       </c>
       <c r="I38" s="23" t="s">
-        <v>327</v>
+        <v>456</v>
       </c>
       <c r="J38" s="23" t="s">
-        <v>328</v>
+        <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B39" s="23" t="s">
-        <v>223</v>
+        <v>199</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>338</v>
+        <v>280</v>
       </c>
       <c r="D39" s="24" t="b">
         <v>0</v>
@@ -3556,21 +3556,21 @@
         <v>1</v>
       </c>
       <c r="I39" s="23" t="s">
-        <v>329</v>
+        <v>457</v>
       </c>
       <c r="J39" s="23" t="s">
-        <v>330</v>
+        <v>275</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B40" s="23" t="s">
-        <v>466</v>
+        <v>387</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>331</v>
+        <v>276</v>
       </c>
       <c r="D40" s="24" t="b">
         <v>0</v>
@@ -3588,21 +3588,21 @@
         <v>1</v>
       </c>
       <c r="I40" s="23" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J40" s="23" t="s">
-        <v>333</v>
+        <v>458</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B41" s="23" t="s">
-        <v>467</v>
+        <v>388</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>332</v>
+        <v>277</v>
       </c>
       <c r="D41" s="24" t="b">
         <v>0</v>
@@ -3620,21 +3620,21 @@
         <v>1</v>
       </c>
       <c r="I41" s="23" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="J41" s="23" t="s">
-        <v>334</v>
+        <v>459</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B42" s="23" t="s">
-        <v>224</v>
+        <v>200</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>335</v>
+        <v>278</v>
       </c>
       <c r="D42" s="24" t="b">
         <v>0</v>
@@ -3652,21 +3652,21 @@
         <v>1</v>
       </c>
       <c r="I42" s="23" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="J42" s="23" t="s">
-        <v>336</v>
+        <v>279</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A43" s="22" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B43" s="23" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D43" s="24" t="b">
         <v>0</v>
@@ -3684,21 +3684,21 @@
         <v>1</v>
       </c>
       <c r="I43" s="23" t="s">
-        <v>465</v>
+        <v>386</v>
       </c>
       <c r="J43" s="23" t="s">
-        <v>337</v>
+        <v>395</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="22" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B44" s="23" t="s">
-        <v>468</v>
+        <v>435</v>
       </c>
       <c r="C44" s="23" t="s">
-        <v>339</v>
+        <v>281</v>
       </c>
       <c r="D44" s="24" t="b">
         <v>0</v>
@@ -3716,21 +3716,21 @@
         <v>1</v>
       </c>
       <c r="I44" s="23" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="J44" s="30" t="s">
-        <v>341</v>
+        <v>283</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B45" s="23" t="s">
-        <v>469</v>
+        <v>436</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>340</v>
+        <v>282</v>
       </c>
       <c r="D45" s="24" t="b">
         <v>0</v>
@@ -3748,21 +3748,21 @@
         <v>1</v>
       </c>
       <c r="I45" s="23" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="J45" s="30" t="s">
-        <v>342</v>
+        <v>284</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B46" s="23" t="s">
-        <v>343</v>
+        <v>285</v>
       </c>
       <c r="C46" s="23" t="s">
-        <v>344</v>
+        <v>286</v>
       </c>
       <c r="D46" s="24" t="b">
         <v>0</v>
@@ -3780,21 +3780,21 @@
         <v>1</v>
       </c>
       <c r="I46" s="23" t="s">
-        <v>100</v>
+        <v>416</v>
       </c>
       <c r="J46" s="23" t="s">
-        <v>345</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A47" s="22" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>226</v>
+        <v>202</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>346</v>
+        <v>288</v>
       </c>
       <c r="D47" s="24" t="b">
         <v>0</v>
@@ -3812,21 +3812,21 @@
         <v>0</v>
       </c>
       <c r="I47" s="23" t="s">
-        <v>348</v>
+        <v>460</v>
       </c>
       <c r="J47" s="23" t="s">
-        <v>349</v>
+        <v>393</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A48" s="22" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B48" s="23" t="s">
-        <v>227</v>
+        <v>203</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>350</v>
+        <v>437</v>
       </c>
       <c r="D48" s="25" t="b">
         <v>0</v>
@@ -3844,21 +3844,21 @@
         <v>0</v>
       </c>
       <c r="I48" s="23" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="J48" s="23" t="s">
-        <v>351</v>
+        <v>290</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B49" s="23" t="s">
-        <v>352</v>
+        <v>291</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>353</v>
+        <v>292</v>
       </c>
       <c r="D49" s="25" t="b">
         <v>0</v>
@@ -3876,21 +3876,21 @@
         <v>1</v>
       </c>
       <c r="I49" s="23" t="s">
-        <v>25</v>
+        <v>417</v>
       </c>
       <c r="J49" s="23" t="s">
-        <v>354</v>
+        <v>293</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B50" s="27" t="s">
-        <v>228</v>
+        <v>204</v>
       </c>
       <c r="C50" s="23" t="s">
-        <v>355</v>
+        <v>294</v>
       </c>
       <c r="D50" s="24" t="b">
         <v>0</v>
@@ -3908,21 +3908,21 @@
         <v>0</v>
       </c>
       <c r="I50" s="23" t="s">
-        <v>356</v>
+        <v>295</v>
       </c>
       <c r="J50" s="23" t="s">
-        <v>357</v>
+        <v>296</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B51" s="27" t="s">
-        <v>229</v>
+        <v>205</v>
       </c>
       <c r="C51" s="23" t="s">
-        <v>355</v>
+        <v>294</v>
       </c>
       <c r="D51" s="24" t="b">
         <v>0</v>
@@ -3940,21 +3940,21 @@
         <v>0</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>358</v>
+        <v>297</v>
       </c>
       <c r="J51" s="30" t="s">
-        <v>359</v>
+        <v>298</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B52" s="23" t="s">
-        <v>230</v>
+        <v>206</v>
       </c>
       <c r="C52" s="23" t="s">
-        <v>360</v>
+        <v>299</v>
       </c>
       <c r="D52" s="25" t="b">
         <v>0</v>
@@ -3972,21 +3972,21 @@
         <v>1</v>
       </c>
       <c r="I52" s="23" t="s">
-        <v>361</v>
+        <v>418</v>
       </c>
       <c r="J52" s="23" t="s">
-        <v>362</v>
+        <v>300</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A53" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B53" s="23" t="s">
-        <v>231</v>
+        <v>207</v>
       </c>
       <c r="C53" s="23" t="s">
-        <v>363</v>
+        <v>301</v>
       </c>
       <c r="D53" s="25" t="b">
         <v>0</v>
@@ -4004,21 +4004,21 @@
         <v>1</v>
       </c>
       <c r="I53" s="23" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J53" s="23" t="s">
-        <v>364</v>
+        <v>302</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="22" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B54" s="23" t="s">
-        <v>365</v>
+        <v>303</v>
       </c>
       <c r="C54" s="23" t="s">
-        <v>366</v>
+        <v>304</v>
       </c>
       <c r="D54" s="25" t="b">
         <v>0</v>
@@ -4036,21 +4036,21 @@
         <v>1</v>
       </c>
       <c r="I54" s="23" t="s">
-        <v>367</v>
+        <v>305</v>
       </c>
       <c r="J54" s="23" t="s">
-        <v>368</v>
+        <v>306</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A55" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B55" s="23" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>369</v>
+        <v>307</v>
       </c>
       <c r="D55" s="25" t="b">
         <v>0</v>
@@ -4068,21 +4068,21 @@
         <v>1</v>
       </c>
       <c r="I55" s="23" t="s">
-        <v>370</v>
+        <v>420</v>
       </c>
       <c r="J55" s="23" t="s">
-        <v>371</v>
+        <v>308</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="22" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B56" s="27" t="s">
-        <v>233</v>
+        <v>209</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>372</v>
+        <v>309</v>
       </c>
       <c r="D56" s="25" t="b">
         <v>0</v>
@@ -4100,21 +4100,21 @@
         <v>0</v>
       </c>
       <c r="I56" s="23" t="s">
-        <v>373</v>
+        <v>419</v>
       </c>
       <c r="J56" s="23" t="s">
-        <v>374</v>
+        <v>310</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="22" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B57" s="23" t="s">
-        <v>234</v>
+        <v>210</v>
       </c>
       <c r="C57" s="23" t="s">
-        <v>375</v>
+        <v>311</v>
       </c>
       <c r="D57" s="24" t="b">
         <v>1</v>
@@ -4132,21 +4132,21 @@
         <v>0</v>
       </c>
       <c r="I57" s="23" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="J57" s="23" t="s">
-        <v>376</v>
+        <v>312</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A58" s="22" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B58" s="27" t="s">
-        <v>235</v>
+        <v>211</v>
       </c>
       <c r="C58" s="23" t="s">
-        <v>377</v>
+        <v>313</v>
       </c>
       <c r="D58" s="24" t="b">
         <v>0</v>
@@ -4164,10 +4164,10 @@
         <v>0</v>
       </c>
       <c r="I58" s="23" t="s">
-        <v>378</v>
+        <v>314</v>
       </c>
       <c r="J58" s="23" t="s">
-        <v>379</v>
+        <v>315</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4175,10 +4175,10 @@
         <v>5</v>
       </c>
       <c r="B59" s="23" t="s">
-        <v>380</v>
+        <v>438</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>375</v>
+        <v>311</v>
       </c>
       <c r="D59" s="24" t="b">
         <v>1</v>
@@ -4196,21 +4196,21 @@
         <v>0</v>
       </c>
       <c r="I59" s="23" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="J59" s="23" t="s">
-        <v>382</v>
+        <v>461</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A60" s="22" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>383</v>
+        <v>316</v>
       </c>
       <c r="C60" s="23" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="D60" s="24" t="b">
         <v>1</v>
@@ -4228,21 +4228,21 @@
         <v>0</v>
       </c>
       <c r="I60" s="23" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="J60" s="23" t="s">
-        <v>384</v>
+        <v>462</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A61" s="22" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B61" s="27" t="s">
-        <v>385</v>
+        <v>317</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>386</v>
+        <v>318</v>
       </c>
       <c r="D61" s="25" t="b">
         <v>0</v>
@@ -4260,21 +4260,21 @@
         <v>0</v>
       </c>
       <c r="I61" s="23" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="J61" s="23" t="s">
-        <v>387</v>
+        <v>463</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A62" s="22" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B62" s="23" t="s">
-        <v>388</v>
+        <v>319</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>389</v>
+        <v>320</v>
       </c>
       <c r="D62" s="25" t="b">
         <v>0</v>
@@ -4292,21 +4292,21 @@
         <v>0</v>
       </c>
       <c r="I62" s="23" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
       <c r="J62" s="23" t="s">
-        <v>391</v>
+        <v>321</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A63" s="22" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B63" s="23" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="C63" s="23" t="s">
-        <v>389</v>
+        <v>320</v>
       </c>
       <c r="D63" s="25" t="b">
         <v>0</v>
@@ -4324,21 +4324,21 @@
         <v>0</v>
       </c>
       <c r="I63" s="23" t="s">
-        <v>392</v>
+        <v>409</v>
       </c>
       <c r="J63" s="23" t="s">
-        <v>391</v>
+        <v>321</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A64" s="22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B64" s="23" t="s">
-        <v>393</v>
+        <v>322</v>
       </c>
       <c r="C64" s="23" t="s">
-        <v>394</v>
+        <v>323</v>
       </c>
       <c r="D64" s="25" t="b">
         <v>0</v>
@@ -4356,21 +4356,21 @@
         <v>1</v>
       </c>
       <c r="I64" s="23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="J64" s="23" t="s">
-        <v>351</v>
+        <v>290</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B65" s="23" t="s">
-        <v>395</v>
+        <v>324</v>
       </c>
       <c r="C65" s="23" t="s">
-        <v>396</v>
+        <v>325</v>
       </c>
       <c r="D65" s="25" t="b">
         <v>0</v>
@@ -4388,21 +4388,21 @@
         <v>1</v>
       </c>
       <c r="I65" s="23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J65" s="23" t="s">
-        <v>397</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A66" s="22" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B66" s="23" t="s">
-        <v>398</v>
+        <v>327</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>399</v>
+        <v>328</v>
       </c>
       <c r="D66" s="24" t="b">
         <v>0</v>
@@ -4420,21 +4420,21 @@
         <v>1</v>
       </c>
       <c r="I66" s="23" t="s">
-        <v>400</v>
+        <v>329</v>
       </c>
       <c r="J66" s="23" t="s">
-        <v>401</v>
+        <v>464</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A67" s="22" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B67" s="27" t="s">
-        <v>402</v>
+        <v>330</v>
       </c>
       <c r="C67" s="23" t="s">
-        <v>403</v>
+        <v>331</v>
       </c>
       <c r="D67" s="24" t="b">
         <v>0</v>
@@ -4452,21 +4452,21 @@
         <v>1</v>
       </c>
       <c r="I67" s="23" t="s">
-        <v>404</v>
+        <v>332</v>
       </c>
       <c r="J67" s="23" t="s">
-        <v>405</v>
+        <v>333</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A68" s="22" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B68" s="23" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="C68" s="23" t="s">
-        <v>406</v>
+        <v>334</v>
       </c>
       <c r="D68" s="24" t="b">
         <v>1</v>
@@ -4484,21 +4484,21 @@
         <v>0</v>
       </c>
       <c r="I68" s="23" t="s">
-        <v>117</v>
+        <v>421</v>
       </c>
       <c r="J68" s="23" t="s">
-        <v>407</v>
+        <v>335</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A69" s="22" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="B69" s="23" t="s">
-        <v>408</v>
+        <v>336</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>410</v>
+        <v>338</v>
       </c>
       <c r="D69" s="25" t="b">
         <v>0</v>
@@ -4516,21 +4516,21 @@
         <v>0</v>
       </c>
       <c r="I69" s="23" t="s">
-        <v>119</v>
+        <v>468</v>
       </c>
       <c r="J69" s="23" t="s">
-        <v>411</v>
+        <v>465</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A70" s="22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B70" s="27" t="s">
-        <v>412</v>
+        <v>339</v>
       </c>
       <c r="C70" s="23" t="s">
-        <v>413</v>
+        <v>340</v>
       </c>
       <c r="D70" s="24" t="b">
         <v>0</v>
@@ -4548,21 +4548,21 @@
         <v>1</v>
       </c>
       <c r="I70" s="23" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="J70" s="23" t="s">
-        <v>414</v>
+        <v>466</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B71" s="23" t="s">
-        <v>415</v>
+        <v>439</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>416</v>
+        <v>341</v>
       </c>
       <c r="D71" s="25" t="b">
         <v>0</v>
@@ -4580,21 +4580,21 @@
         <v>1</v>
       </c>
       <c r="I71" s="23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J71" s="23" t="s">
-        <v>417</v>
+        <v>342</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B72" s="27" t="s">
-        <v>418</v>
+        <v>426</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>419</v>
+        <v>343</v>
       </c>
       <c r="D72" s="25" t="b">
         <v>0</v>
@@ -4612,21 +4612,21 @@
         <v>1</v>
       </c>
       <c r="I72" s="23" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="J72" s="23" t="s">
-        <v>417</v>
+        <v>342</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A73" s="22" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="B73" s="23" t="s">
-        <v>420</v>
+        <v>344</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>421</v>
+        <v>345</v>
       </c>
       <c r="D73" s="24" t="b">
         <v>0</v>
@@ -4644,21 +4644,21 @@
         <v>1</v>
       </c>
       <c r="I73" s="23" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="J73" s="23" t="s">
-        <v>407</v>
+        <v>335</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A74" s="22" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B74" s="23" t="s">
-        <v>422</v>
+        <v>346</v>
       </c>
       <c r="C74" s="23" t="s">
-        <v>423</v>
+        <v>347</v>
       </c>
       <c r="D74" s="24" t="b">
         <v>0</v>
@@ -4676,21 +4676,21 @@
         <v>0</v>
       </c>
       <c r="I74" s="23" t="s">
-        <v>424</v>
+        <v>348</v>
       </c>
       <c r="J74" s="24" t="s">
-        <v>425</v>
+        <v>349</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A75" s="22" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B75" s="27" t="s">
-        <v>426</v>
+        <v>350</v>
       </c>
       <c r="C75" s="23" t="s">
-        <v>427</v>
+        <v>351</v>
       </c>
       <c r="D75" s="24" t="b">
         <v>0</v>
@@ -4708,21 +4708,21 @@
         <v>0</v>
       </c>
       <c r="I75" s="23" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J75" s="23" t="s">
-        <v>428</v>
+        <v>352</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A76" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B76" s="23" t="s">
-        <v>432</v>
+        <v>355</v>
       </c>
       <c r="C76" s="23" t="s">
-        <v>434</v>
+        <v>357</v>
       </c>
       <c r="D76" s="25" t="b">
         <v>0</v>
@@ -4740,21 +4740,21 @@
         <v>1</v>
       </c>
       <c r="I76" s="23" t="s">
-        <v>430</v>
+        <v>353</v>
       </c>
       <c r="J76" s="23" t="s">
-        <v>429</v>
+        <v>467</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A77" s="22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B77" s="23" t="s">
-        <v>433</v>
+        <v>356</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>434</v>
+        <v>357</v>
       </c>
       <c r="D77" s="25" t="b">
         <v>0</v>
@@ -4772,21 +4772,21 @@
         <v>1</v>
       </c>
       <c r="I77" s="23" t="s">
-        <v>431</v>
+        <v>354</v>
       </c>
       <c r="J77" s="23" t="s">
-        <v>435</v>
+        <v>358</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="22" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="B78" s="23" t="s">
-        <v>439</v>
+        <v>362</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>437</v>
+        <v>360</v>
       </c>
       <c r="D78" s="25" t="b">
         <v>0</v>
@@ -4804,21 +4804,21 @@
         <v>0</v>
       </c>
       <c r="I78" s="23" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="J78" s="23" t="s">
-        <v>436</v>
+        <v>359</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A79" s="22" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="B79" s="23" t="s">
-        <v>438</v>
+        <v>361</v>
       </c>
       <c r="C79" s="23" t="s">
-        <v>440</v>
+        <v>363</v>
       </c>
       <c r="D79" s="24" t="b">
         <v>1</v>
@@ -4836,21 +4836,21 @@
         <v>0</v>
       </c>
       <c r="I79" s="23" t="s">
-        <v>441</v>
+        <v>410</v>
       </c>
       <c r="J79" s="23" t="s">
-        <v>442</v>
+        <v>364</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="43" x14ac:dyDescent="0.2">
       <c r="A80" s="22" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B80" s="23" t="s">
-        <v>443</v>
+        <v>365</v>
       </c>
       <c r="C80" s="23" t="s">
-        <v>444</v>
+        <v>366</v>
       </c>
       <c r="D80" s="25" t="b">
         <v>0</v>
@@ -4868,21 +4868,21 @@
         <v>0</v>
       </c>
       <c r="I80" s="23" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J80" s="23" t="s">
-        <v>445</v>
+        <v>367</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B81" s="23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C81" s="23" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D81" s="24" t="b">
         <v>1</v>
@@ -4900,21 +4900,21 @@
         <v>1</v>
       </c>
       <c r="I81" s="23" t="s">
-        <v>448</v>
+        <v>370</v>
       </c>
       <c r="J81" s="23" t="s">
-        <v>446</v>
+        <v>368</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="22" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="B82" s="23" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>450</v>
+        <v>372</v>
       </c>
       <c r="D82" s="24" t="b">
         <v>0</v>
@@ -4932,21 +4932,21 @@
         <v>1</v>
       </c>
       <c r="I82" s="23" t="s">
-        <v>449</v>
+        <v>371</v>
       </c>
       <c r="J82" s="23" t="s">
-        <v>447</v>
+        <v>369</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A83" s="22" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="B83" s="23" t="s">
-        <v>128</v>
+        <v>440</v>
       </c>
       <c r="C83" s="23" t="s">
-        <v>451</v>
+        <v>373</v>
       </c>
       <c r="D83" s="25" t="b">
         <v>0</v>
@@ -4964,21 +4964,21 @@
         <v>0</v>
       </c>
       <c r="I83" s="23" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="J83" s="23" t="s">
-        <v>452</v>
+        <v>374</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A84" s="22" t="s">
-        <v>215</v>
+        <v>193</v>
       </c>
       <c r="B84" s="27" t="s">
-        <v>454</v>
+        <v>376</v>
       </c>
       <c r="C84" s="23" t="s">
-        <v>453</v>
+        <v>375</v>
       </c>
       <c r="D84" s="24" t="b">
         <v>1</v>
@@ -4996,10 +4996,10 @@
         <v>0</v>
       </c>
       <c r="I84" s="23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J84" s="23" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -5007,10 +5007,10 @@
         <v>4</v>
       </c>
       <c r="B85" s="27" t="s">
-        <v>381</v>
+        <v>444</v>
       </c>
       <c r="C85" s="23" t="s">
-        <v>453</v>
+        <v>375</v>
       </c>
       <c r="D85" s="24" t="b">
         <v>1</v>
@@ -5028,21 +5028,21 @@
         <v>0</v>
       </c>
       <c r="I85" s="23" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J85" s="23" t="s">
-        <v>405</v>
+        <v>333</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A86" s="22" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="B86" s="23" t="s">
-        <v>131</v>
+        <v>441</v>
       </c>
       <c r="C86" s="23" t="s">
-        <v>457</v>
+        <v>379</v>
       </c>
       <c r="D86" s="25" t="b">
         <v>0</v>
@@ -5060,21 +5060,21 @@
         <v>0</v>
       </c>
       <c r="I86" s="23" t="s">
-        <v>456</v>
+        <v>378</v>
       </c>
       <c r="J86" s="23" t="s">
-        <v>455</v>
+        <v>377</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A87" s="22" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B87" s="23" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C87" s="23" t="s">
-        <v>460</v>
+        <v>381</v>
       </c>
       <c r="D87" s="24" t="b">
         <v>1</v>
@@ -5092,21 +5092,21 @@
         <v>0</v>
       </c>
       <c r="I87" s="23" t="s">
-        <v>459</v>
+        <v>469</v>
       </c>
       <c r="J87" s="23" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="15" x14ac:dyDescent="0.2">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A88" s="22" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B88" s="23" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C88" s="23" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D88" s="24" t="b">
         <v>1</v>
@@ -5124,21 +5124,21 @@
         <v>0</v>
       </c>
       <c r="I88" s="23" t="s">
-        <v>137</v>
+        <v>422</v>
       </c>
       <c r="J88" s="23" t="s">
-        <v>138</v>
+        <v>470</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="28" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="B89" s="29" t="s">
-        <v>461</v>
+        <v>382</v>
       </c>
       <c r="C89" s="29" t="s">
-        <v>462</v>
+        <v>383</v>
       </c>
       <c r="D89" s="24" t="b">
         <v>1</v>
@@ -5156,10 +5156,10 @@
         <v>0</v>
       </c>
       <c r="I89" s="29" t="s">
-        <v>463</v>
+        <v>384</v>
       </c>
       <c r="J89" s="23" t="s">
-        <v>464</v>
+        <v>385</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="14" x14ac:dyDescent="0.2">
@@ -8096,34 +8096,34 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="E2" s="4" t="b">
         <v>1</v>
@@ -8131,16 +8131,16 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="E3" s="4" t="b">
         <v>1</v>
@@ -8148,16 +8148,16 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="E4" s="4" t="b">
         <v>1</v>
@@ -8165,16 +8165,16 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="E5" s="4" t="b">
         <v>1</v>
@@ -8182,16 +8182,16 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="E6" s="4" t="b">
         <v>1</v>
@@ -8199,16 +8199,16 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="E7" s="4" t="b">
         <v>0</v>
@@ -8216,16 +8216,16 @@
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="E8" s="4" t="b">
         <v>0</v>
@@ -8233,16 +8233,16 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
-        <v>169</v>
+        <v>153</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>167</v>
+        <v>151</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>170</v>
+        <v>154</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
       <c r="E9" s="4" t="b">
         <v>0</v>
@@ -8250,16 +8250,16 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>171</v>
+        <v>155</v>
       </c>
       <c r="B10" s="11" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="E10" s="4" t="b">
         <v>0</v>
@@ -8267,16 +8267,16 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="E11" s="4" t="b">
         <v>0</v>
@@ -8284,16 +8284,16 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="E12" s="4" t="b">
         <v>0</v>
@@ -8627,27 +8627,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="D2" s="4" t="b">
         <v>1</v>
@@ -8655,13 +8655,13 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="15" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="D3" s="4" t="b">
         <v>1</v>
@@ -8669,13 +8669,13 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="D4" s="4" t="b">
         <v>1</v>
@@ -8683,13 +8683,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="D5" s="4" t="b">
         <v>1</v>
@@ -8697,13 +8697,13 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="D6" s="4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
minor fixes to primitive short description
</commit_message>
<xml_diff>
--- a/metadata/binddata.xlsx
+++ b/metadata/binddata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ual895/Git/newdictionary/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBAAF0A-976A-BC4D-9D75-B21B898FE90C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF797C85-5B40-984C-B0D7-92152723881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="500" windowWidth="24260" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4540" yWindow="500" windowWidth="24260" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primitives" sheetId="1" r:id="rId1"/>
@@ -498,9 +498,6 @@
     <t>to</t>
   </si>
   <si>
-    <t>used to begin a command procedure</t>
-  </si>
-  <si>
     <t>to, begin, command</t>
   </si>
   <si>
@@ -810,9 +807,6 @@
     <t>Checks if both provided conditions are true.</t>
   </si>
   <si>
-    <t>Asks agents do things.</t>
-  </si>
-  <si>
     <t>Defines a custom breed of turtles.</t>
   </si>
   <si>
@@ -1077,9 +1071,6 @@
     <t>Mammoths, Tumor, Flocking, Slime</t>
   </si>
   <si>
-    <t>Creates a local variable that only exists within just one procedure or a statement surrended with brackets (`[  ]`).</t>
-  </si>
-  <si>
     <t>variable, local, declare, value, constant, temporary</t>
   </si>
   <si>
@@ -1398,9 +1389,6 @@
     <t>shape, triangle, mobile, agent, tortoise, animal, person, people, object, thing</t>
   </si>
   <si>
-    <t>Reports a specific turtle that has the provided who number.</t>
-  </si>
-  <si>
     <t>El Farol, Party, Segregation, Chemical Equilibrium</t>
   </si>
   <si>
@@ -1560,9 +1548,6 @@
     <t>Removes all the turtles as well as resets the numbering of turtles.</t>
   </si>
   <si>
-    <t>Built-in turtle characteristic that the color of a turtle and allows us to change it.</t>
-  </si>
-  <si>
     <t>Defines variables that can be accessed throughout the whole model and has the same value for all the agents.</t>
   </si>
   <si>
@@ -1690,6 +1675,21 @@
   </si>
   <si>
     <t>If you are not sure where to start learning NetLogo, check out this list of the most useful and frequently used primitives in NetLogo. Once you learn these primitives well, you should be able to learn any other primitive easily.</t>
+  </si>
+  <si>
+    <t>Asks agents to do things.</t>
+  </si>
+  <si>
+    <t>Built-in turtle characteristic that reports the color of a turtle and allows us to change it.</t>
+  </si>
+  <si>
+    <t>Creates a local variable that only exists within a procedure or a statement surrounded with brackets (`[  ]`).</t>
+  </si>
+  <si>
+    <t>Begins a command procedure</t>
+  </si>
+  <si>
+    <t>Reports a specific turtle that has the provided unique number.</t>
   </si>
 </sst>
 </file>
@@ -2237,9 +2237,9 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView topLeftCell="A79" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J89" sqref="J89"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2306,13 +2306,13 @@
     </row>
     <row r="2" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="21" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B2" s="22" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="D2" s="23" t="b">
         <v>0</v>
@@ -2330,10 +2330,10 @@
         <v>1</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2341,10 +2341,10 @@
         <v>10</v>
       </c>
       <c r="B3" s="22" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D3" s="23" t="b">
         <v>0</v>
@@ -2362,21 +2362,21 @@
         <v>1</v>
       </c>
       <c r="I3" s="22" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="J3" s="22" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="21" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="D4" s="24" t="b">
         <v>0</v>
@@ -2394,10 +2394,10 @@
         <v>1</v>
       </c>
       <c r="I4" s="22" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="J4" s="22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2405,10 +2405,10 @@
         <v>38</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>159</v>
+        <v>448</v>
       </c>
       <c r="C5" s="22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D5" s="23" t="b">
         <v>1</v>
@@ -2426,10 +2426,10 @@
         <v>0</v>
       </c>
       <c r="I5" s="22" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="J5" s="22" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2437,10 +2437,10 @@
         <v>11</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D6" s="23" t="b">
         <v>1</v>
@@ -2458,21 +2458,21 @@
         <v>0</v>
       </c>
       <c r="I6" s="22" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="J6" s="22" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C7" s="22" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D7" s="23" t="b">
         <v>0</v>
@@ -2490,21 +2490,21 @@
         <v>1</v>
       </c>
       <c r="I7" s="22" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J7" s="22" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D8" s="23" t="b">
         <v>1</v>
@@ -2522,21 +2522,21 @@
         <v>0</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="J8" s="22" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="29" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D9" s="23" t="b">
         <v>1</v>
@@ -2554,10 +2554,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2565,10 +2565,10 @@
         <v>39</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D10" s="23" t="b">
         <v>1</v>
@@ -2586,10 +2586,10 @@
         <v>0</v>
       </c>
       <c r="I10" s="22" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="J10" s="22" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2597,10 +2597,10 @@
         <v>40</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D11" s="23" t="b">
         <v>1</v>
@@ -2618,10 +2618,10 @@
         <v>0</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="J11" s="22" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15" x14ac:dyDescent="0.2">
@@ -2629,10 +2629,10 @@
         <v>41</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>409</v>
+        <v>449</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D12" s="23" t="b">
         <v>0</v>
@@ -2650,21 +2650,21 @@
         <v>0</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="J12" s="22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C13" s="22" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="D13" s="23" t="b">
         <v>0</v>
@@ -2682,10 +2682,10 @@
         <v>1</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="J13" s="22" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2693,10 +2693,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C14" s="22" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="D14" s="24" t="b">
         <v>0</v>
@@ -2717,18 +2717,18 @@
         <v>13</v>
       </c>
       <c r="J14" s="22" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:26" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D15" s="23" t="b">
         <v>1</v>
@@ -2746,10 +2746,10 @@
         <v>0</v>
       </c>
       <c r="I15" s="22" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="J15" s="22" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="29" x14ac:dyDescent="0.2">
@@ -2757,42 +2757,42 @@
         <v>42</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C16" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="D16" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E16" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F16" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G16" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H16" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I16" s="22" t="s">
+        <v>380</v>
+      </c>
+      <c r="J16" s="22" t="s">
         <v>207</v>
-      </c>
-      <c r="D16" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E16" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="F16" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G16" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H16" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>384</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B17" s="22" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D17" s="24" t="b">
         <v>0</v>
@@ -2810,10 +2810,10 @@
         <v>0</v>
       </c>
       <c r="I17" s="22" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J17" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -2821,42 +2821,42 @@
         <v>14</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="D18" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E18" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F18" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G18" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H18" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I18" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="J18" s="22" t="s">
         <v>213</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="D18" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E18" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F18" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G18" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>385</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A19" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B19" s="22" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D19" s="24" t="b">
         <v>0</v>
@@ -2874,53 +2874,53 @@
         <v>0</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J19" s="22" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>218</v>
+      </c>
+      <c r="D20" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F20" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G20" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H20" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="I20" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="B20" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="C20" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="D20" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E20" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F20" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G20" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="22" t="s">
-        <v>68</v>
-      </c>
       <c r="J20" s="22" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A21" s="21" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B21" s="22" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D21" s="24" t="b">
         <v>0</v>
@@ -2938,10 +2938,10 @@
         <v>0</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="J21" s="22" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -2949,10 +2949,10 @@
         <v>43</v>
       </c>
       <c r="B22" s="22" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C22" s="22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D22" s="23" t="b">
         <v>0</v>
@@ -2970,42 +2970,42 @@
         <v>0</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="J22" s="22" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A23" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="C23" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="D23" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E23" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F23" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G23" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H23" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="D23" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E23" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F23" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G23" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="22" t="s">
-        <v>71</v>
-      </c>
       <c r="J23" s="22" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
@@ -3013,10 +3013,10 @@
         <v>44</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D24" s="23" t="b">
         <v>0</v>
@@ -3034,21 +3034,21 @@
         <v>0</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="J24" s="22" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="C25" s="22" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D25" s="23" t="b">
         <v>0</v>
@@ -3066,10 +3066,10 @@
         <v>0</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="J25" s="22" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3077,75 +3077,75 @@
         <v>15</v>
       </c>
       <c r="B26" s="22" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="C26" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="D26" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F26" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G26" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H26" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="J26" s="22" t="s">
         <v>228</v>
-      </c>
-      <c r="D26" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F26" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G26" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I26" s="22" t="s">
-        <v>229</v>
-      </c>
-      <c r="J26" s="22" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="22" t="s">
+        <v>400</v>
+      </c>
+      <c r="C27" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="D27" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E27" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F27" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G27" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H27" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I27" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B27" s="22" t="s">
-        <v>404</v>
-      </c>
-      <c r="C27" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="D27" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E27" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F27" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G27" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I27" s="22" t="s">
-        <v>73</v>
-      </c>
       <c r="J27" s="22" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B28" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C28" s="22" t="s">
         <v>233</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>235</v>
-      </c>
       <c r="D28" s="23" t="b">
         <v>0</v>
       </c>
@@ -3162,10 +3162,10 @@
         <v>1</v>
       </c>
       <c r="I28" s="22" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="J28" s="22" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3173,11 +3173,11 @@
         <v>16</v>
       </c>
       <c r="B29" s="22" t="s">
+        <v>232</v>
+      </c>
+      <c r="C29" s="22" t="s">
         <v>234</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>236</v>
-      </c>
       <c r="D29" s="24" t="b">
         <v>0</v>
       </c>
@@ -3194,10 +3194,10 @@
         <v>1</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J29" s="22" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3205,10 +3205,10 @@
         <v>17</v>
       </c>
       <c r="B30" s="22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C30" s="22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D30" s="24" t="b">
         <v>0</v>
@@ -3226,10 +3226,10 @@
         <v>1</v>
       </c>
       <c r="I30" s="22" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="J30" s="28" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3237,10 +3237,10 @@
         <v>18</v>
       </c>
       <c r="B31" s="22" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C31" s="22" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D31" s="24" t="b">
         <v>0</v>
@@ -3261,7 +3261,7 @@
         <v>19</v>
       </c>
       <c r="J31" s="22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3269,31 +3269,31 @@
         <v>20</v>
       </c>
       <c r="B32" s="22" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C32" s="22" t="s">
+        <v>239</v>
+      </c>
+      <c r="D32" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E32" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F32" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G32" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H32" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I32" s="22" t="s">
         <v>241</v>
       </c>
-      <c r="D32" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E32" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F32" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G32" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H32" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I32" s="22" t="s">
-        <v>243</v>
-      </c>
       <c r="J32" s="22" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3301,10 +3301,10 @@
         <v>21</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C33" s="22" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D33" s="23" t="b">
         <v>1</v>
@@ -3322,21 +3322,21 @@
         <v>0</v>
       </c>
       <c r="I33" s="22" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="J33" s="22" t="s">
-        <v>434</v>
+        <v>429</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C34" s="22" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="D34" s="24" t="b">
         <v>0</v>
@@ -3354,42 +3354,42 @@
         <v>0</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J34" s="22" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="22" t="s">
+        <v>450</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="D35" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E35" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F35" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G35" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H35" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I35" s="22" t="s">
         <v>76</v>
       </c>
-      <c r="B35" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>249</v>
-      </c>
-      <c r="D35" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E35" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F35" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G35" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H35" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" s="22" t="s">
-        <v>77</v>
-      </c>
       <c r="J35" s="22" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3397,10 +3397,10 @@
         <v>22</v>
       </c>
       <c r="B36" s="22" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D36" s="24" t="b">
         <v>0</v>
@@ -3418,10 +3418,10 @@
         <v>0</v>
       </c>
       <c r="I36" s="22" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="J36" s="22" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3429,10 +3429,10 @@
         <v>6</v>
       </c>
       <c r="B37" s="22" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="D37" s="24" t="b">
         <v>0</v>
@@ -3450,21 +3450,21 @@
         <v>0</v>
       </c>
       <c r="I37" s="22" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J37" s="22" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D38" s="23" t="b">
         <v>0</v>
@@ -3482,21 +3482,21 @@
         <v>1</v>
       </c>
       <c r="I38" s="22" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="J38" s="22" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D39" s="23" t="b">
         <v>0</v>
@@ -3514,53 +3514,53 @@
         <v>1</v>
       </c>
       <c r="I39" s="22" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="J39" s="22" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="22" t="s">
+        <v>362</v>
+      </c>
+      <c r="C40" s="22" t="s">
+        <v>252</v>
+      </c>
+      <c r="D40" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F40" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G40" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H40" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I40" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="22" t="s">
-        <v>366</v>
-      </c>
-      <c r="C40" s="22" t="s">
-        <v>255</v>
-      </c>
-      <c r="D40" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F40" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G40" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H40" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I40" s="22" t="s">
-        <v>79</v>
-      </c>
       <c r="J40" s="22" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" s="22" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C41" s="22" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="D41" s="23" t="b">
         <v>0</v>
@@ -3578,54 +3578,54 @@
         <v>1</v>
       </c>
       <c r="I41" s="22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J41" s="22" t="s">
-        <v>438</v>
+        <v>433</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="D42" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E42" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F42" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G42" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H42" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I42" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>257</v>
-      </c>
-      <c r="D42" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E42" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F42" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G42" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I42" s="22" t="s">
-        <v>84</v>
-      </c>
       <c r="J42" s="22" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="C43" s="22" t="s">
-        <v>86</v>
-      </c>
       <c r="D43" s="23" t="b">
         <v>0</v>
       </c>
@@ -3642,53 +3642,53 @@
         <v>1</v>
       </c>
       <c r="I43" s="22" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="J43" s="22" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="C44" s="22" t="s">
+        <v>257</v>
+      </c>
+      <c r="D44" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F44" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G44" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H44" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="22" t="s">
-        <v>414</v>
-      </c>
-      <c r="C44" s="22" t="s">
-        <v>260</v>
-      </c>
-      <c r="D44" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F44" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G44" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H44" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I44" s="22" t="s">
-        <v>88</v>
-      </c>
       <c r="J44" s="29" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="21" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D45" s="23" t="b">
         <v>0</v>
@@ -3706,21 +3706,21 @@
         <v>1</v>
       </c>
       <c r="I45" s="22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J45" s="29" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C46" s="22" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D46" s="23" t="b">
         <v>0</v>
@@ -3738,10 +3738,10 @@
         <v>1</v>
       </c>
       <c r="I46" s="22" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="J46" s="22" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="47" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3749,10 +3749,10 @@
         <v>45</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D47" s="23" t="b">
         <v>0</v>
@@ -3770,42 +3770,42 @@
         <v>0</v>
       </c>
       <c r="I47" s="22" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="J47" s="22" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
     </row>
     <row r="48" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A48" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="D48" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E48" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F48" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G48" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I48" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="B48" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C48" s="22" t="s">
-        <v>416</v>
-      </c>
-      <c r="D48" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E48" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F48" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G48" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="H48" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I48" s="22" t="s">
-        <v>92</v>
-      </c>
       <c r="J48" s="22" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="49" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3813,10 +3813,10 @@
         <v>23</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D49" s="24" t="b">
         <v>0</v>
@@ -3834,10 +3834,10 @@
         <v>1</v>
       </c>
       <c r="I49" s="22" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="J49" s="22" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="50" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -3845,10 +3845,10 @@
         <v>46</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D50" s="23" t="b">
         <v>0</v>
@@ -3866,10 +3866,10 @@
         <v>0</v>
       </c>
       <c r="I50" s="22" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J50" s="22" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="51" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -3877,42 +3877,42 @@
         <v>47</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C51" s="22" t="s">
+        <v>270</v>
+      </c>
+      <c r="D51" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E51" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F51" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G51" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H51" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I51" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="D51" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E51" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F51" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G51" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="H51" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I51" s="22" t="s">
-        <v>276</v>
-      </c>
       <c r="J51" s="29" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C52" s="22" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D52" s="24" t="b">
         <v>0</v>
@@ -3930,10 +3930,10 @@
         <v>1</v>
       </c>
       <c r="I52" s="22" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="J52" s="22" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="53" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -3941,10 +3941,10 @@
         <v>24</v>
       </c>
       <c r="B53" s="22" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C53" s="22" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D53" s="24" t="b">
         <v>0</v>
@@ -3965,39 +3965,39 @@
         <v>25</v>
       </c>
       <c r="J53" s="22" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B54" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="C54" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="D54" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E54" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G54" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H54" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I54" s="22" t="s">
+        <v>281</v>
+      </c>
+      <c r="J54" s="22" t="s">
         <v>282</v>
-      </c>
-      <c r="C54" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="D54" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E54" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="F54" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G54" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="H54" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I54" s="22" t="s">
-        <v>284</v>
-      </c>
-      <c r="J54" s="22" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="55" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4005,10 +4005,10 @@
         <v>26</v>
       </c>
       <c r="B55" s="22" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C55" s="22" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D55" s="24" t="b">
         <v>0</v>
@@ -4026,10 +4026,10 @@
         <v>1</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="J55" s="22" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="56" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4037,10 +4037,10 @@
         <v>48</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C56" s="22" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D56" s="24" t="b">
         <v>0</v>
@@ -4058,42 +4058,42 @@
         <v>0</v>
       </c>
       <c r="I56" s="22" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="J56" s="22" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="57" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" s="22" t="s">
+        <v>287</v>
+      </c>
+      <c r="D57" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E57" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G57" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H57" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I57" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B57" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="C57" s="22" t="s">
-        <v>290</v>
-      </c>
-      <c r="D57" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E57" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F57" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G57" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H57" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I57" s="22" t="s">
-        <v>96</v>
-      </c>
       <c r="J57" s="22" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="58" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4101,10 +4101,10 @@
         <v>49</v>
       </c>
       <c r="B58" s="26" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C58" s="22" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="D58" s="23" t="b">
         <v>0</v>
@@ -4122,10 +4122,10 @@
         <v>0</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="J58" s="22" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="59" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4133,10 +4133,10 @@
         <v>5</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="D59" s="23" t="b">
         <v>1</v>
@@ -4154,42 +4154,42 @@
         <v>0</v>
       </c>
       <c r="I59" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J59" s="22" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A60" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B60" s="22" t="s">
+        <v>292</v>
+      </c>
+      <c r="C60" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="B60" s="22" t="s">
-        <v>295</v>
-      </c>
-      <c r="C60" s="22" t="s">
+      <c r="D60" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E60" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F60" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G60" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H60" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I60" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="D60" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E60" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F60" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G60" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H60" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I60" s="22" t="s">
-        <v>99</v>
-      </c>
       <c r="J60" s="22" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
     </row>
     <row r="61" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4197,10 +4197,10 @@
         <v>50</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D61" s="24" t="b">
         <v>0</v>
@@ -4221,18 +4221,18 @@
         <v>51</v>
       </c>
       <c r="J61" s="22" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
     </row>
     <row r="62" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A62" s="21" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D62" s="24" t="b">
         <v>0</v>
@@ -4250,21 +4250,21 @@
         <v>0</v>
       </c>
       <c r="I62" s="22" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="J62" s="22" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="63" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A63" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="22" t="s">
-        <v>103</v>
-      </c>
       <c r="C63" s="22" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D63" s="24" t="b">
         <v>0</v>
@@ -4282,10 +4282,10 @@
         <v>0</v>
       </c>
       <c r="I63" s="22" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="J63" s="22" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="64" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4293,10 +4293,10 @@
         <v>27</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="D64" s="24" t="b">
         <v>0</v>
@@ -4317,7 +4317,7 @@
         <v>28</v>
       </c>
       <c r="J64" s="22" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4325,10 +4325,10 @@
         <v>29</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D65" s="24" t="b">
         <v>0</v>
@@ -4349,18 +4349,18 @@
         <v>30</v>
       </c>
       <c r="J65" s="22" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="66" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A66" s="21" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D66" s="23" t="b">
         <v>0</v>
@@ -4378,10 +4378,10 @@
         <v>1</v>
       </c>
       <c r="I66" s="22" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="J66" s="22" t="s">
-        <v>443</v>
+        <v>438</v>
       </c>
     </row>
     <row r="67" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4389,42 +4389,42 @@
         <v>52</v>
       </c>
       <c r="B67" s="26" t="s">
+        <v>306</v>
+      </c>
+      <c r="C67" s="22" t="s">
+        <v>307</v>
+      </c>
+      <c r="D67" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E67" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="F67" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="G67" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="H67" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I67" s="22" t="s">
+        <v>308</v>
+      </c>
+      <c r="J67" s="22" t="s">
         <v>309</v>
-      </c>
-      <c r="C67" s="22" t="s">
-        <v>310</v>
-      </c>
-      <c r="D67" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E67" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="F67" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="G67" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="H67" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I67" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="J67" s="22" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="68" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A68" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B68" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="B68" s="22" t="s">
-        <v>106</v>
-      </c>
       <c r="C68" s="22" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="D68" s="23" t="b">
         <v>1</v>
@@ -4442,21 +4442,21 @@
         <v>0</v>
       </c>
       <c r="I68" s="22" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="J68" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="69" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A69" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B69" s="22" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C69" s="22" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="D69" s="24" t="b">
         <v>0</v>
@@ -4474,10 +4474,10 @@
         <v>0</v>
       </c>
       <c r="I69" s="22" t="s">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="J69" s="22" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="70" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4485,10 +4485,10 @@
         <v>53</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C70" s="22" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="D70" s="23" t="b">
         <v>0</v>
@@ -4509,7 +4509,7 @@
         <v>54</v>
       </c>
       <c r="J70" s="22" t="s">
-        <v>445</v>
+        <v>440</v>
       </c>
     </row>
     <row r="71" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4517,10 +4517,10 @@
         <v>31</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C71" s="22" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D71" s="24" t="b">
         <v>0</v>
@@ -4541,7 +4541,7 @@
         <v>32</v>
       </c>
       <c r="J71" s="22" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4549,10 +4549,10 @@
         <v>55</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="C72" s="22" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D72" s="24" t="b">
         <v>0</v>
@@ -4573,39 +4573,39 @@
         <v>56</v>
       </c>
       <c r="J72" s="22" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="73" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A73" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="B73" s="22" t="s">
+        <v>320</v>
+      </c>
+      <c r="C73" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="D73" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E73" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F73" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G73" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H73" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I73" s="22" t="s">
         <v>108</v>
       </c>
-      <c r="B73" s="22" t="s">
-        <v>323</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>324</v>
-      </c>
-      <c r="D73" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E73" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F73" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G73" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H73" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="I73" s="22" t="s">
-        <v>109</v>
-      </c>
       <c r="J73" s="22" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4613,31 +4613,31 @@
         <v>33</v>
       </c>
       <c r="B74" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="C74" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="D74" s="23" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F74" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G74" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H74" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I74" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="J74" s="23" t="s">
         <v>325</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>326</v>
-      </c>
-      <c r="D74" s="23" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F74" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G74" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H74" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I74" s="22" t="s">
-        <v>327</v>
-      </c>
-      <c r="J74" s="23" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="75" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4645,10 +4645,10 @@
         <v>57</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C75" s="22" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="D75" s="23" t="b">
         <v>0</v>
@@ -4669,7 +4669,7 @@
         <v>58</v>
       </c>
       <c r="J75" s="22" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="76" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4677,10 +4677,10 @@
         <v>34</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C76" s="22" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D76" s="24" t="b">
         <v>0</v>
@@ -4698,10 +4698,10 @@
         <v>1</v>
       </c>
       <c r="I76" s="22" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="J76" s="22" t="s">
-        <v>446</v>
+        <v>441</v>
       </c>
     </row>
     <row r="77" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4709,10 +4709,10 @@
         <v>35</v>
       </c>
       <c r="B77" s="22" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C77" s="22" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="D77" s="24" t="b">
         <v>0</v>
@@ -4730,74 +4730,74 @@
         <v>1</v>
       </c>
       <c r="I77" s="22" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="J77" s="22" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="B78" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="C78" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="D78" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E78" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F78" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="G78" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H78" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I78" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="B78" s="22" t="s">
-        <v>341</v>
-      </c>
-      <c r="C78" s="22" t="s">
-        <v>339</v>
-      </c>
-      <c r="D78" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E78" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F78" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="G78" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H78" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I78" s="22" t="s">
-        <v>111</v>
-      </c>
       <c r="J78" s="22" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A79" s="21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B79" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="D79" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="E79" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="F79" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G79" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H79" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I79" s="22" t="s">
+        <v>385</v>
+      </c>
+      <c r="J79" s="22" t="s">
         <v>340</v>
-      </c>
-      <c r="C79" s="22" t="s">
-        <v>342</v>
-      </c>
-      <c r="D79" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="E79" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="F79" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G79" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H79" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I79" s="22" t="s">
-        <v>389</v>
-      </c>
-      <c r="J79" s="22" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="80" spans="1:10" ht="43" x14ac:dyDescent="0.2">
@@ -4805,10 +4805,10 @@
         <v>36</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="D80" s="24" t="b">
         <v>0</v>
@@ -4829,7 +4829,7 @@
         <v>37</v>
       </c>
       <c r="J80" s="22" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
     </row>
     <row r="81" spans="1:10" ht="15" x14ac:dyDescent="0.2">
@@ -4837,11 +4837,11 @@
         <v>59</v>
       </c>
       <c r="B81" s="22" t="s">
+        <v>451</v>
+      </c>
+      <c r="C81" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="C81" s="22" t="s">
-        <v>61</v>
-      </c>
       <c r="D81" s="23" t="b">
         <v>1</v>
       </c>
@@ -4858,21 +4858,21 @@
         <v>1</v>
       </c>
       <c r="I81" s="22" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="J81" s="22" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B82" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B82" s="22" t="s">
-        <v>114</v>
-      </c>
       <c r="C82" s="22" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D82" s="23" t="b">
         <v>0</v>
@@ -4890,53 +4890,53 @@
         <v>1</v>
       </c>
       <c r="I82" s="22" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="J82" s="22" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="83" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A83" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B83" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="C83" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="D83" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="E83" s="23" t="b">
+        <v>1</v>
+      </c>
+      <c r="F83" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="G83" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="H83" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="I83" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="B83" s="22" t="s">
-        <v>419</v>
-      </c>
-      <c r="C83" s="22" t="s">
-        <v>352</v>
-      </c>
-      <c r="D83" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="E83" s="23" t="b">
-        <v>1</v>
-      </c>
-      <c r="F83" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="G83" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="H83" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="I83" s="22" t="s">
-        <v>116</v>
-      </c>
       <c r="J83" s="22" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
     </row>
     <row r="84" spans="1:10" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.2">
       <c r="A84" s="21" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>355</v>
+        <v>452</v>
       </c>
       <c r="C84" s="22" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D84" s="23" t="b">
         <v>1</v>
@@ -4954,10 +4954,10 @@
         <v>0</v>
       </c>
       <c r="I84" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J84" s="22" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="85" spans="1:10" ht="29" x14ac:dyDescent="0.2">
@@ -4965,10 +4965,10 @@
         <v>4</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="C85" s="22" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="D85" s="23" t="b">
         <v>1</v>
@@ -4986,21 +4986,21 @@
         <v>0</v>
       </c>
       <c r="I85" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J85" s="22" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="86" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A86" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C86" s="22" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D86" s="24" t="b">
         <v>0</v>
@@ -5018,21 +5018,21 @@
         <v>0</v>
       </c>
       <c r="I86" s="22" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="J86" s="22" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
     </row>
     <row r="87" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A87" s="21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B87" s="22" t="s">
         <v>118</v>
       </c>
-      <c r="B87" s="22" t="s">
-        <v>119</v>
-      </c>
       <c r="C87" s="22" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="D87" s="23" t="b">
         <v>1</v>
@@ -5050,22 +5050,22 @@
         <v>0</v>
       </c>
       <c r="I87" s="22" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="J87" s="22" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
     </row>
     <row r="88" spans="1:10" ht="29" x14ac:dyDescent="0.2">
       <c r="A88" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B88" s="22" t="s">
         <v>120</v>
       </c>
-      <c r="B88" s="22" t="s">
+      <c r="C88" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="C88" s="22" t="s">
-        <v>122</v>
-      </c>
       <c r="D88" s="23" t="b">
         <v>1</v>
       </c>
@@ -5082,21 +5082,21 @@
         <v>0</v>
       </c>
       <c r="I88" s="22" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="J88" s="22" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
     </row>
     <row r="89" spans="1:10" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B89" s="28" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C89" s="28" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="D89" s="23" t="b">
         <v>1</v>
@@ -5114,10 +5114,10 @@
         <v>0</v>
       </c>
       <c r="I89" s="28" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="J89" s="22" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
     </row>
     <row r="90" spans="1:10" ht="14" x14ac:dyDescent="0.2">
@@ -8040,7 +8040,7 @@
   </sheetPr>
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
@@ -8054,34 +8054,34 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="C2" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>142</v>
-      </c>
       <c r="D2" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E2" s="4" t="b">
         <v>1</v>
@@ -8089,16 +8089,16 @@
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>128</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="E3" s="4" t="b">
         <v>0</v>
@@ -8106,16 +8106,16 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>134</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="C4" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="D4" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="4" t="b">
         <v>1</v>
@@ -8123,16 +8123,16 @@
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="D5" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E5" s="4" t="b">
         <v>1</v>
@@ -8140,16 +8140,16 @@
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="31" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E6" s="4" t="b">
         <v>0</v>
@@ -8480,27 +8480,27 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="C2" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="D2" s="4" t="b">
         <v>1</v>
@@ -8508,13 +8508,13 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>146</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="3" t="s">
         <v>147</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>148</v>
       </c>
       <c r="D3" s="4" t="b">
         <v>1</v>
@@ -8522,13 +8522,13 @@
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="C4" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>151</v>
       </c>
       <c r="D4" s="4" t="b">
         <v>1</v>
@@ -8536,13 +8536,13 @@
     </row>
     <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="D5" s="4" t="b">
         <v>1</v>
@@ -8550,13 +8550,13 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="B6" s="18" t="s">
+      <c r="C6" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="D6" s="4" t="b">
         <v>1</v>

</xml_diff>

<commit_message>
minor fix in the articles section.
</commit_message>
<xml_diff>
--- a/metadata/binddata.xlsx
+++ b/metadata/binddata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ual895/Git/newdictionary/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF797C85-5B40-984C-B0D7-92152723881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C65C0A6-6CEA-A340-9B04-9C1685206EE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="500" windowWidth="24260" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4540" yWindow="500" windowWidth="24260" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Primitives" sheetId="1" r:id="rId1"/>
@@ -316,7 +316,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="453">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="456">
   <si>
     <t>primitive</t>
   </si>
@@ -1690,6 +1690,15 @@
   </si>
   <si>
     <t>Reports a specific turtle that has the provided unique number.</t>
+  </si>
+  <si>
+    <t>/article/shapes-and-colors-in-netlogo</t>
+  </si>
+  <si>
+    <t>Shapes and colors in NetLogo</t>
+  </si>
+  <si>
+    <t>Learn how to customize the look of your models with NetLogo's Turtle Shapes Editor, Link Shapes Editor, and Color Swatches tools.</t>
   </si>
 </sst>
 </file>
@@ -2237,7 +2246,7 @@
   </sheetPr>
   <dimension ref="A1:Z1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A79" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="B85" sqref="B85"/>
     </sheetView>
@@ -8040,9 +8049,9 @@
   </sheetPr>
   <dimension ref="A1:F96"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -8156,7 +8165,21 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C7" s="7"/>
+      <c r="A7" s="11" t="s">
+        <v>454</v>
+      </c>
+      <c r="B7" t="s">
+        <v>453</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="E7" s="11" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C8" s="7"/>
@@ -8426,7 +8449,7 @@
       <c r="C96" s="7"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F3 D2:E5 D6 E6:E96">
+  <conditionalFormatting sqref="F3 D2:E5 E6:E96 D6:D7">
     <cfRule type="notContainsBlanks" dxfId="6" priority="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>

</xml_diff>